<commit_message>
Creacion graficos de analisis de sensibilidad Se incorporaron graficos al doc
</commit_message>
<xml_diff>
--- a/FLUJO PESIMISTA.xlsx
+++ b/FLUJO PESIMISTA.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14260" tabRatio="884"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="25605" windowHeight="14205" tabRatio="884"/>
   </bookViews>
   <sheets>
     <sheet name="FLUJO CAJA PESIMISTA" sheetId="8" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="CREACIÓN CURSOS" sheetId="5" r:id="rId9"/>
     <sheet name="Plan de Marketing" sheetId="11" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -440,13 +440,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00;[Red]\-&quot;$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="175" formatCode="0.00000000%"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;\ #,##0.00;[Red]\-&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="0.00000000%"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1014,7 +1014,7 @@
   <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1036,7 +1036,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="206">
+  <cellXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1060,9 +1060,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1112,7 +1109,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1121,7 +1118,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1135,7 +1132,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1144,28 +1141,28 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1218,8 +1215,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1259,16 +1256,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1280,7 +1277,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="5" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1293,134 +1290,20 @@
     <xf numFmtId="3" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="4" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1431,14 +1314,132 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="5" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="175" fontId="5" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
@@ -1463,10 +1464,15 @@
     <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentual" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1837,612 +1843,613 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="4.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17">
-      <c r="A1" s="204" t="s">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="165" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="204"/>
-      <c r="C1" s="204"/>
-      <c r="D1" s="204"/>
-      <c r="E1" s="204"/>
-      <c r="F1" s="204"/>
-      <c r="G1" s="204"/>
-      <c r="H1" s="204"/>
-      <c r="I1" s="204"/>
-      <c r="J1" s="204"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="B4" s="52"/>
-      <c r="C4" s="84" t="s">
+      <c r="B1" s="165"/>
+      <c r="C1" s="165"/>
+      <c r="D1" s="165"/>
+      <c r="E1" s="165"/>
+      <c r="F1" s="165"/>
+      <c r="G1" s="165"/>
+      <c r="H1" s="165"/>
+      <c r="I1" s="165"/>
+      <c r="J1" s="165"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="51"/>
+      <c r="C4" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="84"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-    </row>
-    <row r="5" spans="1:10" ht="13" thickBot="1">
-      <c r="B5" s="77" t="s">
+      <c r="D4" s="83"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+    </row>
+    <row r="5" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="76" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="86">
+      <c r="D5" s="85">
         <v>0</v>
       </c>
-      <c r="E5" s="86">
+      <c r="E5" s="85">
         <v>1</v>
       </c>
-      <c r="F5" s="86">
+      <c r="F5" s="85">
         <v>2</v>
       </c>
-      <c r="G5" s="86">
+      <c r="G5" s="85">
         <v>3</v>
       </c>
-      <c r="H5" s="86">
+      <c r="H5" s="85">
         <v>4</v>
       </c>
-      <c r="I5" s="86">
+      <c r="I5" s="85">
         <v>5</v>
       </c>
-      <c r="J5" s="86">
+      <c r="J5" s="85">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13" thickTop="1">
-      <c r="B6" s="79" t="s">
+    <row r="6" spans="1:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="80" t="s">
+      <c r="C6" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106">
+      <c r="D6" s="105"/>
+      <c r="E6" s="105">
         <f>INGRESOS!D18</f>
         <v>109500000</v>
       </c>
-      <c r="F6" s="106">
+      <c r="F6" s="105">
         <f>INGRESOS!F18</f>
         <v>135999999.99999997</v>
       </c>
-      <c r="G6" s="106">
+      <c r="G6" s="105">
         <f>INGRESOS!H18</f>
         <v>153591999.99999997</v>
       </c>
-      <c r="H6" s="106">
+      <c r="H6" s="105">
         <f>INGRESOS!J18</f>
         <v>173567527.27272725</v>
       </c>
-      <c r="I6" s="106">
+      <c r="I6" s="105">
         <f>INGRESOS!L18</f>
         <v>196260904.29752061</v>
       </c>
-      <c r="J6" s="106">
+      <c r="J6" s="105">
         <f>INGRESOS!N18</f>
         <v>222054492.23365882</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="B7" s="79" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="80" t="s">
+      <c r="C7" s="79" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106">
+      <c r="D7" s="105"/>
+      <c r="E7" s="105">
         <v>5000000</v>
       </c>
-      <c r="F7" s="106">
+      <c r="F7" s="105">
         <f>E7*1.3</f>
         <v>6500000</v>
       </c>
-      <c r="G7" s="106">
+      <c r="G7" s="105">
         <f>F7*1.3</f>
         <v>8450000</v>
       </c>
-      <c r="H7" s="106">
+      <c r="H7" s="105">
         <f>G7*1.3</f>
         <v>10985000</v>
       </c>
-      <c r="I7" s="106">
+      <c r="I7" s="105">
         <f>H7*1.3</f>
         <v>14280500</v>
       </c>
-      <c r="J7" s="106">
+      <c r="J7" s="105">
         <f>I7*1.3</f>
         <v>18564650</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="B8" s="81" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="107"/>
-      <c r="E8" s="107">
+      <c r="D8" s="106"/>
+      <c r="E8" s="106">
+        <f>-'CREACIÓN CURSOS'!D14</f>
+        <v>-4400000</v>
+      </c>
+      <c r="F8" s="106">
         <f>-'CREACIÓN CURSOS'!E14</f>
         <v>-4400000</v>
       </c>
-      <c r="F8" s="107">
+      <c r="G8" s="106">
         <f>-'CREACIÓN CURSOS'!F14</f>
         <v>-4400000</v>
       </c>
-      <c r="G8" s="107">
+      <c r="H8" s="106">
         <f>-'CREACIÓN CURSOS'!G14</f>
         <v>-4400000</v>
       </c>
-      <c r="H8" s="107">
+      <c r="I8" s="106">
         <f>-'CREACIÓN CURSOS'!H14</f>
         <v>-4400000</v>
       </c>
-      <c r="I8" s="107">
+      <c r="J8" s="106">
         <f>-'CREACIÓN CURSOS'!I14</f>
         <v>-4400000</v>
       </c>
-      <c r="J8" s="107">
-        <f>-'CREACIÓN CURSOS'!J14</f>
-        <v>-4400000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="B9" s="81" t="s">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="82" t="s">
+      <c r="C9" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="107"/>
-      <c r="E9" s="107">
+      <c r="D9" s="106"/>
+      <c r="E9" s="106">
         <f>-INGRESOS!D18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-8212500.0000000009</v>
       </c>
-      <c r="F9" s="107">
+      <c r="F9" s="106">
         <f>-INGRESOS!F18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-10200000</v>
       </c>
-      <c r="G9" s="107">
+      <c r="G9" s="106">
         <f>-INGRESOS!H18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-11519400</v>
       </c>
-      <c r="H9" s="107">
+      <c r="H9" s="106">
         <f>-INGRESOS!J18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-13017564.545454545</v>
       </c>
-      <c r="I9" s="107">
+      <c r="I9" s="106">
         <f>-INGRESOS!L18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-14719567.822314048</v>
       </c>
-      <c r="J9" s="107">
+      <c r="J9" s="106">
         <f>-INGRESOS!N18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-16654086.917524414</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="B10" s="81" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="82" t="s">
+      <c r="C10" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="107"/>
-      <c r="E10" s="107">
+      <c r="D10" s="106"/>
+      <c r="E10" s="106">
         <f>-'ESTRUCTURA DE COSTOS'!H8</f>
         <v>-113378600</v>
       </c>
-      <c r="F10" s="107">
+      <c r="F10" s="106">
         <f>-'ESTRUCTURA DE COSTOS'!I8</f>
         <v>-123847530.00000001</v>
       </c>
-      <c r="G10" s="107">
+      <c r="G10" s="106">
         <f>-'ESTRUCTURA DE COSTOS'!J8</f>
         <v>-135319906.50000003</v>
       </c>
-      <c r="H10" s="107">
+      <c r="H10" s="106">
         <f>-'ESTRUCTURA DE COSTOS'!K8</f>
         <v>-147893901.82500005</v>
       </c>
-      <c r="I10" s="107">
+      <c r="I10" s="106">
         <f>-'ESTRUCTURA DE COSTOS'!L8</f>
         <v>-161677396.91625005</v>
       </c>
-      <c r="J10" s="107">
+      <c r="J10" s="106">
         <f>-'ESTRUCTURA DE COSTOS'!M8</f>
         <v>-176788946.76206258</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="B11" s="81" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="82" t="s">
+      <c r="C11" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="107"/>
-      <c r="E11" s="107">
+      <c r="D11" s="106"/>
+      <c r="E11" s="106">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="F11" s="107">
+      <c r="F11" s="106">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="G11" s="107">
+      <c r="G11" s="106">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="H11" s="107">
+      <c r="H11" s="106">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="I11" s="107">
+      <c r="I11" s="106">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="J11" s="107">
+      <c r="J11" s="106">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="B12" s="88" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="89" t="s">
+      <c r="C12" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="108"/>
-      <c r="E12" s="109">
+      <c r="D12" s="107"/>
+      <c r="E12" s="108">
         <f t="shared" ref="E12:J12" si="0">SUM(E6:E11)</f>
         <v>-12017766.666666666</v>
       </c>
-      <c r="F12" s="109">
+      <c r="F12" s="108">
         <f t="shared" si="0"/>
         <v>3525803.3333332888</v>
       </c>
-      <c r="G12" s="109">
+      <c r="G12" s="108">
         <f t="shared" si="0"/>
         <v>10276026.833333274</v>
       </c>
-      <c r="H12" s="109">
+      <c r="H12" s="108">
         <f t="shared" si="0"/>
         <v>18714394.235606004</v>
       </c>
-      <c r="I12" s="109">
+      <c r="I12" s="108">
         <f t="shared" si="0"/>
         <v>29217772.892289836</v>
       </c>
-      <c r="J12" s="109">
+      <c r="J12" s="108">
         <f t="shared" si="0"/>
         <v>42249441.88740515</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="B13" s="81" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="82" t="s">
+      <c r="C13" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="107"/>
-      <c r="E13" s="107">
+      <c r="D13" s="106"/>
+      <c r="E13" s="106">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="F13" s="107">
+      <c r="F13" s="106">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="G13" s="107">
+      <c r="G13" s="106">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="H13" s="107">
+      <c r="H13" s="106">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="I13" s="107">
+      <c r="I13" s="106">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="J13" s="107">
+      <c r="J13" s="106">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="B14" s="88" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="89" t="s">
+      <c r="C14" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="108"/>
-      <c r="E14" s="109">
+      <c r="D14" s="107"/>
+      <c r="E14" s="108">
         <f t="shared" ref="E14:J14" si="1">SUM(E12:E13)</f>
         <v>-14857091.532231411</v>
       </c>
-      <c r="F14" s="109">
+      <c r="F14" s="108">
         <f t="shared" si="1"/>
         <v>686478.4677685434</v>
       </c>
-      <c r="G14" s="109">
+      <c r="G14" s="108">
         <f t="shared" si="1"/>
         <v>7436701.9677685294</v>
       </c>
-      <c r="H14" s="109">
+      <c r="H14" s="108">
         <f t="shared" si="1"/>
         <v>15875069.370041259</v>
       </c>
-      <c r="I14" s="109">
+      <c r="I14" s="108">
         <f t="shared" si="1"/>
         <v>26378448.026725091</v>
       </c>
-      <c r="J14" s="109">
+      <c r="J14" s="108">
         <f t="shared" si="1"/>
         <v>39410117.021840401</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="B15" s="81" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="82" t="s">
+      <c r="C15" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="107"/>
-      <c r="E15" s="107">
+      <c r="D15" s="106"/>
+      <c r="E15" s="106">
         <f t="shared" ref="E15:J15" si="2">+IF(E14&gt;0,-(E14*0.17),0)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="107">
+      <c r="F15" s="106">
         <f t="shared" si="2"/>
         <v>-116701.33952065239</v>
       </c>
-      <c r="G15" s="107">
+      <c r="G15" s="106">
         <f t="shared" si="2"/>
         <v>-1264239.3345206501</v>
       </c>
-      <c r="H15" s="107">
+      <c r="H15" s="106">
         <f t="shared" si="2"/>
         <v>-2698761.792907014</v>
       </c>
-      <c r="I15" s="107">
+      <c r="I15" s="106">
         <f t="shared" si="2"/>
         <v>-4484336.1645432655</v>
       </c>
-      <c r="J15" s="107">
+      <c r="J15" s="106">
         <f t="shared" si="2"/>
         <v>-6699719.8937128689</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="B16" s="81" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="82" t="s">
+      <c r="C16" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="107"/>
-      <c r="E16" s="107">
+      <c r="D16" s="106"/>
+      <c r="E16" s="106">
         <f t="shared" ref="E16:J16" si="3">-(E11)</f>
         <v>526666.66666666663</v>
       </c>
-      <c r="F16" s="107">
+      <c r="F16" s="106">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
-      <c r="G16" s="107">
+      <c r="G16" s="106">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
-      <c r="H16" s="107">
+      <c r="H16" s="106">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
-      <c r="I16" s="107">
+      <c r="I16" s="106">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
-      <c r="J16" s="107">
+      <c r="J16" s="106">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
-      <c r="B17" s="81" t="s">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="82" t="s">
+      <c r="C17" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="107"/>
-      <c r="E17" s="107">
+      <c r="D17" s="106"/>
+      <c r="E17" s="106">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="F17" s="107">
+      <c r="F17" s="106">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="G17" s="107">
+      <c r="G17" s="106">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="H17" s="107">
+      <c r="H17" s="106">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="I17" s="107">
+      <c r="I17" s="106">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="J17" s="107">
+      <c r="J17" s="106">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
     </row>
-    <row r="18" spans="2:10">
-      <c r="B18" s="81" t="s">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="82" t="s">
+      <c r="C18" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="107">
+      <c r="D18" s="106">
         <f>-INVERSION!D20</f>
         <v>-20610000</v>
       </c>
-      <c r="E18" s="107"/>
-      <c r="F18" s="107"/>
-      <c r="G18" s="107"/>
-      <c r="H18" s="107"/>
-      <c r="I18" s="107"/>
-      <c r="J18" s="107"/>
-    </row>
-    <row r="19" spans="2:10" ht="13" thickBot="1">
-      <c r="B19" s="78"/>
-      <c r="C19" s="83" t="s">
+      <c r="E18" s="106"/>
+      <c r="F18" s="106"/>
+      <c r="G18" s="106"/>
+      <c r="H18" s="106"/>
+      <c r="I18" s="106"/>
+      <c r="J18" s="106"/>
+    </row>
+    <row r="19" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="77"/>
+      <c r="C19" s="82" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="156">
+      <c r="D19" s="155">
         <f>'G. FINANCIERO'!C5</f>
         <v>12366000</v>
       </c>
-      <c r="E19" s="110"/>
-      <c r="F19" s="110"/>
-      <c r="G19" s="110"/>
-      <c r="H19" s="110"/>
-      <c r="I19" s="110"/>
-      <c r="J19" s="110"/>
-    </row>
-    <row r="20" spans="2:10" ht="13" thickTop="1">
-      <c r="B20" s="79" t="s">
+      <c r="E19" s="109"/>
+      <c r="F19" s="109"/>
+      <c r="G19" s="109"/>
+      <c r="H19" s="109"/>
+      <c r="I19" s="109"/>
+      <c r="J19" s="109"/>
+    </row>
+    <row r="20" spans="2:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="87" t="s">
+      <c r="C20" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="131">
+      <c r="D20" s="130">
         <f>SUM(D18:D19)</f>
         <v>-8244000</v>
       </c>
-      <c r="E20" s="131">
+      <c r="E20" s="130">
         <f t="shared" ref="E20:J20" si="4">SUM(E14:E19)</f>
         <v>-16391424.865564745</v>
       </c>
-      <c r="F20" s="131">
+      <c r="F20" s="130">
         <f t="shared" si="4"/>
         <v>-964556.2050854424</v>
       </c>
-      <c r="G20" s="131">
+      <c r="G20" s="130">
         <f t="shared" si="4"/>
         <v>4638129.2999145463</v>
       </c>
-      <c r="H20" s="131">
+      <c r="H20" s="130">
         <f t="shared" si="4"/>
         <v>11641974.24380091</v>
       </c>
-      <c r="I20" s="131">
+      <c r="I20" s="130">
         <f t="shared" si="4"/>
         <v>20359778.528848495</v>
       </c>
-      <c r="J20" s="131">
+      <c r="J20" s="130">
         <f t="shared" si="4"/>
         <v>31176063.794794198</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="13" thickBot="1">
-      <c r="B21" s="136"/>
-      <c r="C21" s="136"/>
-      <c r="D21" s="137"/>
-      <c r="E21" s="137"/>
-      <c r="F21" s="137"/>
-      <c r="G21" s="137"/>
-      <c r="H21" s="137"/>
-      <c r="I21" s="137"/>
-      <c r="J21" s="137"/>
-    </row>
-    <row r="22" spans="2:10">
-      <c r="B22" s="132"/>
-      <c r="C22" s="138" t="s">
+    <row r="21" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="135"/>
+      <c r="C21" s="135"/>
+      <c r="D21" s="136"/>
+      <c r="E21" s="136"/>
+      <c r="F21" s="136"/>
+      <c r="G21" s="136"/>
+      <c r="H21" s="136"/>
+      <c r="I21" s="136"/>
+      <c r="J21" s="136"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B22" s="131"/>
+      <c r="C22" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="143">
+      <c r="D22" s="142">
         <f>NPV(D24,E20:J20)+D20</f>
         <v>10079906.799768489</v>
       </c>
-      <c r="E22" s="137"/>
-      <c r="F22" s="139"/>
-      <c r="G22" s="137"/>
-      <c r="H22" s="137"/>
-      <c r="I22" s="137"/>
-      <c r="J22" s="137"/>
-    </row>
-    <row r="23" spans="2:10" ht="13" thickBot="1">
-      <c r="B23" s="133"/>
-      <c r="C23" s="140" t="s">
+      <c r="E22" s="136"/>
+      <c r="F22" s="138"/>
+      <c r="G22" s="136"/>
+      <c r="H22" s="136"/>
+      <c r="I22" s="136"/>
+      <c r="J22" s="136"/>
+    </row>
+    <row r="23" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="132"/>
+      <c r="C23" s="139" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="205">
+      <c r="D23" s="164">
         <f>IRR(D20:J20)</f>
         <v>0.25017156683584729</v>
       </c>
-      <c r="E23" s="136"/>
-      <c r="F23" s="141"/>
-      <c r="G23" s="136"/>
-      <c r="H23" s="136"/>
-      <c r="I23" s="136"/>
-      <c r="J23" s="136"/>
-    </row>
-    <row r="24" spans="2:10" ht="13" thickBot="1">
-      <c r="B24" s="134"/>
-      <c r="C24" s="142" t="s">
+      <c r="E23" s="135"/>
+      <c r="F23" s="140"/>
+      <c r="G23" s="135"/>
+      <c r="H23" s="135"/>
+      <c r="I23" s="135"/>
+      <c r="J23" s="135"/>
+    </row>
+    <row r="24" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="133"/>
+      <c r="C24" s="141" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="135">
+      <c r="D24" s="134">
         <v>0.15</v>
       </c>
-      <c r="E24" s="136"/>
-      <c r="F24" s="136"/>
-      <c r="G24" s="136"/>
-      <c r="H24" s="136"/>
-      <c r="I24" s="136"/>
-      <c r="J24" s="136"/>
-    </row>
-    <row r="27" spans="2:10">
-      <c r="C27" s="153"/>
-      <c r="D27" s="154"/>
+      <c r="E24" s="135"/>
+      <c r="F24" s="135"/>
+      <c r="G24" s="135"/>
+      <c r="H24" s="135"/>
+      <c r="I24" s="135"/>
+      <c r="J24" s="135"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C27" s="152"/>
+      <c r="D27" s="153"/>
       <c r="I27" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="2:10">
-      <c r="D31" s="155"/>
-    </row>
-    <row r="33" spans="3:10">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="D31" s="154"/>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
         <v>8</v>
       </c>
@@ -2471,7 +2478,7 @@
         <v>154608960.00000009</v>
       </c>
     </row>
-    <row r="34" spans="3:10">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>130</v>
       </c>
@@ -2500,7 +2507,7 @@
         <v>22179986.762062501</v>
       </c>
     </row>
-    <row r="35" spans="3:10">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
         <v>131</v>
       </c>
@@ -2529,7 +2536,7 @@
         <v>176788946.76206258</v>
       </c>
     </row>
-    <row r="37" spans="3:10">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E37" s="2">
         <f>E10+E35</f>
         <v>0</v>
@@ -2555,13 +2562,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:10">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C38" s="2">
         <f>F33-E33</f>
         <v>9600000.0000000149</v>
       </c>
     </row>
-    <row r="39" spans="3:10">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C39">
         <f>C38/12</f>
         <v>800000.00000000128</v>
@@ -2591,29 +2598,29 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>129</v>
       </c>
@@ -2633,77 +2640,77 @@
   <sheetPr codeName="Hoja2" enableFormatConditionsCalculation="0"/>
   <dimension ref="B3:D20"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="13" thickBot="1"/>
-    <row r="4" spans="2:4" ht="13" thickBot="1">
-      <c r="B4" s="161" t="s">
+    <row r="3" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="170" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="162"/>
+      <c r="C4" s="171"/>
       <c r="D4" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="13" thickBot="1">
-      <c r="B5" s="159" t="s">
+    <row r="5" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="168" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="160"/>
-      <c r="D5" s="45"/>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="40"/>
-      <c r="C6" s="41" t="s">
+      <c r="C5" s="169"/>
+      <c r="D5" s="44"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="39"/>
+      <c r="C6" s="40" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="2:4" ht="13" thickBot="1">
-      <c r="B7" s="40"/>
-      <c r="C7" s="41" t="s">
+    <row r="7" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="39"/>
+      <c r="C7" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="18"/>
     </row>
-    <row r="8" spans="2:4" ht="13" thickBot="1">
-      <c r="B8" s="159" t="s">
+    <row r="8" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="168" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="163"/>
-      <c r="D8" s="46">
+      <c r="C8" s="172"/>
+      <c r="D8" s="45">
         <v>5000000</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="13" thickBot="1">
-      <c r="B9" s="159" t="s">
+    <row r="9" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="168" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="160"/>
-      <c r="D9" s="46">
+      <c r="C9" s="169"/>
+      <c r="D9" s="45">
         <v>2500000</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="13" thickBot="1">
-      <c r="B10" s="159" t="s">
+    <row r="10" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="168" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="160"/>
-      <c r="D10" s="45"/>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="42">
+      <c r="C10" s="169"/>
+      <c r="D10" s="44"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="41">
         <v>7</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="40" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="14">
@@ -2711,19 +2718,19 @@
         <v>2800000</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="42">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="41">
         <v>1</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="40" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="14">
         <v>300000</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="13" thickBot="1">
-      <c r="B13" s="43">
+    <row r="13" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="42">
         <v>1</v>
       </c>
       <c r="C13" s="13" t="s">
@@ -2733,15 +2740,15 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="13" thickBot="1">
-      <c r="B14" s="159" t="s">
+    <row r="14" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="168" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="160"/>
-      <c r="D14" s="45"/>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="43"/>
+      <c r="C14" s="169"/>
+      <c r="D14" s="44"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="42"/>
       <c r="C15" s="13" t="s">
         <v>10</v>
       </c>
@@ -2749,18 +2756,18 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="43"/>
-      <c r="C16" s="113" t="s">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="42"/>
+      <c r="C16" s="112" t="s">
         <v>106</v>
       </c>
       <c r="D16" s="14">
-        <f>'CREACIÓN CURSOS'!D14</f>
+        <f>'CREACIÓN CURSOS'!C14</f>
         <v>4400000</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="43"/>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="42"/>
       <c r="C17" s="13" t="s">
         <v>84</v>
       </c>
@@ -2768,8 +2775,8 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="43"/>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="42"/>
       <c r="C18" s="13" t="s">
         <v>83</v>
       </c>
@@ -2777,21 +2784,21 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="13" thickBot="1">
-      <c r="B19" s="44"/>
-      <c r="C19" s="114" t="s">
+    <row r="19" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="43"/>
+      <c r="C19" s="113" t="s">
         <v>107</v>
       </c>
       <c r="D19" s="18">
         <v>5000000</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="13" thickBot="1">
-      <c r="B20" s="157" t="s">
+    <row r="20" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="158"/>
-      <c r="D20" s="47">
+      <c r="C20" s="167"/>
+      <c r="D20" s="46">
         <f>SUM(D5:D19)</f>
         <v>20610000</v>
       </c>
@@ -2821,780 +2828,741 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P30"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="3.1640625" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.1640625" customWidth="1"/>
-    <col min="5" max="5" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.83203125" customWidth="1"/>
-    <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16">
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
-      <c r="M2" s="101"/>
-      <c r="N2" s="101"/>
-      <c r="O2" s="101"/>
-      <c r="P2" s="101"/>
-    </row>
-    <row r="3" spans="2:16" ht="13" thickBot="1">
-      <c r="B3" s="101"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="101"/>
-      <c r="O3" s="101"/>
-      <c r="P3" s="101"/>
-    </row>
-    <row r="4" spans="2:16" ht="13" thickBot="1">
-      <c r="B4" s="101"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="178" t="s">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="100"/>
+      <c r="O2" s="100"/>
+      <c r="P2" s="100"/>
+    </row>
+    <row r="3" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
+    </row>
+    <row r="4" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="185" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="180"/>
-      <c r="F4" s="178" t="s">
+      <c r="E4" s="187"/>
+      <c r="F4" s="185" t="s">
         <v>96</v>
       </c>
-      <c r="G4" s="179"/>
-      <c r="H4" s="180" t="s">
+      <c r="G4" s="186"/>
+      <c r="H4" s="187" t="s">
         <v>97</v>
       </c>
-      <c r="I4" s="180"/>
-      <c r="J4" s="178" t="s">
+      <c r="I4" s="187"/>
+      <c r="J4" s="185" t="s">
         <v>98</v>
       </c>
-      <c r="K4" s="179"/>
-      <c r="L4" s="180" t="s">
+      <c r="K4" s="186"/>
+      <c r="L4" s="187" t="s">
         <v>99</v>
       </c>
-      <c r="M4" s="180"/>
-      <c r="N4" s="178" t="s">
+      <c r="M4" s="187"/>
+      <c r="N4" s="185" t="s">
         <v>100</v>
       </c>
-      <c r="O4" s="179"/>
-      <c r="P4" s="101"/>
-    </row>
-    <row r="5" spans="2:16" ht="13" thickBot="1">
-      <c r="B5" s="101"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="102" t="s">
+      <c r="O4" s="186"/>
+      <c r="P4" s="100"/>
+    </row>
+    <row r="5" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="100"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="101" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="103" t="s">
+      <c r="E5" s="102" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="102" t="s">
+      <c r="F5" s="101" t="s">
         <v>91</v>
       </c>
-      <c r="G5" s="104" t="s">
+      <c r="G5" s="103" t="s">
         <v>92</v>
       </c>
-      <c r="H5" s="103" t="s">
+      <c r="H5" s="102" t="s">
         <v>91</v>
       </c>
-      <c r="I5" s="103" t="s">
+      <c r="I5" s="102" t="s">
         <v>92</v>
       </c>
-      <c r="J5" s="102" t="s">
+      <c r="J5" s="101" t="s">
         <v>91</v>
       </c>
-      <c r="K5" s="104" t="s">
+      <c r="K5" s="103" t="s">
         <v>92</v>
       </c>
-      <c r="L5" s="103" t="s">
+      <c r="L5" s="102" t="s">
         <v>91</v>
       </c>
-      <c r="M5" s="103" t="s">
+      <c r="M5" s="102" t="s">
         <v>92</v>
       </c>
-      <c r="N5" s="102" t="s">
+      <c r="N5" s="101" t="s">
         <v>91</v>
       </c>
-      <c r="O5" s="104" t="s">
+      <c r="O5" s="103" t="s">
         <v>92</v>
       </c>
-      <c r="P5" s="101"/>
-    </row>
-    <row r="6" spans="2:16" ht="13" thickBot="1">
-      <c r="B6" s="101"/>
-      <c r="C6" s="168" t="s">
+      <c r="P5" s="100"/>
+    </row>
+    <row r="6" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="100"/>
+      <c r="C6" s="189" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="147">
+      <c r="D6" s="146">
         <f>12*1*20</f>
         <v>240</v>
       </c>
-      <c r="E6" s="111">
+      <c r="E6" s="110">
         <v>180000</v>
       </c>
-      <c r="F6" s="111">
+      <c r="F6" s="110">
         <f>20*1.1*12</f>
         <v>264</v>
       </c>
-      <c r="G6" s="111">
+      <c r="G6" s="110">
         <v>180000</v>
       </c>
-      <c r="H6" s="111">
+      <c r="H6" s="110">
         <f>F6*(1+$C$29)</f>
         <v>288</v>
       </c>
-      <c r="I6" s="111">
+      <c r="I6" s="110">
         <v>180000</v>
       </c>
-      <c r="J6" s="111">
+      <c r="J6" s="110">
         <f>H6*(1+$C$29)</f>
         <v>314.18181818181813</v>
       </c>
-      <c r="K6" s="111">
+      <c r="K6" s="110">
         <v>180000</v>
       </c>
-      <c r="L6" s="111">
+      <c r="L6" s="110">
         <f>J6*(1+$C$29)</f>
         <v>342.7438016528925</v>
       </c>
-      <c r="M6" s="111">
+      <c r="M6" s="110">
         <v>180000</v>
       </c>
-      <c r="N6" s="111">
+      <c r="N6" s="110">
         <f>L6*(1+$C$29)</f>
         <v>373.90232907588268</v>
       </c>
-      <c r="O6" s="111">
+      <c r="O6" s="110">
         <v>180000</v>
       </c>
-      <c r="P6" s="101"/>
-    </row>
-    <row r="7" spans="2:16" ht="13" thickBot="1">
-      <c r="B7" s="101"/>
-      <c r="C7" s="169"/>
-      <c r="D7" s="171">
+      <c r="P6" s="100"/>
+    </row>
+    <row r="7" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="100"/>
+      <c r="C7" s="190"/>
+      <c r="D7" s="179">
         <f>D6*E6</f>
         <v>43200000</v>
       </c>
-      <c r="E7" s="172"/>
-      <c r="F7" s="171">
+      <c r="E7" s="184"/>
+      <c r="F7" s="179">
         <f>F6*G6</f>
         <v>47520000</v>
       </c>
-      <c r="G7" s="173"/>
-      <c r="H7" s="172">
+      <c r="G7" s="180"/>
+      <c r="H7" s="184">
         <f>H6*I6</f>
         <v>51840000</v>
       </c>
-      <c r="I7" s="172"/>
-      <c r="J7" s="171">
+      <c r="I7" s="184"/>
+      <c r="J7" s="179">
         <f>J6*K6</f>
         <v>56552727.272727266</v>
       </c>
-      <c r="K7" s="173"/>
-      <c r="L7" s="172">
+      <c r="K7" s="180"/>
+      <c r="L7" s="184">
         <f>L6*M6</f>
         <v>61693884.297520652</v>
       </c>
-      <c r="M7" s="172"/>
-      <c r="N7" s="171">
+      <c r="M7" s="184"/>
+      <c r="N7" s="179">
         <f>N6*O6</f>
         <v>67302419.23365888</v>
       </c>
-      <c r="O7" s="173"/>
-      <c r="P7" s="101"/>
-    </row>
-    <row r="8" spans="2:16" ht="13" thickBot="1">
-      <c r="B8" s="101"/>
-      <c r="C8" s="168" t="s">
+      <c r="O7" s="180"/>
+      <c r="P7" s="100"/>
+    </row>
+    <row r="8" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="100"/>
+      <c r="C8" s="189" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="111">
+      <c r="D8" s="110">
         <f>D10*0.9</f>
         <v>90</v>
       </c>
-      <c r="E8" s="111">
+      <c r="E8" s="110">
         <v>70000</v>
       </c>
-      <c r="F8" s="111">
+      <c r="F8" s="110">
         <f>(F10-D10)*0.9+0.2*D10</f>
         <v>33.499999999999986</v>
       </c>
-      <c r="G8" s="111">
+      <c r="G8" s="110">
         <v>70000</v>
       </c>
-      <c r="H8" s="111">
+      <c r="H8" s="110">
         <f>(H10-F10)*0.9+0.2*F10</f>
         <v>38.524999999999991</v>
       </c>
-      <c r="I8" s="111">
+      <c r="I8" s="110">
         <v>70000</v>
       </c>
-      <c r="J8" s="111">
+      <c r="J8" s="110">
         <f>(J10-H10)*0.9+0.2*H10</f>
         <v>44.30374999999998</v>
       </c>
-      <c r="K8" s="111">
+      <c r="K8" s="110">
         <v>70000</v>
       </c>
-      <c r="L8" s="111">
+      <c r="L8" s="110">
         <f>(L10-J10)*0.9+0.2*J10</f>
         <v>50.949312499999976</v>
       </c>
-      <c r="M8" s="111">
+      <c r="M8" s="110">
         <v>70000</v>
       </c>
-      <c r="N8" s="111">
+      <c r="N8" s="110">
         <f>(N10-L10)*0.9+0.2*L10</f>
         <v>58.591709374999965</v>
       </c>
-      <c r="O8" s="111">
+      <c r="O8" s="110">
         <v>70000</v>
       </c>
-      <c r="P8" s="101"/>
-    </row>
-    <row r="9" spans="2:16" ht="13" thickBot="1">
-      <c r="B9" s="101"/>
-      <c r="C9" s="170"/>
-      <c r="D9" s="174">
+      <c r="P8" s="100"/>
+    </row>
+    <row r="9" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="100"/>
+      <c r="C9" s="191"/>
+      <c r="D9" s="182">
         <f>D8*E8</f>
         <v>6300000</v>
       </c>
-      <c r="E9" s="165"/>
-      <c r="F9" s="174">
+      <c r="E9" s="181"/>
+      <c r="F9" s="182">
         <f>F8*G8</f>
         <v>2344999.9999999991</v>
       </c>
-      <c r="G9" s="181"/>
-      <c r="H9" s="165">
+      <c r="G9" s="183"/>
+      <c r="H9" s="181">
         <f>H8*I8</f>
         <v>2696749.9999999995</v>
       </c>
-      <c r="I9" s="165"/>
-      <c r="J9" s="174">
+      <c r="I9" s="181"/>
+      <c r="J9" s="182">
         <f>J8*K8</f>
         <v>3101262.4999999986</v>
       </c>
-      <c r="K9" s="181"/>
-      <c r="L9" s="165">
+      <c r="K9" s="183"/>
+      <c r="L9" s="181">
         <f>L8*M8</f>
         <v>3566451.8749999981</v>
       </c>
-      <c r="M9" s="165"/>
-      <c r="N9" s="174">
+      <c r="M9" s="181"/>
+      <c r="N9" s="182">
         <f>N8*O8</f>
         <v>4101419.6562499977</v>
       </c>
-      <c r="O9" s="181"/>
-      <c r="P9" s="101"/>
-    </row>
-    <row r="10" spans="2:16" ht="13" thickBot="1">
-      <c r="B10" s="101"/>
-      <c r="C10" s="169" t="s">
+      <c r="O9" s="183"/>
+      <c r="P9" s="100"/>
+    </row>
+    <row r="10" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="100"/>
+      <c r="C10" s="190" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="111">
+      <c r="D10" s="110">
         <v>100</v>
       </c>
-      <c r="E10" s="111">
+      <c r="E10" s="110">
         <f>$C$23*12</f>
         <v>600000</v>
       </c>
-      <c r="F10" s="111">
+      <c r="F10" s="110">
         <f>D10*(1+$C$26)</f>
         <v>114.99999999999999</v>
       </c>
-      <c r="G10" s="111">
+      <c r="G10" s="110">
         <f>$C$23*12</f>
         <v>600000</v>
       </c>
-      <c r="H10" s="111">
+      <c r="H10" s="110">
         <f>F10*(1+$C$26)</f>
         <v>132.24999999999997</v>
       </c>
-      <c r="I10" s="111">
+      <c r="I10" s="110">
         <f>$C$23*12</f>
         <v>600000</v>
       </c>
-      <c r="J10" s="111">
+      <c r="J10" s="110">
         <f>H10*(1+$C$26)</f>
         <v>152.08749999999995</v>
       </c>
-      <c r="K10" s="111">
+      <c r="K10" s="110">
         <f>$C$23*12</f>
         <v>600000</v>
       </c>
-      <c r="L10" s="111">
+      <c r="L10" s="110">
         <f>J10*(1+$C$26)</f>
         <v>174.90062499999993</v>
       </c>
-      <c r="M10" s="111">
+      <c r="M10" s="110">
         <f>$C$23*12</f>
         <v>600000</v>
       </c>
-      <c r="N10" s="111">
+      <c r="N10" s="110">
         <f>L10*(1+$C$26)</f>
         <v>201.13571874999991</v>
       </c>
-      <c r="O10" s="111">
+      <c r="O10" s="110">
         <f>$C$23*12</f>
         <v>600000</v>
       </c>
-      <c r="P10" s="101"/>
-    </row>
-    <row r="11" spans="2:16" ht="13" thickBot="1">
-      <c r="B11" s="101"/>
-      <c r="C11" s="169"/>
-      <c r="D11" s="171">
+      <c r="P10" s="100"/>
+    </row>
+    <row r="11" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="100"/>
+      <c r="C11" s="190"/>
+      <c r="D11" s="179">
         <f>D10*E10</f>
         <v>60000000</v>
       </c>
-      <c r="E11" s="172"/>
-      <c r="F11" s="171">
+      <c r="E11" s="184"/>
+      <c r="F11" s="179">
         <f>F10*G10</f>
         <v>68999999.999999985</v>
       </c>
-      <c r="G11" s="173"/>
-      <c r="H11" s="172">
+      <c r="G11" s="180"/>
+      <c r="H11" s="184">
         <f>H10*I10</f>
         <v>79349999.999999985</v>
       </c>
-      <c r="I11" s="172"/>
-      <c r="J11" s="171">
+      <c r="I11" s="184"/>
+      <c r="J11" s="179">
         <f>J10*K10</f>
         <v>91252499.99999997</v>
       </c>
-      <c r="K11" s="173"/>
-      <c r="L11" s="172">
+      <c r="K11" s="180"/>
+      <c r="L11" s="184">
         <f>L10*M10</f>
         <v>104940374.99999996</v>
       </c>
-      <c r="M11" s="172"/>
-      <c r="N11" s="171">
+      <c r="M11" s="184"/>
+      <c r="N11" s="179">
         <f>N10*O10</f>
         <v>120681431.24999994</v>
       </c>
-      <c r="O11" s="173"/>
-      <c r="P11" s="101"/>
-    </row>
-    <row r="12" spans="2:16" ht="13" thickBot="1">
-      <c r="B12" s="101"/>
-      <c r="C12" s="168" t="s">
+      <c r="O11" s="180"/>
+      <c r="P11" s="100"/>
+    </row>
+    <row r="12" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="100"/>
+      <c r="C12" s="189" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="111"/>
-      <c r="E12" s="111"/>
-      <c r="F12" s="111">
+      <c r="D12" s="110"/>
+      <c r="E12" s="110"/>
+      <c r="F12" s="110">
         <f>0.7*F10</f>
         <v>80.499999999999986</v>
       </c>
-      <c r="G12" s="111">
+      <c r="G12" s="110">
         <f>10000*12</f>
         <v>120000</v>
       </c>
-      <c r="H12" s="111">
+      <c r="H12" s="110">
         <f>0.7*H10</f>
         <v>92.574999999999974</v>
       </c>
-      <c r="I12" s="111">
+      <c r="I12" s="110">
         <f>10000*12</f>
         <v>120000</v>
       </c>
-      <c r="J12" s="111">
+      <c r="J12" s="110">
         <f>0.7*J10</f>
         <v>106.46124999999996</v>
       </c>
-      <c r="K12" s="111">
+      <c r="K12" s="110">
         <f>10000*12</f>
         <v>120000</v>
       </c>
-      <c r="L12" s="111">
+      <c r="L12" s="110">
         <f>0.7*L10</f>
         <v>122.43043749999994</v>
       </c>
-      <c r="M12" s="111">
+      <c r="M12" s="110">
         <f>10000*12</f>
         <v>120000</v>
       </c>
-      <c r="N12" s="111">
+      <c r="N12" s="110">
         <f>0.7*N10</f>
         <v>140.79500312499994</v>
       </c>
-      <c r="O12" s="111">
+      <c r="O12" s="110">
         <f>10000*12</f>
         <v>120000</v>
       </c>
-      <c r="P12" s="101"/>
-    </row>
-    <row r="13" spans="2:16" ht="13" thickBot="1">
-      <c r="B13" s="101"/>
-      <c r="C13" s="170"/>
-      <c r="D13" s="174">
+      <c r="P12" s="100"/>
+    </row>
+    <row r="13" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="100"/>
+      <c r="C13" s="191"/>
+      <c r="D13" s="182">
         <f>D12*E12</f>
         <v>0</v>
       </c>
-      <c r="E13" s="165"/>
-      <c r="F13" s="174">
+      <c r="E13" s="181"/>
+      <c r="F13" s="182">
         <f>F12*G12</f>
         <v>9659999.9999999981</v>
       </c>
-      <c r="G13" s="181"/>
-      <c r="H13" s="165">
+      <c r="G13" s="183"/>
+      <c r="H13" s="181">
         <f>H12*I12</f>
         <v>11108999.999999996</v>
       </c>
-      <c r="I13" s="165"/>
-      <c r="J13" s="174">
+      <c r="I13" s="181"/>
+      <c r="J13" s="182">
         <f>J12*K12</f>
         <v>12775349.999999996</v>
       </c>
-      <c r="K13" s="181"/>
-      <c r="L13" s="165">
+      <c r="K13" s="183"/>
+      <c r="L13" s="181">
         <f>L12*M12</f>
         <v>14691652.499999993</v>
       </c>
-      <c r="M13" s="165"/>
-      <c r="N13" s="174">
+      <c r="M13" s="181"/>
+      <c r="N13" s="182">
         <f>N12*O12</f>
         <v>16895400.374999993</v>
       </c>
-      <c r="O13" s="181"/>
-      <c r="P13" s="101"/>
-    </row>
-    <row r="14" spans="2:16" ht="13" thickBot="1">
-      <c r="B14" s="101"/>
-      <c r="C14" s="169" t="s">
+      <c r="O13" s="183"/>
+      <c r="P13" s="100"/>
+    </row>
+    <row r="14" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="100"/>
+      <c r="C14" s="190" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="111"/>
-      <c r="E14" s="111"/>
-      <c r="F14" s="111">
+      <c r="D14" s="110"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="110">
         <f>0.3*F10</f>
         <v>34.499999999999993</v>
       </c>
-      <c r="G14" s="111">
+      <c r="G14" s="110">
         <v>50000</v>
       </c>
-      <c r="H14" s="111">
+      <c r="H14" s="110">
         <f>0.3*H10</f>
         <v>39.67499999999999</v>
       </c>
-      <c r="I14" s="111">
+      <c r="I14" s="110">
         <v>50000</v>
       </c>
-      <c r="J14" s="111">
+      <c r="J14" s="110">
         <f>0.3*J10</f>
         <v>45.626249999999985</v>
       </c>
-      <c r="K14" s="111">
+      <c r="K14" s="110">
         <v>50000</v>
       </c>
-      <c r="L14" s="111">
+      <c r="L14" s="110">
         <f>0.3*L10</f>
         <v>52.47018749999998</v>
       </c>
-      <c r="M14" s="111">
+      <c r="M14" s="110">
         <v>50000</v>
       </c>
-      <c r="N14" s="111">
+      <c r="N14" s="110">
         <f>0.3*N10</f>
         <v>60.340715624999973</v>
       </c>
-      <c r="O14" s="111">
+      <c r="O14" s="110">
         <v>50000</v>
       </c>
-      <c r="P14" s="101"/>
-    </row>
-    <row r="15" spans="2:16" ht="13" thickBot="1">
-      <c r="B15" s="101"/>
-      <c r="C15" s="169"/>
-      <c r="D15" s="171">
+      <c r="P14" s="100"/>
+    </row>
+    <row r="15" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="100"/>
+      <c r="C15" s="190"/>
+      <c r="D15" s="179">
         <f>D14*E14</f>
         <v>0</v>
       </c>
-      <c r="E15" s="172"/>
-      <c r="F15" s="171">
+      <c r="E15" s="184"/>
+      <c r="F15" s="179">
         <f>F14*G14</f>
         <v>1724999.9999999995</v>
       </c>
-      <c r="G15" s="173"/>
-      <c r="H15" s="172">
+      <c r="G15" s="180"/>
+      <c r="H15" s="184">
         <f>H14*I14</f>
         <v>1983749.9999999995</v>
       </c>
-      <c r="I15" s="172"/>
-      <c r="J15" s="171">
+      <c r="I15" s="184"/>
+      <c r="J15" s="179">
         <f>J14*K14</f>
         <v>2281312.4999999991</v>
       </c>
-      <c r="K15" s="173"/>
-      <c r="L15" s="172">
+      <c r="K15" s="180"/>
+      <c r="L15" s="184">
         <f>L14*M14</f>
         <v>2623509.3749999991</v>
       </c>
-      <c r="M15" s="172"/>
-      <c r="N15" s="171">
+      <c r="M15" s="184"/>
+      <c r="N15" s="179">
         <f>N14*O14</f>
         <v>3017035.7812499986</v>
       </c>
-      <c r="O15" s="173"/>
-      <c r="P15" s="101"/>
-    </row>
-    <row r="16" spans="2:16" ht="13" thickBot="1">
-      <c r="B16" s="101"/>
-      <c r="C16" s="168" t="s">
+      <c r="O15" s="180"/>
+      <c r="P15" s="100"/>
+    </row>
+    <row r="16" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="100"/>
+      <c r="C16" s="189" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="111"/>
-      <c r="E16" s="111"/>
-      <c r="F16" s="111">
+      <c r="D16" s="110"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="110">
         <f>0.5*F10</f>
         <v>57.499999999999993</v>
       </c>
-      <c r="G16" s="111">
+      <c r="G16" s="110">
         <v>100000</v>
       </c>
-      <c r="H16" s="111">
+      <c r="H16" s="110">
         <f>0.5*H10</f>
         <v>66.124999999999986</v>
       </c>
-      <c r="I16" s="111">
+      <c r="I16" s="110">
         <v>100000</v>
       </c>
-      <c r="J16" s="111">
+      <c r="J16" s="110">
         <f>0.5*J10</f>
         <v>76.043749999999974</v>
       </c>
-      <c r="K16" s="111">
+      <c r="K16" s="110">
         <v>100000</v>
       </c>
-      <c r="L16" s="111">
+      <c r="L16" s="110">
         <f>0.5*L10</f>
         <v>87.450312499999967</v>
       </c>
-      <c r="M16" s="111">
+      <c r="M16" s="110">
         <v>100000</v>
       </c>
-      <c r="N16" s="111">
+      <c r="N16" s="110">
         <f>0.5*N10</f>
         <v>100.56785937499995</v>
       </c>
-      <c r="O16" s="111">
+      <c r="O16" s="110">
         <v>100000</v>
       </c>
-      <c r="P16" s="101"/>
-    </row>
-    <row r="17" spans="2:16" ht="13" thickBot="1">
-      <c r="B17" s="101"/>
-      <c r="C17" s="170"/>
-      <c r="D17" s="166">
+      <c r="P16" s="100"/>
+    </row>
+    <row r="17" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="100"/>
+      <c r="C17" s="191"/>
+      <c r="D17" s="175">
         <f>D16*E16</f>
         <v>0</v>
       </c>
-      <c r="E17" s="167"/>
-      <c r="F17" s="166">
+      <c r="E17" s="178"/>
+      <c r="F17" s="175">
         <f>F16*G16</f>
         <v>5749999.9999999991</v>
       </c>
-      <c r="G17" s="182"/>
-      <c r="H17" s="167">
+      <c r="G17" s="176"/>
+      <c r="H17" s="178">
         <f>H16*I16</f>
         <v>6612499.9999999981</v>
       </c>
-      <c r="I17" s="167"/>
-      <c r="J17" s="166">
+      <c r="I17" s="178"/>
+      <c r="J17" s="175">
         <f>J16*K16</f>
         <v>7604374.9999999972</v>
       </c>
-      <c r="K17" s="182"/>
-      <c r="L17" s="167">
+      <c r="K17" s="176"/>
+      <c r="L17" s="178">
         <f>L16*M16</f>
         <v>8745031.2499999963</v>
       </c>
-      <c r="M17" s="167"/>
-      <c r="N17" s="166">
+      <c r="M17" s="178"/>
+      <c r="N17" s="175">
         <f>N16*O16</f>
         <v>10056785.937499996</v>
       </c>
-      <c r="O17" s="182"/>
-      <c r="P17" s="101"/>
-    </row>
-    <row r="18" spans="2:16" ht="13" thickBot="1">
-      <c r="B18" s="101"/>
-      <c r="C18" s="105" t="s">
+      <c r="O17" s="176"/>
+      <c r="P17" s="100"/>
+    </row>
+    <row r="18" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="100"/>
+      <c r="C18" s="104" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="175">
+      <c r="D18" s="173">
         <f>D7+D9+D11+D13+D15+D17</f>
         <v>109500000</v>
       </c>
-      <c r="E18" s="176"/>
-      <c r="F18" s="175">
+      <c r="E18" s="177"/>
+      <c r="F18" s="173">
         <f>F7+F9+F11+F13+F15+F17</f>
         <v>135999999.99999997</v>
       </c>
-      <c r="G18" s="177"/>
-      <c r="H18" s="176">
+      <c r="G18" s="174"/>
+      <c r="H18" s="177">
         <f>H7+H9+H11+H13+H15+H17</f>
         <v>153591999.99999997</v>
       </c>
-      <c r="I18" s="176"/>
-      <c r="J18" s="175">
+      <c r="I18" s="177"/>
+      <c r="J18" s="173">
         <f>J7+J9+J11+J13+J15+J17</f>
         <v>173567527.27272725</v>
       </c>
-      <c r="K18" s="177"/>
-      <c r="L18" s="176">
+      <c r="K18" s="174"/>
+      <c r="L18" s="177">
         <f>L7+L9+L11+L13+L15+L17</f>
         <v>196260904.29752061</v>
       </c>
-      <c r="M18" s="176"/>
-      <c r="N18" s="175">
+      <c r="M18" s="177"/>
+      <c r="N18" s="173">
         <f>N7+N9+N11+N13+N15+N17</f>
         <v>222054492.23365882</v>
       </c>
-      <c r="O18" s="177"/>
-      <c r="P18" s="101"/>
-    </row>
-    <row r="19" spans="2:16">
-      <c r="B19" s="101"/>
-      <c r="C19" s="101"/>
-      <c r="D19" s="101"/>
-      <c r="E19" s="101"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="101"/>
-      <c r="H19" s="101"/>
-      <c r="I19" s="101"/>
-      <c r="J19" s="101"/>
-      <c r="K19" s="101"/>
-      <c r="L19" s="101"/>
-      <c r="M19" s="101"/>
-      <c r="N19" s="101"/>
-      <c r="O19" s="101"/>
-      <c r="P19" s="101"/>
-    </row>
-    <row r="20" spans="2:16">
-      <c r="C20" s="101"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="101"/>
-      <c r="H20" s="101"/>
-      <c r="I20" s="101"/>
-      <c r="J20" s="101"/>
-      <c r="K20" s="101"/>
-      <c r="L20" s="101"/>
-      <c r="M20" s="101"/>
-      <c r="N20" s="101"/>
-      <c r="O20" s="101"/>
-      <c r="P20" s="101"/>
-    </row>
-    <row r="21" spans="2:16">
-      <c r="C21" s="164" t="s">
+      <c r="O18" s="174"/>
+      <c r="P18" s="100"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B19" s="100"/>
+      <c r="C19" s="100"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="100"/>
+      <c r="F19" s="100"/>
+      <c r="G19" s="100"/>
+      <c r="H19" s="100"/>
+      <c r="I19" s="100"/>
+      <c r="J19" s="100"/>
+      <c r="K19" s="100"/>
+      <c r="L19" s="100"/>
+      <c r="M19" s="100"/>
+      <c r="N19" s="100"/>
+      <c r="O19" s="100"/>
+      <c r="P19" s="100"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="C20" s="100"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="100"/>
+      <c r="F20" s="100"/>
+      <c r="G20" s="100"/>
+      <c r="H20" s="100"/>
+      <c r="I20" s="100"/>
+      <c r="J20" s="100"/>
+      <c r="K20" s="100"/>
+      <c r="L20" s="100"/>
+      <c r="M20" s="100"/>
+      <c r="N20" s="100"/>
+      <c r="O20" s="100"/>
+      <c r="P20" s="100"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="C21" s="188" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="2:16">
-      <c r="C22" s="164"/>
-    </row>
-    <row r="23" spans="2:16">
-      <c r="C23" s="148">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="C22" s="188"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="C23" s="147">
         <v>50000</v>
       </c>
     </row>
-    <row r="25" spans="2:16" ht="24">
-      <c r="C25" s="144" t="s">
+    <row r="25" spans="2:16" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C25" s="143" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="2:16">
-      <c r="C26" s="145">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="C26" s="144">
         <v>0.15</v>
       </c>
     </row>
-    <row r="28" spans="2:16" ht="24">
-      <c r="C28" s="146" t="s">
+    <row r="28" spans="2:16" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="C28" s="145" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="2:16">
-      <c r="C29" s="151">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="C29" s="150">
         <f>(F6-D6)/F6</f>
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:16">
-      <c r="C30" s="150"/>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="C30" s="149"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="L13:M13"/>
     <mergeCell ref="D17:E17"/>
@@ -3611,6 +3579,45 @@
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="J15:K15"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -3629,55 +3636,56 @@
   <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="101"/>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="G1" s="101"/>
-    </row>
-    <row r="2" spans="1:13" ht="13" thickBot="1">
-      <c r="A2" s="101"/>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="G2" s="101"/>
-    </row>
-    <row r="3" spans="1:13" ht="13" thickBot="1">
-      <c r="A3" s="101"/>
-      <c r="B3" s="128" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="100"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="G1" s="100"/>
+    </row>
+    <row r="2" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="100"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="G2" s="100"/>
+    </row>
+    <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="100"/>
+      <c r="B3" s="127" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="127"/>
+      <c r="C3" s="126"/>
       <c r="D3" s="20" t="s">
         <v>39</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="130"/>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="101"/>
-      <c r="B4" s="191" t="s">
+      <c r="G3" s="129"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="100"/>
+      <c r="B4" s="195" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="192"/>
+      <c r="C4" s="196"/>
       <c r="D4" s="6">
         <v>600000</v>
       </c>
@@ -3685,14 +3693,14 @@
         <f>D4*12</f>
         <v>7200000</v>
       </c>
-      <c r="G4" s="101"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="101"/>
-      <c r="B5" s="187" t="s">
+      <c r="G4" s="100"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="100"/>
+      <c r="B5" s="193" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="188"/>
+      <c r="C5" s="194"/>
       <c r="D5" s="4">
         <f>IF('HW y SW'!C5=0,100000,0)</f>
         <v>0</v>
@@ -3701,32 +3709,32 @@
         <f>'HW y SW'!G4</f>
         <v>500000</v>
       </c>
-      <c r="G5" s="101"/>
-      <c r="H5" s="195">
+      <c r="G5" s="100"/>
+      <c r="H5" s="156">
         <v>1</v>
       </c>
-      <c r="I5" s="195">
+      <c r="I5" s="156">
         <v>2</v>
       </c>
-      <c r="J5" s="195">
+      <c r="J5" s="156">
         <v>3</v>
       </c>
-      <c r="K5" s="195">
+      <c r="K5" s="156">
         <v>4</v>
       </c>
-      <c r="L5" s="195">
+      <c r="L5" s="156">
         <v>5</v>
       </c>
-      <c r="M5" s="195">
+      <c r="M5" s="156">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="101"/>
-      <c r="B6" s="187" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="100"/>
+      <c r="B6" s="193" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="188"/>
+      <c r="C6" s="194"/>
       <c r="D6" s="4">
         <f>PERSONAL!E12</f>
         <v>8000000</v>
@@ -3735,40 +3743,40 @@
         <f t="shared" ref="E6:E11" si="0">D6*12</f>
         <v>96000000</v>
       </c>
-      <c r="G6" s="196" t="s">
+      <c r="G6" s="157" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="197">
+      <c r="H6" s="158">
         <f>E6</f>
         <v>96000000</v>
       </c>
-      <c r="I6" s="198">
+      <c r="I6" s="159">
         <f>H6*(1+$I$10)</f>
         <v>105600000.00000001</v>
       </c>
-      <c r="J6" s="198">
+      <c r="J6" s="159">
         <f t="shared" ref="J6:M6" si="1">I6*(1+$I$10)</f>
         <v>116160000.00000003</v>
       </c>
-      <c r="K6" s="198">
+      <c r="K6" s="159">
         <f t="shared" si="1"/>
         <v>127776000.00000004</v>
       </c>
-      <c r="L6" s="198">
+      <c r="L6" s="159">
         <f t="shared" si="1"/>
         <v>140553600.00000006</v>
       </c>
-      <c r="M6" s="198">
+      <c r="M6" s="159">
         <f t="shared" si="1"/>
         <v>154608960.00000009</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="101"/>
-      <c r="B7" s="187" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="100"/>
+      <c r="B7" s="193" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="188"/>
+      <c r="C7" s="194"/>
       <c r="D7" s="4">
         <v>100000</v>
       </c>
@@ -3776,78 +3784,78 @@
         <f t="shared" si="0"/>
         <v>1200000</v>
       </c>
-      <c r="G7" s="196" t="s">
+      <c r="G7" s="157" t="s">
         <v>130</v>
       </c>
-      <c r="H7" s="197">
+      <c r="H7" s="158">
         <f>SUM(E4:E13)-H6</f>
         <v>17378600</v>
       </c>
-      <c r="I7" s="198">
+      <c r="I7" s="159">
         <f>H7*(1+$I$11)</f>
         <v>18247530</v>
       </c>
-      <c r="J7" s="198">
+      <c r="J7" s="159">
         <f t="shared" ref="J7:M7" si="2">I7*(1+$I$11)</f>
         <v>19159906.5</v>
       </c>
-      <c r="K7" s="198">
+      <c r="K7" s="159">
         <f t="shared" si="2"/>
         <v>20117901.824999999</v>
       </c>
-      <c r="L7" s="198">
+      <c r="L7" s="159">
         <f t="shared" si="2"/>
         <v>21123796.916250002</v>
       </c>
-      <c r="M7" s="198">
+      <c r="M7" s="159">
         <f t="shared" si="2"/>
         <v>22179986.762062501</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="101"/>
-      <c r="B8" s="187" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="100"/>
+      <c r="B8" s="193" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="188"/>
+      <c r="C8" s="194"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4">
         <v>13000</v>
       </c>
-      <c r="G8" s="199" t="s">
+      <c r="G8" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="200">
+      <c r="H8" s="161">
         <f>H6+H7</f>
         <v>113378600</v>
       </c>
-      <c r="I8" s="201">
+      <c r="I8" s="162">
         <f t="shared" ref="I8:M8" si="3">SUM(I6:I7)</f>
         <v>123847530.00000001</v>
       </c>
-      <c r="J8" s="201">
+      <c r="J8" s="162">
         <f t="shared" si="3"/>
         <v>135319906.50000003</v>
       </c>
-      <c r="K8" s="201">
+      <c r="K8" s="162">
         <f t="shared" si="3"/>
         <v>147893901.82500005</v>
       </c>
-      <c r="L8" s="201">
+      <c r="L8" s="162">
         <f t="shared" si="3"/>
         <v>161677396.91625005</v>
       </c>
-      <c r="M8" s="201">
+      <c r="M8" s="162">
         <f t="shared" si="3"/>
         <v>176788946.76206258</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="101"/>
-      <c r="B9" s="187" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="100"/>
+      <c r="B9" s="193" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="188"/>
+      <c r="C9" s="194"/>
       <c r="D9" s="4">
         <v>50000</v>
       </c>
@@ -3855,14 +3863,14 @@
         <f t="shared" si="0"/>
         <v>600000</v>
       </c>
-      <c r="G9" s="101"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="101"/>
-      <c r="B10" s="187" t="s">
+      <c r="G9" s="100"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="100"/>
+      <c r="B10" s="193" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="188"/>
+      <c r="C10" s="194"/>
       <c r="D10" s="4">
         <v>45000</v>
       </c>
@@ -3870,20 +3878,20 @@
         <f t="shared" si="0"/>
         <v>540000</v>
       </c>
-      <c r="G10" s="202" t="s">
+      <c r="G10" s="192" t="s">
         <v>132</v>
       </c>
-      <c r="H10" s="202"/>
-      <c r="I10" s="203">
+      <c r="H10" s="192"/>
+      <c r="I10" s="163">
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="101"/>
-      <c r="B11" s="187" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="100"/>
+      <c r="B11" s="193" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="188"/>
+      <c r="C11" s="194"/>
       <c r="D11" s="4">
         <v>45000</v>
       </c>
@@ -3891,36 +3899,36 @@
         <f t="shared" si="0"/>
         <v>540000</v>
       </c>
-      <c r="G11" s="202" t="s">
+      <c r="G11" s="192" t="s">
         <v>133</v>
       </c>
-      <c r="H11" s="202"/>
-      <c r="I11" s="203">
+      <c r="H11" s="192"/>
+      <c r="I11" s="163">
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="101"/>
-      <c r="B12" s="187" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="100"/>
+      <c r="B12" s="193" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="188"/>
+      <c r="C12" s="194"/>
       <c r="D12" s="4">
-        <f>'CREACIÓN CURSOS'!D9</f>
+        <f>'CREACIÓN CURSOS'!C9</f>
         <v>1100000</v>
       </c>
       <c r="E12" s="4">
-        <f>'CREACIÓN CURSOS'!D14</f>
+        <f>'CREACIÓN CURSOS'!C14</f>
         <v>4400000</v>
       </c>
-      <c r="G12" s="101"/>
-    </row>
-    <row r="13" spans="1:13" ht="13" thickBot="1">
-      <c r="A13" s="101"/>
-      <c r="B13" s="183" t="s">
+      <c r="G12" s="100"/>
+    </row>
+    <row r="13" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="100"/>
+      <c r="B13" s="197" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="185"/>
+      <c r="C13" s="199"/>
       <c r="D13" s="5">
         <f>SUM(D4:D12)*0.02</f>
         <v>198800</v>
@@ -3929,92 +3937,92 @@
         <f>D13*12</f>
         <v>2385600</v>
       </c>
-      <c r="G13" s="101"/>
-    </row>
-    <row r="14" spans="1:13" ht="13" thickBot="1">
-      <c r="A14" s="101"/>
-      <c r="B14" s="101"/>
-      <c r="C14" s="157" t="s">
+      <c r="G13" s="100"/>
+    </row>
+    <row r="14" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="100"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="186"/>
+      <c r="D14" s="200"/>
       <c r="E14" s="11">
         <f>SUM(E4:E13)</f>
         <v>113378600</v>
       </c>
-      <c r="G14" s="101"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="101"/>
-      <c r="B15" s="101"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="129"/>
-      <c r="E15" s="129"/>
-      <c r="G15" s="101"/>
-    </row>
-    <row r="16" spans="1:13" ht="13" thickBot="1">
-      <c r="A16" s="101"/>
-      <c r="B16" s="101"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="129"/>
-      <c r="E16" s="129"/>
-      <c r="G16" s="101"/>
-    </row>
-    <row r="17" spans="1:7" ht="13" thickBot="1">
-      <c r="A17" s="101"/>
-      <c r="B17" s="189" t="s">
+      <c r="G14" s="100"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="100"/>
+      <c r="B15" s="100"/>
+      <c r="C15" s="100"/>
+      <c r="D15" s="128"/>
+      <c r="E15" s="128"/>
+      <c r="G15" s="100"/>
+    </row>
+    <row r="16" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="100"/>
+      <c r="B16" s="100"/>
+      <c r="C16" s="100"/>
+      <c r="D16" s="128"/>
+      <c r="E16" s="128"/>
+      <c r="G16" s="100"/>
+    </row>
+    <row r="17" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="100"/>
+      <c r="B17" s="201" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="190"/>
-      <c r="D17" s="30" t="s">
+      <c r="C17" s="202"/>
+      <c r="D17" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="101"/>
-      <c r="G17" s="101"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="101"/>
-      <c r="B18" s="25" t="s">
+      <c r="E17" s="100"/>
+      <c r="G17" s="100"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="100"/>
+      <c r="B18" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="99">
+      <c r="C18" s="25"/>
+      <c r="D18" s="98">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E18" s="101"/>
-      <c r="G18" s="101"/>
-    </row>
-    <row r="19" spans="1:7" ht="13" thickBot="1">
-      <c r="A19" s="101"/>
-      <c r="B19" s="183" t="s">
+      <c r="E18" s="100"/>
+      <c r="G18" s="100"/>
+    </row>
+    <row r="19" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="100"/>
+      <c r="B19" s="197" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="184"/>
-      <c r="D19" s="100">
+      <c r="C19" s="198"/>
+      <c r="D19" s="99">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E19" s="101"/>
-      <c r="G19" s="101"/>
-    </row>
-    <row r="20" spans="1:7" ht="13" thickBot="1">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="126" t="s">
+      <c r="E19" s="100"/>
+      <c r="G19" s="100"/>
+    </row>
+    <row r="20" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="100"/>
+      <c r="B20" s="100"/>
+      <c r="C20" s="100"/>
+      <c r="D20" s="125" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="101"/>
-      <c r="G20" s="101"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="101"/>
-      <c r="E21" s="101"/>
-      <c r="G21" s="101"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="E20" s="100"/>
+      <c r="G20" s="100"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="100"/>
+      <c r="B21" s="100"/>
+      <c r="C21" s="100"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="100"/>
+      <c r="G21" s="100"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D23">
         <f>E14*D19</f>
         <v>566893</v>
@@ -4022,6 +4030,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="B9:C9"/>
@@ -4031,12 +4045,6 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -4054,61 +4062,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:G9"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:7" ht="13" thickBot="1"/>
-    <row r="7" spans="2:7" ht="13" thickBot="1">
-      <c r="B7" s="48"/>
-      <c r="C7" s="75" t="s">
+    <row r="6" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="47"/>
+      <c r="C7" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="75" t="s">
+      <c r="E7" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="75" t="s">
+      <c r="G7" s="74" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="13" thickBot="1">
-      <c r="B8" s="23" t="s">
+    <row r="8" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="49">
+      <c r="C8" s="48">
         <f>SUM(INVERSION!D11:D13)</f>
         <v>3160000</v>
       </c>
-      <c r="D8" s="50">
+      <c r="D8" s="49">
         <v>6</v>
       </c>
-      <c r="E8" s="49">
+      <c r="E8" s="48">
         <v>0</v>
       </c>
-      <c r="F8" s="51"/>
+      <c r="F8" s="50"/>
       <c r="G8" s="5">
         <f>(C8-E8)/D8</f>
         <v>526666.66666666663</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="13" thickBot="1">
-      <c r="F9" s="76" t="s">
+    <row r="9" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="47">
+      <c r="G9" s="46">
         <f>SUM(G8:G8)</f>
         <v>526666.66666666663</v>
       </c>
@@ -4127,242 +4135,245 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:F18"/>
+  <dimension ref="B4:F19"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="64">
+      <c r="C4" s="63">
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="57" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="60">
+      <c r="C5" s="59">
         <f>INVERSION!D20*'G. FINANCIERO'!C4</f>
         <v>12366000</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="149">
+      <c r="D5" s="51"/>
+      <c r="E5" s="148">
         <f>PMT(C6,B17,C5)</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="F5" s="149"/>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="63" t="s">
+      <c r="F5" s="148"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="65">
+      <c r="C6" s="64">
         <v>0.1</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="63" t="s">
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="66">
+      <c r="C7" s="65">
         <f>C5/B17</f>
         <v>2061000</v>
       </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-    </row>
-    <row r="10" spans="2:6" ht="17.25" customHeight="1" thickBot="1">
-      <c r="B10" s="59" t="s">
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+    </row>
+    <row r="10" spans="2:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="59" t="s">
+      <c r="E10" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="F10" s="59" t="s">
+      <c r="F10" s="58" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="13" thickBot="1">
-      <c r="B11" s="90" t="s">
+    <row r="11" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="89" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="91" t="s">
+      <c r="C11" s="90" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="92" t="s">
+      <c r="D11" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="93" t="s">
+      <c r="E11" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="94" t="s">
+      <c r="F11" s="93" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="61">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="60">
         <v>1</v>
       </c>
-      <c r="C12" s="62">
+      <c r="C12" s="61">
         <f>C5</f>
         <v>12366000</v>
       </c>
-      <c r="D12" s="67">
+      <c r="D12" s="66">
         <f t="shared" ref="D12:D17" si="0">$C$7</f>
         <v>2061000</v>
       </c>
-      <c r="E12" s="73">
+      <c r="E12" s="72">
         <f t="shared" ref="E12:E17" si="1">+$C$6*C12</f>
         <v>1236600</v>
       </c>
-      <c r="F12" s="70">
+      <c r="F12" s="69">
         <f t="shared" ref="F12:F17" si="2">+(D12+E12)</f>
         <v>3297600</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="54">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="53">
         <v>2</v>
       </c>
-      <c r="C13" s="53">
+      <c r="C13" s="52">
         <f>+(C12-D12)</f>
         <v>10305000</v>
       </c>
-      <c r="D13" s="68">
+      <c r="D13" s="67">
         <f>$C$7</f>
         <v>2061000</v>
       </c>
-      <c r="E13" s="73">
+      <c r="E13" s="72">
         <f t="shared" si="1"/>
         <v>1030500</v>
       </c>
-      <c r="F13" s="71">
+      <c r="F13" s="70">
         <f t="shared" si="2"/>
         <v>3091500</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
-      <c r="B14" s="54">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="53">
         <v>3</v>
       </c>
-      <c r="C14" s="53">
+      <c r="C14" s="52">
         <f>+(C13-D13)</f>
         <v>8244000</v>
       </c>
-      <c r="D14" s="68">
+      <c r="D14" s="67">
         <f t="shared" si="0"/>
         <v>2061000</v>
       </c>
-      <c r="E14" s="73">
+      <c r="E14" s="72">
         <f t="shared" si="1"/>
         <v>824400</v>
       </c>
-      <c r="F14" s="71">
+      <c r="F14" s="70">
         <f t="shared" si="2"/>
         <v>2885400</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
-      <c r="B15" s="54">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="53">
         <v>4</v>
       </c>
-      <c r="C15" s="53">
+      <c r="C15" s="52">
         <f>+(C14-D14)</f>
         <v>6183000</v>
       </c>
-      <c r="D15" s="68">
+      <c r="D15" s="67">
         <f t="shared" si="0"/>
         <v>2061000</v>
       </c>
-      <c r="E15" s="73">
+      <c r="E15" s="72">
         <f t="shared" si="1"/>
         <v>618300</v>
       </c>
-      <c r="F15" s="71">
+      <c r="F15" s="70">
         <f t="shared" si="2"/>
         <v>2679300</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
-      <c r="B16" s="54">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="53">
         <v>5</v>
       </c>
-      <c r="C16" s="53">
+      <c r="C16" s="52">
         <f>+(C15-D15)</f>
         <v>4122000</v>
       </c>
-      <c r="D16" s="68">
+      <c r="D16" s="67">
         <f t="shared" si="0"/>
         <v>2061000</v>
       </c>
-      <c r="E16" s="73">
+      <c r="E16" s="72">
         <f t="shared" si="1"/>
         <v>412200</v>
       </c>
-      <c r="F16" s="71">
+      <c r="F16" s="70">
         <f t="shared" si="2"/>
         <v>2473200</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="13" thickBot="1">
-      <c r="B17" s="55">
+    <row r="17" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="54">
         <v>6</v>
       </c>
-      <c r="C17" s="56">
+      <c r="C17" s="55">
         <f>+(C16-D16)</f>
         <v>2061000</v>
       </c>
-      <c r="D17" s="69">
+      <c r="D17" s="68">
         <f t="shared" si="0"/>
         <v>2061000</v>
       </c>
-      <c r="E17" s="74">
+      <c r="E17" s="73">
         <f t="shared" si="1"/>
         <v>206100</v>
       </c>
-      <c r="F17" s="72">
+      <c r="F17" s="71">
         <f t="shared" si="2"/>
         <v>2267100</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="13" thickBot="1">
-      <c r="C18" s="56"/>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="52"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="205"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4381,102 +4392,102 @@
   <sheetPr codeName="Hoja3" enableFormatConditionsCalculation="0"/>
   <dimension ref="B3:G16"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="13" thickBot="1">
+    <row r="3" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="13" thickBot="1">
+    <row r="4" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
         <v>3</v>
       </c>
       <c r="F4" t="s">
         <v>116</v>
       </c>
-      <c r="G4" s="152">
+      <c r="G4" s="151">
         <v>500000</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="13" thickBot="1">
-      <c r="B5" s="39" t="s">
+    <row r="5" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="38" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="3">
         <v>4000000</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="13" thickBot="1">
-      <c r="B6" s="37" t="s">
+    <row r="6" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="37">
         <f>SUM(C5)</f>
         <v>4000000</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="2:7" ht="13" thickBot="1">
+    <row r="11" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:7" ht="13" thickBot="1">
+    <row r="12" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="31" t="s">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="31">
         <v>500000</v>
       </c>
     </row>
-    <row r="14" spans="2:7">
-      <c r="B14" s="33" t="s">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="34">
+      <c r="C14" s="33">
         <v>500000</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="13" thickBot="1">
-      <c r="B15" s="33" t="s">
+    <row r="15" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="33">
         <v>500000</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="13" thickBot="1">
-      <c r="B16" s="35" t="s">
+    <row r="16" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="36">
+      <c r="C16" s="35">
         <f>SUM(C13:C15)</f>
         <v>1500000</v>
       </c>
@@ -4498,16 +4509,17 @@
   <sheetPr codeName="Hoja4" enableFormatConditionsCalculation="0"/>
   <dimension ref="B1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="13" thickBot="1">
+    <row r="1" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F1">
         <v>2</v>
       </c>
@@ -4524,13 +4536,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="13" thickBot="1">
-      <c r="D2" s="189" t="s">
+    <row r="2" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="201" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="193"/>
-    </row>
-    <row r="3" spans="2:10" ht="13" thickBot="1">
+      <c r="E2" s="203"/>
+    </row>
+    <row r="3" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
@@ -4544,22 +4556,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
-      <c r="B4" s="96">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="95">
         <v>1</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="45">
+      <c r="D4" s="44">
         <v>1500000</v>
       </c>
-      <c r="E4" s="98">
+      <c r="E4" s="97">
         <f t="shared" ref="E4:E11" si="0">B4*D4</f>
         <v>1500000</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="12">
         <v>1</v>
       </c>
@@ -4574,7 +4586,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="12">
         <v>2</v>
       </c>
@@ -4589,7 +4601,7 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="12">
         <v>3</v>
       </c>
@@ -4604,7 +4616,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
         <v>1</v>
       </c>
@@ -4619,7 +4631,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
         <v>1</v>
       </c>
@@ -4634,7 +4646,7 @@
         <v>850000</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="12">
         <v>1</v>
       </c>
@@ -4649,7 +4661,7 @@
         <v>850000</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="13" thickBot="1">
+    <row r="11" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="16">
         <v>1</v>
       </c>
@@ -4664,8 +4676,8 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="13" thickBot="1">
-      <c r="E12" s="95">
+    <row r="12" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="94">
         <f>SUM(E4:E11)</f>
         <v>8000000</v>
       </c>
@@ -4708,132 +4720,136 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja5" enableFormatConditionsCalculation="0"/>
-  <dimension ref="C3:J14"/>
+  <dimension ref="B3:I14"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21:F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" ht="13" thickBot="1"/>
-    <row r="4" spans="3:10" ht="13" thickBot="1">
-      <c r="C4" s="194" t="s">
+    <row r="3" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="204" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="186"/>
-    </row>
-    <row r="5" spans="3:10" ht="13" thickBot="1">
-      <c r="C5" s="27" t="s">
+      <c r="C4" s="200"/>
+    </row>
+    <row r="5" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="3:10">
-      <c r="C6" s="21" t="s">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="4">
+      <c r="C6" s="4">
         <v>500000</v>
       </c>
     </row>
-    <row r="7" spans="3:10">
-      <c r="C7" s="7" t="s">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="4">
+      <c r="C7" s="4">
         <v>100000</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="3:10" ht="13" thickBot="1">
-      <c r="C8" s="112" t="s">
+    <row r="8" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="111" t="s">
         <v>103</v>
       </c>
-      <c r="D8" s="5">
+      <c r="C8" s="5">
         <v>500000</v>
       </c>
     </row>
-    <row r="9" spans="3:10" ht="13" thickBot="1">
-      <c r="C9" s="28" t="s">
+    <row r="9" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="36">
-        <f>SUM(D6:D8)</f>
+      <c r="C9" s="35">
+        <f>SUM(C6:C8)</f>
         <v>1100000</v>
       </c>
     </row>
-    <row r="11" spans="3:10" ht="13" thickBot="1"/>
-    <row r="12" spans="3:10" ht="13" thickBot="1">
-      <c r="D12" s="115" t="s">
+    <row r="11" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="114" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="121" t="s">
+      <c r="D12" s="120" t="s">
         <v>93</v>
       </c>
-      <c r="F12" s="119" t="s">
+      <c r="E12" s="118" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="121" t="s">
+      <c r="F12" s="120" t="s">
         <v>97</v>
       </c>
-      <c r="H12" s="119" t="s">
+      <c r="G12" s="118" t="s">
         <v>98</v>
       </c>
-      <c r="I12" s="121" t="s">
+      <c r="H12" s="120" t="s">
         <v>99</v>
       </c>
-      <c r="J12" s="120" t="s">
+      <c r="I12" s="119" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="3:10">
-      <c r="C13" s="115" t="s">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="114" t="s">
         <v>105</v>
       </c>
-      <c r="D13" s="31">
+      <c r="C13" s="30">
         <v>4</v>
       </c>
-      <c r="E13" s="21">
+      <c r="D13" s="21">
         <v>4</v>
       </c>
-      <c r="F13" s="116">
+      <c r="E13" s="115">
         <v>4</v>
       </c>
-      <c r="G13" s="21">
+      <c r="F13" s="21">
         <v>4</v>
       </c>
-      <c r="H13" s="116">
+      <c r="G13" s="115">
         <v>4</v>
       </c>
-      <c r="I13" s="21">
+      <c r="H13" s="21">
         <v>4</v>
       </c>
-      <c r="J13" s="117">
+      <c r="I13" s="116">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="3:10" ht="13" thickBot="1">
-      <c r="C14" s="118" t="s">
+    <row r="14" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="117" t="s">
         <v>19</v>
       </c>
+      <c r="C14" s="121">
+        <f>$C$9*C13</f>
+        <v>4400000</v>
+      </c>
       <c r="D14" s="122">
-        <f>$D$9*D13</f>
+        <f t="shared" ref="D14:I14" si="0">$C$9*D13</f>
         <v>4400000</v>
       </c>
       <c r="E14" s="123">
-        <f t="shared" ref="E14:J14" si="0">$D$9*E13</f>
+        <f t="shared" si="0"/>
         <v>4400000</v>
       </c>
-      <c r="F14" s="124">
+      <c r="F14" s="122">
         <f t="shared" si="0"/>
         <v>4400000</v>
       </c>
@@ -4841,22 +4857,18 @@
         <f t="shared" si="0"/>
         <v>4400000</v>
       </c>
-      <c r="H14" s="124">
+      <c r="H14" s="122">
         <f t="shared" si="0"/>
         <v>4400000</v>
       </c>
-      <c r="I14" s="123">
+      <c r="I14" s="124">
         <f t="shared" si="0"/>
         <v>4400000</v>
       </c>
-      <c r="J14" s="125">
-        <f t="shared" si="0"/>
-        <v>4400000</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>

</xml_diff>

<commit_message>
cambio formato de los Flujos
Cambio formato FLUJO PESIMISTA
Cambio formato FLUJO
</commit_message>
<xml_diff>
--- a/FLUJO PESIMISTA.xlsx
+++ b/FLUJO PESIMISTA.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="25605" windowHeight="14205" tabRatio="884"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14020" tabRatio="884"/>
   </bookViews>
   <sheets>
     <sheet name="FLUJO CAJA PESIMISTA" sheetId="8" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="CREACIÓN CURSOS" sheetId="5" r:id="rId9"/>
     <sheet name="Plan de Marketing" sheetId="11" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -440,15 +440,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="7">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;\ #,##0.00;[Red]\-&quot;$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="0.00000000%"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00;[Red]\-&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -473,12 +473,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -508,8 +502,25 @@
       <sz val="14"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -536,12 +547,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="51"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="31"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -558,8 +563,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BBB59"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="38">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -820,16 +849,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="double">
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -841,19 +870,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="medium">
         <color auto="1"/>
       </top>
@@ -866,90 +882,10 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right/>
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -987,56 +923,132 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFC2D69A"/>
+      </left>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="double">
-        <color auto="1"/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFC2D69A"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
+      <left/>
+      <right style="medium">
+        <color rgb="FFC2D69A"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFC2D69A"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFC2D69A"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFC2D69A"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFC2D69A"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFC2D69A"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFC2D69A"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFC2D69A"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
+      <right style="medium">
+        <color rgb="FFC2D69A"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
+      <top style="medium">
+        <color rgb="FFC2D69A"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color rgb="FFC2D69A"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFC2D69A"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFC2D69A"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFC2D69A"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFC2D69A"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="207">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1109,7 +1121,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1118,7 +1130,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1132,7 +1144,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1141,28 +1153,28 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1171,52 +1183,27 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1228,21 +1215,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1256,28 +1228,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1290,158 +1249,217 @@
     <xf numFmtId="3" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="4" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="5" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="10" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="9" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="27">
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
@@ -1452,6 +1470,8 @@
     <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
@@ -1462,9 +1482,11 @@
     <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentual" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1841,615 +1863,609 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J39"/>
+  <dimension ref="B1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="165" t="s">
+    <row r="1" spans="2:10" ht="17">
+      <c r="B1" s="134" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="165"/>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="165"/>
-      <c r="I1" s="165"/>
-      <c r="J1" s="165"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="51"/>
-      <c r="C4" s="83" t="s">
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="134"/>
+      <c r="J1" s="134"/>
+    </row>
+    <row r="4" spans="2:10" ht="14" thickBot="1">
+      <c r="B4" s="187"/>
+      <c r="C4" s="188" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-    </row>
-    <row r="5" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="76" t="s">
+      <c r="D4" s="189"/>
+      <c r="E4" s="187"/>
+      <c r="F4" s="187"/>
+      <c r="G4" s="187"/>
+      <c r="H4" s="187"/>
+      <c r="I4" s="187"/>
+      <c r="J4" s="187"/>
+    </row>
+    <row r="5" spans="2:10" ht="16" thickBot="1">
+      <c r="B5" s="174" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="174" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="85">
+      <c r="D5" s="175">
         <v>0</v>
       </c>
-      <c r="E5" s="85">
+      <c r="E5" s="175">
         <v>1</v>
       </c>
-      <c r="F5" s="85">
+      <c r="F5" s="175">
         <v>2</v>
       </c>
-      <c r="G5" s="85">
+      <c r="G5" s="175">
         <v>3</v>
       </c>
-      <c r="H5" s="85">
+      <c r="H5" s="175">
         <v>4</v>
       </c>
-      <c r="I5" s="85">
+      <c r="I5" s="175">
         <v>5</v>
       </c>
-      <c r="J5" s="85">
+      <c r="J5" s="175">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="78" t="s">
+    <row r="6" spans="2:10" ht="13" thickBot="1">
+      <c r="B6" s="176" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="79" t="s">
+      <c r="C6" s="176" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105">
+      <c r="D6" s="190"/>
+      <c r="E6" s="177">
         <f>INGRESOS!D18</f>
         <v>109500000</v>
       </c>
-      <c r="F6" s="105">
+      <c r="F6" s="177">
         <f>INGRESOS!F18</f>
         <v>135999999.99999997</v>
       </c>
-      <c r="G6" s="105">
+      <c r="G6" s="177">
         <f>INGRESOS!H18</f>
         <v>153591999.99999997</v>
       </c>
-      <c r="H6" s="105">
+      <c r="H6" s="177">
         <f>INGRESOS!J18</f>
         <v>173567527.27272725</v>
       </c>
-      <c r="I6" s="105">
+      <c r="I6" s="177">
         <f>INGRESOS!L18</f>
         <v>196260904.29752061</v>
       </c>
-      <c r="J6" s="105">
+      <c r="J6" s="177">
         <f>INGRESOS!N18</f>
         <v>222054492.23365882</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="78" t="s">
+    <row r="7" spans="2:10" ht="13" thickBot="1">
+      <c r="B7" s="176" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="176" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="105"/>
-      <c r="E7" s="105">
+      <c r="D7" s="191"/>
+      <c r="E7" s="177">
         <v>5000000</v>
       </c>
-      <c r="F7" s="105">
+      <c r="F7" s="177">
         <f>E7*1.3</f>
         <v>6500000</v>
       </c>
-      <c r="G7" s="105">
+      <c r="G7" s="177">
         <f>F7*1.3</f>
         <v>8450000</v>
       </c>
-      <c r="H7" s="105">
+      <c r="H7" s="177">
         <f>G7*1.3</f>
         <v>10985000</v>
       </c>
-      <c r="I7" s="105">
+      <c r="I7" s="177">
         <f>H7*1.3</f>
         <v>14280500</v>
       </c>
-      <c r="J7" s="105">
+      <c r="J7" s="177">
         <f>I7*1.3</f>
         <v>18564650</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="80" t="s">
+    <row r="8" spans="2:10" ht="13" thickBot="1">
+      <c r="B8" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="81" t="s">
+      <c r="C8" s="176" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="106"/>
-      <c r="E8" s="106">
+      <c r="D8" s="191"/>
+      <c r="E8" s="177">
         <f>-'CREACIÓN CURSOS'!D14</f>
         <v>-4400000</v>
       </c>
-      <c r="F8" s="106">
+      <c r="F8" s="177">
         <f>-'CREACIÓN CURSOS'!E14</f>
         <v>-4400000</v>
       </c>
-      <c r="G8" s="106">
+      <c r="G8" s="177">
         <f>-'CREACIÓN CURSOS'!F14</f>
         <v>-4400000</v>
       </c>
-      <c r="H8" s="106">
+      <c r="H8" s="177">
         <f>-'CREACIÓN CURSOS'!G14</f>
         <v>-4400000</v>
       </c>
-      <c r="I8" s="106">
+      <c r="I8" s="177">
         <f>-'CREACIÓN CURSOS'!H14</f>
         <v>-4400000</v>
       </c>
-      <c r="J8" s="106">
+      <c r="J8" s="177">
         <f>-'CREACIÓN CURSOS'!I14</f>
         <v>-4400000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="80" t="s">
+    <row r="9" spans="2:10" ht="13" thickBot="1">
+      <c r="B9" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="81" t="s">
+      <c r="C9" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="106"/>
-      <c r="E9" s="106">
+      <c r="D9" s="191"/>
+      <c r="E9" s="177">
         <f>-INGRESOS!D18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-8212500.0000000009</v>
       </c>
-      <c r="F9" s="106">
+      <c r="F9" s="177">
         <f>-INGRESOS!F18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-10200000</v>
       </c>
-      <c r="G9" s="106">
+      <c r="G9" s="177">
         <f>-INGRESOS!H18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-11519400</v>
       </c>
-      <c r="H9" s="106">
+      <c r="H9" s="177">
         <f>-INGRESOS!J18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-13017564.545454545</v>
       </c>
-      <c r="I9" s="106">
+      <c r="I9" s="177">
         <f>-INGRESOS!L18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-14719567.822314048</v>
       </c>
-      <c r="J9" s="106">
+      <c r="J9" s="177">
         <f>-INGRESOS!N18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-16654086.917524414</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="80" t="s">
+    <row r="10" spans="2:10" ht="13" thickBot="1">
+      <c r="B10" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="81" t="s">
+      <c r="C10" s="176" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="106"/>
-      <c r="E10" s="106">
+      <c r="D10" s="191"/>
+      <c r="E10" s="177">
         <f>-'ESTRUCTURA DE COSTOS'!H8</f>
         <v>-113378600</v>
       </c>
-      <c r="F10" s="106">
+      <c r="F10" s="177">
         <f>-'ESTRUCTURA DE COSTOS'!I8</f>
         <v>-123847530.00000001</v>
       </c>
-      <c r="G10" s="106">
+      <c r="G10" s="177">
         <f>-'ESTRUCTURA DE COSTOS'!J8</f>
         <v>-135319906.50000003</v>
       </c>
-      <c r="H10" s="106">
+      <c r="H10" s="177">
         <f>-'ESTRUCTURA DE COSTOS'!K8</f>
         <v>-147893901.82500005</v>
       </c>
-      <c r="I10" s="106">
+      <c r="I10" s="177">
         <f>-'ESTRUCTURA DE COSTOS'!L8</f>
         <v>-161677396.91625005</v>
       </c>
-      <c r="J10" s="106">
+      <c r="J10" s="177">
         <f>-'ESTRUCTURA DE COSTOS'!M8</f>
         <v>-176788946.76206258</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="80" t="s">
+    <row r="11" spans="2:10" ht="13" thickBot="1">
+      <c r="B11" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="81" t="s">
+      <c r="C11" s="176" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="106"/>
-      <c r="E11" s="106">
+      <c r="D11" s="191"/>
+      <c r="E11" s="177">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="F11" s="106">
+      <c r="F11" s="177">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="G11" s="106">
+      <c r="G11" s="177">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="H11" s="106">
+      <c r="H11" s="177">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="I11" s="106">
+      <c r="I11" s="177">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="J11" s="106">
+      <c r="J11" s="177">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="87" t="s">
+    <row r="12" spans="2:10" ht="13" thickBot="1">
+      <c r="B12" s="178" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="88" t="s">
+      <c r="C12" s="178" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="107"/>
-      <c r="E12" s="108">
+      <c r="D12" s="192"/>
+      <c r="E12" s="179">
         <f t="shared" ref="E12:J12" si="0">SUM(E6:E11)</f>
         <v>-12017766.666666666</v>
       </c>
-      <c r="F12" s="108">
+      <c r="F12" s="179">
         <f t="shared" si="0"/>
         <v>3525803.3333332888</v>
       </c>
-      <c r="G12" s="108">
+      <c r="G12" s="179">
         <f t="shared" si="0"/>
         <v>10276026.833333274</v>
       </c>
-      <c r="H12" s="108">
+      <c r="H12" s="179">
         <f t="shared" si="0"/>
         <v>18714394.235606004</v>
       </c>
-      <c r="I12" s="108">
+      <c r="I12" s="179">
         <f t="shared" si="0"/>
         <v>29217772.892289836</v>
       </c>
-      <c r="J12" s="108">
+      <c r="J12" s="179">
         <f t="shared" si="0"/>
         <v>42249441.88740515</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="80" t="s">
+    <row r="13" spans="2:10" ht="13" thickBot="1">
+      <c r="B13" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="81" t="s">
+      <c r="C13" s="176" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="106"/>
-      <c r="E13" s="106">
+      <c r="D13" s="191"/>
+      <c r="E13" s="177">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="F13" s="106">
+      <c r="F13" s="177">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="G13" s="106">
+      <c r="G13" s="177">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="H13" s="106">
+      <c r="H13" s="177">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="I13" s="106">
+      <c r="I13" s="177">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="J13" s="106">
+      <c r="J13" s="177">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="87" t="s">
+    <row r="14" spans="2:10" ht="13" thickBot="1">
+      <c r="B14" s="178" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="88" t="s">
+      <c r="C14" s="178" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="107"/>
-      <c r="E14" s="108">
+      <c r="D14" s="192"/>
+      <c r="E14" s="179">
         <f t="shared" ref="E14:J14" si="1">SUM(E12:E13)</f>
         <v>-14857091.532231411</v>
       </c>
-      <c r="F14" s="108">
+      <c r="F14" s="179">
         <f t="shared" si="1"/>
         <v>686478.4677685434</v>
       </c>
-      <c r="G14" s="108">
+      <c r="G14" s="179">
         <f t="shared" si="1"/>
         <v>7436701.9677685294</v>
       </c>
-      <c r="H14" s="108">
+      <c r="H14" s="179">
         <f t="shared" si="1"/>
         <v>15875069.370041259</v>
       </c>
-      <c r="I14" s="108">
+      <c r="I14" s="179">
         <f t="shared" si="1"/>
         <v>26378448.026725091</v>
       </c>
-      <c r="J14" s="108">
+      <c r="J14" s="179">
         <f t="shared" si="1"/>
         <v>39410117.021840401</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="80" t="s">
+    <row r="15" spans="2:10" ht="13" thickBot="1">
+      <c r="B15" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="81" t="s">
+      <c r="C15" s="176" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="106"/>
-      <c r="E15" s="106">
+      <c r="D15" s="191"/>
+      <c r="E15" s="177">
         <f t="shared" ref="E15:J15" si="2">+IF(E14&gt;0,-(E14*0.17),0)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="106">
+      <c r="F15" s="177">
         <f t="shared" si="2"/>
         <v>-116701.33952065239</v>
       </c>
-      <c r="G15" s="106">
+      <c r="G15" s="177">
         <f t="shared" si="2"/>
         <v>-1264239.3345206501</v>
       </c>
-      <c r="H15" s="106">
+      <c r="H15" s="177">
         <f t="shared" si="2"/>
         <v>-2698761.792907014</v>
       </c>
-      <c r="I15" s="106">
+      <c r="I15" s="177">
         <f t="shared" si="2"/>
         <v>-4484336.1645432655</v>
       </c>
-      <c r="J15" s="106">
+      <c r="J15" s="177">
         <f t="shared" si="2"/>
         <v>-6699719.8937128689</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="80" t="s">
+    <row r="16" spans="2:10" ht="13" thickBot="1">
+      <c r="B16" s="176" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="81" t="s">
+      <c r="C16" s="176" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="106"/>
-      <c r="E16" s="106">
+      <c r="D16" s="191"/>
+      <c r="E16" s="177">
         <f t="shared" ref="E16:J16" si="3">-(E11)</f>
         <v>526666.66666666663</v>
       </c>
-      <c r="F16" s="106">
+      <c r="F16" s="177">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
-      <c r="G16" s="106">
+      <c r="G16" s="177">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
-      <c r="H16" s="106">
+      <c r="H16" s="177">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
-      <c r="I16" s="106">
+      <c r="I16" s="177">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
-      <c r="J16" s="106">
+      <c r="J16" s="177">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="80" t="s">
+    <row r="17" spans="2:10" ht="13" thickBot="1">
+      <c r="B17" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="81" t="s">
+      <c r="C17" s="176" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="106"/>
-      <c r="E17" s="106">
+      <c r="D17" s="191"/>
+      <c r="E17" s="177">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="F17" s="106">
+      <c r="F17" s="177">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="G17" s="106">
+      <c r="G17" s="177">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="H17" s="106">
+      <c r="H17" s="177">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="I17" s="106">
+      <c r="I17" s="177">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="J17" s="106">
+      <c r="J17" s="177">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="80" t="s">
+    <row r="18" spans="2:10" ht="13" thickBot="1">
+      <c r="B18" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="81" t="s">
+      <c r="C18" s="176" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="106">
+      <c r="D18" s="193">
         <f>-INVERSION!D20</f>
         <v>-20610000</v>
       </c>
-      <c r="E18" s="106"/>
-      <c r="F18" s="106"/>
-      <c r="G18" s="106"/>
-      <c r="H18" s="106"/>
-      <c r="I18" s="106"/>
-      <c r="J18" s="106"/>
-    </row>
-    <row r="19" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="77"/>
-      <c r="C19" s="82" t="s">
+      <c r="E18" s="177"/>
+      <c r="F18" s="177"/>
+      <c r="G18" s="177"/>
+      <c r="H18" s="177"/>
+      <c r="I18" s="177"/>
+      <c r="J18" s="177"/>
+    </row>
+    <row r="19" spans="2:10" ht="13" thickBot="1">
+      <c r="B19" s="176"/>
+      <c r="C19" s="176" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="155">
+      <c r="D19" s="194">
         <f>'G. FINANCIERO'!C5</f>
         <v>12366000</v>
       </c>
-      <c r="E19" s="109"/>
-      <c r="F19" s="109"/>
-      <c r="G19" s="109"/>
-      <c r="H19" s="109"/>
-      <c r="I19" s="109"/>
-      <c r="J19" s="109"/>
-    </row>
-    <row r="20" spans="2:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="78" t="s">
+      <c r="E19" s="177"/>
+      <c r="F19" s="177"/>
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177"/>
+      <c r="J19" s="177"/>
+    </row>
+    <row r="20" spans="2:10" ht="13" thickBot="1">
+      <c r="B20" s="180" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="180" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="130">
+      <c r="D20" s="181">
         <f>SUM(D18:D19)</f>
         <v>-8244000</v>
       </c>
-      <c r="E20" s="130">
+      <c r="E20" s="182">
         <f t="shared" ref="E20:J20" si="4">SUM(E14:E19)</f>
         <v>-16391424.865564745</v>
       </c>
-      <c r="F20" s="130">
+      <c r="F20" s="182">
         <f t="shared" si="4"/>
         <v>-964556.2050854424</v>
       </c>
-      <c r="G20" s="130">
+      <c r="G20" s="182">
         <f t="shared" si="4"/>
         <v>4638129.2999145463</v>
       </c>
-      <c r="H20" s="130">
+      <c r="H20" s="182">
         <f t="shared" si="4"/>
         <v>11641974.24380091</v>
       </c>
-      <c r="I20" s="130">
+      <c r="I20" s="182">
         <f t="shared" si="4"/>
         <v>20359778.528848495</v>
       </c>
-      <c r="J20" s="130">
+      <c r="J20" s="182">
         <f t="shared" si="4"/>
         <v>31176063.794794198</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="135"/>
-      <c r="C21" s="135"/>
-      <c r="D21" s="136"/>
-      <c r="E21" s="136"/>
-      <c r="F21" s="136"/>
-      <c r="G21" s="136"/>
-      <c r="H21" s="136"/>
-      <c r="I21" s="136"/>
-      <c r="J21" s="136"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="131"/>
-      <c r="C22" s="137" t="s">
+    <row r="21" spans="2:10" ht="13" thickBot="1">
+      <c r="B21" s="195"/>
+      <c r="C21" s="195"/>
+      <c r="D21" s="196"/>
+      <c r="E21" s="196"/>
+      <c r="F21" s="196"/>
+      <c r="G21" s="196"/>
+      <c r="H21" s="196"/>
+      <c r="I21" s="196"/>
+      <c r="J21" s="196"/>
+    </row>
+    <row r="22" spans="2:10" ht="16" thickBot="1">
+      <c r="B22" s="183" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="142">
+      <c r="C22" s="184"/>
+      <c r="D22" s="185">
         <f>NPV(D24,E20:J20)+D20</f>
         <v>10079906.799768489</v>
       </c>
-      <c r="E22" s="136"/>
-      <c r="F22" s="138"/>
-      <c r="G22" s="136"/>
-      <c r="H22" s="136"/>
-      <c r="I22" s="136"/>
-      <c r="J22" s="136"/>
-    </row>
-    <row r="23" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="132"/>
-      <c r="C23" s="139" t="s">
+      <c r="E22" s="196"/>
+      <c r="F22" s="197"/>
+      <c r="G22" s="196"/>
+      <c r="H22" s="196"/>
+      <c r="I22" s="196"/>
+      <c r="J22" s="196"/>
+    </row>
+    <row r="23" spans="2:10" ht="16" thickBot="1">
+      <c r="B23" s="183" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="164">
+      <c r="C23" s="184"/>
+      <c r="D23" s="186">
         <f>IRR(D20:J20)</f>
         <v>0.25017156683584729</v>
       </c>
-      <c r="E23" s="135"/>
-      <c r="F23" s="140"/>
-      <c r="G23" s="135"/>
-      <c r="H23" s="135"/>
-      <c r="I23" s="135"/>
-      <c r="J23" s="135"/>
-    </row>
-    <row r="24" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="133"/>
-      <c r="C24" s="141" t="s">
+      <c r="E23" s="195"/>
+      <c r="F23" s="198"/>
+      <c r="G23" s="195"/>
+      <c r="H23" s="195"/>
+      <c r="I23" s="195"/>
+      <c r="J23" s="195"/>
+    </row>
+    <row r="24" spans="2:10" ht="16" thickBot="1">
+      <c r="B24" s="183" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="134">
+      <c r="C24" s="183"/>
+      <c r="D24" s="186">
         <v>0.15</v>
       </c>
-      <c r="E24" s="135"/>
-      <c r="F24" s="135"/>
-      <c r="G24" s="135"/>
-      <c r="H24" s="135"/>
-      <c r="I24" s="135"/>
-      <c r="J24" s="135"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C27" s="152"/>
-      <c r="D27" s="153"/>
+      <c r="E24" s="195"/>
+      <c r="F24" s="195"/>
+      <c r="G24" s="195"/>
+      <c r="H24" s="195"/>
+      <c r="I24" s="195"/>
+      <c r="J24" s="195"/>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="C27" s="121"/>
+      <c r="D27" s="122"/>
       <c r="I27" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="D31" s="154"/>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:10">
+      <c r="D31" s="123"/>
+    </row>
+    <row r="33" spans="3:10">
       <c r="C33" t="s">
         <v>8</v>
       </c>
@@ -2478,7 +2494,7 @@
         <v>154608960.00000009</v>
       </c>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:10">
       <c r="C34" t="s">
         <v>130</v>
       </c>
@@ -2507,7 +2523,7 @@
         <v>22179986.762062501</v>
       </c>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:10">
       <c r="C35" t="s">
         <v>131</v>
       </c>
@@ -2536,7 +2552,7 @@
         <v>176788946.76206258</v>
       </c>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:10">
       <c r="E37" s="2">
         <f>E10+E35</f>
         <v>0</v>
@@ -2562,21 +2578,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:10">
       <c r="C38" s="2">
         <f>F33-E33</f>
         <v>9600000.0000000149</v>
       </c>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:10">
       <c r="C39">
         <f>C38/12</f>
         <v>800000.00000000128</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+  <mergeCells count="4">
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B1:J1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -2598,29 +2617,29 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:2">
       <c r="B3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:2">
       <c r="B4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:2">
       <c r="B6" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:2">
       <c r="B7" t="s">
         <v>129</v>
       </c>
@@ -2640,73 +2659,73 @@
   <sheetPr codeName="Hoja2" enableFormatConditionsCalculation="0"/>
   <dimension ref="B3:D20"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="170" t="s">
+    <row r="3" spans="2:4" ht="13" thickBot="1"/>
+    <row r="4" spans="2:4" ht="13" thickBot="1">
+      <c r="B4" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="171"/>
+      <c r="C4" s="140"/>
       <c r="D4" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="168" t="s">
+    <row r="5" spans="2:4" ht="13" thickBot="1">
+      <c r="B5" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="169"/>
+      <c r="C5" s="138"/>
       <c r="D5" s="44"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4">
       <c r="B6" s="39"/>
       <c r="C6" s="40" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="13" thickBot="1">
       <c r="B7" s="39"/>
       <c r="C7" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="18"/>
     </row>
-    <row r="8" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="168" t="s">
+    <row r="8" spans="2:4" ht="13" thickBot="1">
+      <c r="B8" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="172"/>
+      <c r="C8" s="141"/>
       <c r="D8" s="45">
         <v>5000000</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="168" t="s">
+    <row r="9" spans="2:4" ht="13" thickBot="1">
+      <c r="B9" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="169"/>
+      <c r="C9" s="138"/>
       <c r="D9" s="45">
         <v>2500000</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="168" t="s">
+    <row r="10" spans="2:4" ht="13" thickBot="1">
+      <c r="B10" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="169"/>
+      <c r="C10" s="138"/>
       <c r="D10" s="44"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4">
       <c r="B11" s="41">
         <v>7</v>
       </c>
@@ -2718,7 +2737,7 @@
         <v>2800000</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4">
       <c r="B12" s="41">
         <v>1</v>
       </c>
@@ -2729,7 +2748,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" ht="13" thickBot="1">
       <c r="B13" s="42">
         <v>1</v>
       </c>
@@ -2740,14 +2759,14 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="168" t="s">
+    <row r="14" spans="2:4" ht="13" thickBot="1">
+      <c r="B14" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="169"/>
+      <c r="C14" s="138"/>
       <c r="D14" s="44"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4">
       <c r="B15" s="42"/>
       <c r="C15" s="13" t="s">
         <v>10</v>
@@ -2756,9 +2775,9 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4">
       <c r="B16" s="42"/>
-      <c r="C16" s="112" t="s">
+      <c r="C16" s="94" t="s">
         <v>106</v>
       </c>
       <c r="D16" s="14">
@@ -2766,7 +2785,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4">
       <c r="B17" s="42"/>
       <c r="C17" s="13" t="s">
         <v>84</v>
@@ -2775,7 +2794,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4">
       <c r="B18" s="42"/>
       <c r="C18" s="13" t="s">
         <v>83</v>
@@ -2784,20 +2803,20 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="13" thickBot="1">
       <c r="B19" s="43"/>
-      <c r="C19" s="113" t="s">
+      <c r="C19" s="95" t="s">
         <v>107</v>
       </c>
       <c r="D19" s="18">
         <v>5000000</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="166" t="s">
+    <row r="20" spans="2:4" ht="13" thickBot="1">
+      <c r="B20" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="167"/>
+      <c r="C20" s="136"/>
       <c r="D20" s="46">
         <f>SUM(D5:D19)</f>
         <v>20610000</v>
@@ -2828,741 +2847,780 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P30"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="3.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.85546875" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" customWidth="1"/>
+    <col min="5" max="5" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.83203125" customWidth="1"/>
+    <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="M2" s="100"/>
-      <c r="N2" s="100"/>
-      <c r="O2" s="100"/>
-      <c r="P2" s="100"/>
-    </row>
-    <row r="3" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
-      <c r="L3" s="100"/>
-      <c r="M3" s="100"/>
-      <c r="N3" s="100"/>
-      <c r="O3" s="100"/>
-      <c r="P3" s="100"/>
-    </row>
-    <row r="4" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="100"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="185" t="s">
+    <row r="2" spans="2:16">
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
+      <c r="N2" s="87"/>
+      <c r="O2" s="87"/>
+      <c r="P2" s="87"/>
+    </row>
+    <row r="3" spans="2:16" ht="13" thickBot="1">
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
+    </row>
+    <row r="4" spans="2:16" ht="13" thickBot="1">
+      <c r="B4" s="87"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="156" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="187"/>
-      <c r="F4" s="185" t="s">
+      <c r="E4" s="158"/>
+      <c r="F4" s="156" t="s">
         <v>96</v>
       </c>
-      <c r="G4" s="186"/>
-      <c r="H4" s="187" t="s">
+      <c r="G4" s="157"/>
+      <c r="H4" s="158" t="s">
         <v>97</v>
       </c>
-      <c r="I4" s="187"/>
-      <c r="J4" s="185" t="s">
+      <c r="I4" s="158"/>
+      <c r="J4" s="156" t="s">
         <v>98</v>
       </c>
-      <c r="K4" s="186"/>
-      <c r="L4" s="187" t="s">
+      <c r="K4" s="157"/>
+      <c r="L4" s="158" t="s">
         <v>99</v>
       </c>
-      <c r="M4" s="187"/>
-      <c r="N4" s="185" t="s">
+      <c r="M4" s="158"/>
+      <c r="N4" s="156" t="s">
         <v>100</v>
       </c>
-      <c r="O4" s="186"/>
-      <c r="P4" s="100"/>
-    </row>
-    <row r="5" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="101" t="s">
+      <c r="O4" s="157"/>
+      <c r="P4" s="87"/>
+    </row>
+    <row r="5" spans="2:16" ht="13" thickBot="1">
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="88" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="102" t="s">
+      <c r="E5" s="89" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="101" t="s">
+      <c r="F5" s="88" t="s">
         <v>91</v>
       </c>
-      <c r="G5" s="103" t="s">
+      <c r="G5" s="90" t="s">
         <v>92</v>
       </c>
-      <c r="H5" s="102" t="s">
+      <c r="H5" s="89" t="s">
         <v>91</v>
       </c>
-      <c r="I5" s="102" t="s">
+      <c r="I5" s="89" t="s">
         <v>92</v>
       </c>
-      <c r="J5" s="101" t="s">
+      <c r="J5" s="88" t="s">
         <v>91</v>
       </c>
-      <c r="K5" s="103" t="s">
+      <c r="K5" s="90" t="s">
         <v>92</v>
       </c>
-      <c r="L5" s="102" t="s">
+      <c r="L5" s="89" t="s">
         <v>91</v>
       </c>
-      <c r="M5" s="102" t="s">
+      <c r="M5" s="89" t="s">
         <v>92</v>
       </c>
-      <c r="N5" s="101" t="s">
+      <c r="N5" s="88" t="s">
         <v>91</v>
       </c>
-      <c r="O5" s="103" t="s">
+      <c r="O5" s="90" t="s">
         <v>92</v>
       </c>
-      <c r="P5" s="100"/>
-    </row>
-    <row r="6" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="100"/>
-      <c r="C6" s="189" t="s">
+      <c r="P5" s="87"/>
+    </row>
+    <row r="6" spans="2:16" ht="13" thickBot="1">
+      <c r="B6" s="87"/>
+      <c r="C6" s="146" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="146">
+      <c r="D6" s="115">
         <f>12*1*20</f>
         <v>240</v>
       </c>
-      <c r="E6" s="110">
+      <c r="E6" s="92">
         <v>180000</v>
       </c>
-      <c r="F6" s="110">
+      <c r="F6" s="92">
         <f>20*1.1*12</f>
         <v>264</v>
       </c>
-      <c r="G6" s="110">
+      <c r="G6" s="92">
         <v>180000</v>
       </c>
-      <c r="H6" s="110">
+      <c r="H6" s="92">
         <f>F6*(1+$C$29)</f>
         <v>288</v>
       </c>
-      <c r="I6" s="110">
+      <c r="I6" s="92">
         <v>180000</v>
       </c>
-      <c r="J6" s="110">
+      <c r="J6" s="92">
         <f>H6*(1+$C$29)</f>
         <v>314.18181818181813</v>
       </c>
-      <c r="K6" s="110">
+      <c r="K6" s="92">
         <v>180000</v>
       </c>
-      <c r="L6" s="110">
+      <c r="L6" s="92">
         <f>J6*(1+$C$29)</f>
         <v>342.7438016528925</v>
       </c>
-      <c r="M6" s="110">
+      <c r="M6" s="92">
         <v>180000</v>
       </c>
-      <c r="N6" s="110">
+      <c r="N6" s="92">
         <f>L6*(1+$C$29)</f>
         <v>373.90232907588268</v>
       </c>
-      <c r="O6" s="110">
+      <c r="O6" s="92">
         <v>180000</v>
       </c>
-      <c r="P6" s="100"/>
-    </row>
-    <row r="7" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="100"/>
-      <c r="C7" s="190"/>
-      <c r="D7" s="179">
+      <c r="P6" s="87"/>
+    </row>
+    <row r="7" spans="2:16" ht="13" thickBot="1">
+      <c r="B7" s="87"/>
+      <c r="C7" s="147"/>
+      <c r="D7" s="149">
         <f>D6*E6</f>
         <v>43200000</v>
       </c>
-      <c r="E7" s="184"/>
-      <c r="F7" s="179">
+      <c r="E7" s="150"/>
+      <c r="F7" s="149">
         <f>F6*G6</f>
         <v>47520000</v>
       </c>
-      <c r="G7" s="180"/>
-      <c r="H7" s="184">
+      <c r="G7" s="151"/>
+      <c r="H7" s="150">
         <f>H6*I6</f>
         <v>51840000</v>
       </c>
-      <c r="I7" s="184"/>
-      <c r="J7" s="179">
+      <c r="I7" s="150"/>
+      <c r="J7" s="149">
         <f>J6*K6</f>
         <v>56552727.272727266</v>
       </c>
-      <c r="K7" s="180"/>
-      <c r="L7" s="184">
+      <c r="K7" s="151"/>
+      <c r="L7" s="150">
         <f>L6*M6</f>
         <v>61693884.297520652</v>
       </c>
-      <c r="M7" s="184"/>
-      <c r="N7" s="179">
+      <c r="M7" s="150"/>
+      <c r="N7" s="149">
         <f>N6*O6</f>
         <v>67302419.23365888</v>
       </c>
-      <c r="O7" s="180"/>
-      <c r="P7" s="100"/>
-    </row>
-    <row r="8" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="100"/>
-      <c r="C8" s="189" t="s">
+      <c r="O7" s="151"/>
+      <c r="P7" s="87"/>
+    </row>
+    <row r="8" spans="2:16" ht="13" thickBot="1">
+      <c r="B8" s="87"/>
+      <c r="C8" s="146" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="110">
+      <c r="D8" s="92">
         <f>D10*0.9</f>
         <v>90</v>
       </c>
-      <c r="E8" s="110">
+      <c r="E8" s="92">
         <v>70000</v>
       </c>
-      <c r="F8" s="110">
+      <c r="F8" s="92">
         <f>(F10-D10)*0.9+0.2*D10</f>
         <v>33.499999999999986</v>
       </c>
-      <c r="G8" s="110">
+      <c r="G8" s="92">
         <v>70000</v>
       </c>
-      <c r="H8" s="110">
+      <c r="H8" s="92">
         <f>(H10-F10)*0.9+0.2*F10</f>
         <v>38.524999999999991</v>
       </c>
-      <c r="I8" s="110">
+      <c r="I8" s="92">
         <v>70000</v>
       </c>
-      <c r="J8" s="110">
+      <c r="J8" s="92">
         <f>(J10-H10)*0.9+0.2*H10</f>
         <v>44.30374999999998</v>
       </c>
-      <c r="K8" s="110">
+      <c r="K8" s="92">
         <v>70000</v>
       </c>
-      <c r="L8" s="110">
+      <c r="L8" s="92">
         <f>(L10-J10)*0.9+0.2*J10</f>
         <v>50.949312499999976</v>
       </c>
-      <c r="M8" s="110">
+      <c r="M8" s="92">
         <v>70000</v>
       </c>
-      <c r="N8" s="110">
+      <c r="N8" s="92">
         <f>(N10-L10)*0.9+0.2*L10</f>
         <v>58.591709374999965</v>
       </c>
-      <c r="O8" s="110">
+      <c r="O8" s="92">
         <v>70000</v>
       </c>
-      <c r="P8" s="100"/>
-    </row>
-    <row r="9" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="100"/>
-      <c r="C9" s="191"/>
-      <c r="D9" s="182">
+      <c r="P8" s="87"/>
+    </row>
+    <row r="9" spans="2:16" ht="13" thickBot="1">
+      <c r="B9" s="87"/>
+      <c r="C9" s="148"/>
+      <c r="D9" s="152">
         <f>D8*E8</f>
         <v>6300000</v>
       </c>
-      <c r="E9" s="181"/>
-      <c r="F9" s="182">
+      <c r="E9" s="143"/>
+      <c r="F9" s="152">
         <f>F8*G8</f>
         <v>2344999.9999999991</v>
       </c>
-      <c r="G9" s="183"/>
-      <c r="H9" s="181">
+      <c r="G9" s="159"/>
+      <c r="H9" s="143">
         <f>H8*I8</f>
         <v>2696749.9999999995</v>
       </c>
-      <c r="I9" s="181"/>
-      <c r="J9" s="182">
+      <c r="I9" s="143"/>
+      <c r="J9" s="152">
         <f>J8*K8</f>
         <v>3101262.4999999986</v>
       </c>
-      <c r="K9" s="183"/>
-      <c r="L9" s="181">
+      <c r="K9" s="159"/>
+      <c r="L9" s="143">
         <f>L8*M8</f>
         <v>3566451.8749999981</v>
       </c>
-      <c r="M9" s="181"/>
-      <c r="N9" s="182">
+      <c r="M9" s="143"/>
+      <c r="N9" s="152">
         <f>N8*O8</f>
         <v>4101419.6562499977</v>
       </c>
-      <c r="O9" s="183"/>
-      <c r="P9" s="100"/>
-    </row>
-    <row r="10" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="100"/>
-      <c r="C10" s="190" t="s">
+      <c r="O9" s="159"/>
+      <c r="P9" s="87"/>
+    </row>
+    <row r="10" spans="2:16" ht="13" thickBot="1">
+      <c r="B10" s="87"/>
+      <c r="C10" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="110">
+      <c r="D10" s="92">
         <v>100</v>
       </c>
-      <c r="E10" s="110">
+      <c r="E10" s="92">
         <f>$C$23*12</f>
         <v>600000</v>
       </c>
-      <c r="F10" s="110">
+      <c r="F10" s="92">
         <f>D10*(1+$C$26)</f>
         <v>114.99999999999999</v>
       </c>
-      <c r="G10" s="110">
+      <c r="G10" s="92">
         <f>$C$23*12</f>
         <v>600000</v>
       </c>
-      <c r="H10" s="110">
+      <c r="H10" s="92">
         <f>F10*(1+$C$26)</f>
         <v>132.24999999999997</v>
       </c>
-      <c r="I10" s="110">
+      <c r="I10" s="92">
         <f>$C$23*12</f>
         <v>600000</v>
       </c>
-      <c r="J10" s="110">
+      <c r="J10" s="92">
         <f>H10*(1+$C$26)</f>
         <v>152.08749999999995</v>
       </c>
-      <c r="K10" s="110">
+      <c r="K10" s="92">
         <f>$C$23*12</f>
         <v>600000</v>
       </c>
-      <c r="L10" s="110">
+      <c r="L10" s="92">
         <f>J10*(1+$C$26)</f>
         <v>174.90062499999993</v>
       </c>
-      <c r="M10" s="110">
+      <c r="M10" s="92">
         <f>$C$23*12</f>
         <v>600000</v>
       </c>
-      <c r="N10" s="110">
+      <c r="N10" s="92">
         <f>L10*(1+$C$26)</f>
         <v>201.13571874999991</v>
       </c>
-      <c r="O10" s="110">
+      <c r="O10" s="92">
         <f>$C$23*12</f>
         <v>600000</v>
       </c>
-      <c r="P10" s="100"/>
-    </row>
-    <row r="11" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="100"/>
-      <c r="C11" s="190"/>
-      <c r="D11" s="179">
+      <c r="P10" s="87"/>
+    </row>
+    <row r="11" spans="2:16" ht="13" thickBot="1">
+      <c r="B11" s="87"/>
+      <c r="C11" s="147"/>
+      <c r="D11" s="149">
         <f>D10*E10</f>
         <v>60000000</v>
       </c>
-      <c r="E11" s="184"/>
-      <c r="F11" s="179">
+      <c r="E11" s="150"/>
+      <c r="F11" s="149">
         <f>F10*G10</f>
         <v>68999999.999999985</v>
       </c>
-      <c r="G11" s="180"/>
-      <c r="H11" s="184">
+      <c r="G11" s="151"/>
+      <c r="H11" s="150">
         <f>H10*I10</f>
         <v>79349999.999999985</v>
       </c>
-      <c r="I11" s="184"/>
-      <c r="J11" s="179">
+      <c r="I11" s="150"/>
+      <c r="J11" s="149">
         <f>J10*K10</f>
         <v>91252499.99999997</v>
       </c>
-      <c r="K11" s="180"/>
-      <c r="L11" s="184">
+      <c r="K11" s="151"/>
+      <c r="L11" s="150">
         <f>L10*M10</f>
         <v>104940374.99999996</v>
       </c>
-      <c r="M11" s="184"/>
-      <c r="N11" s="179">
+      <c r="M11" s="150"/>
+      <c r="N11" s="149">
         <f>N10*O10</f>
         <v>120681431.24999994</v>
       </c>
-      <c r="O11" s="180"/>
-      <c r="P11" s="100"/>
-    </row>
-    <row r="12" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="100"/>
-      <c r="C12" s="189" t="s">
+      <c r="O11" s="151"/>
+      <c r="P11" s="87"/>
+    </row>
+    <row r="12" spans="2:16" ht="13" thickBot="1">
+      <c r="B12" s="87"/>
+      <c r="C12" s="146" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="110"/>
-      <c r="E12" s="110"/>
-      <c r="F12" s="110">
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="92">
         <f>0.7*F10</f>
         <v>80.499999999999986</v>
       </c>
-      <c r="G12" s="110">
+      <c r="G12" s="92">
         <f>10000*12</f>
         <v>120000</v>
       </c>
-      <c r="H12" s="110">
+      <c r="H12" s="92">
         <f>0.7*H10</f>
         <v>92.574999999999974</v>
       </c>
-      <c r="I12" s="110">
+      <c r="I12" s="92">
         <f>10000*12</f>
         <v>120000</v>
       </c>
-      <c r="J12" s="110">
+      <c r="J12" s="92">
         <f>0.7*J10</f>
         <v>106.46124999999996</v>
       </c>
-      <c r="K12" s="110">
+      <c r="K12" s="92">
         <f>10000*12</f>
         <v>120000</v>
       </c>
-      <c r="L12" s="110">
+      <c r="L12" s="92">
         <f>0.7*L10</f>
         <v>122.43043749999994</v>
       </c>
-      <c r="M12" s="110">
+      <c r="M12" s="92">
         <f>10000*12</f>
         <v>120000</v>
       </c>
-      <c r="N12" s="110">
+      <c r="N12" s="92">
         <f>0.7*N10</f>
         <v>140.79500312499994</v>
       </c>
-      <c r="O12" s="110">
+      <c r="O12" s="92">
         <f>10000*12</f>
         <v>120000</v>
       </c>
-      <c r="P12" s="100"/>
-    </row>
-    <row r="13" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="100"/>
-      <c r="C13" s="191"/>
-      <c r="D13" s="182">
+      <c r="P12" s="87"/>
+    </row>
+    <row r="13" spans="2:16" ht="13" thickBot="1">
+      <c r="B13" s="87"/>
+      <c r="C13" s="148"/>
+      <c r="D13" s="152">
         <f>D12*E12</f>
         <v>0</v>
       </c>
-      <c r="E13" s="181"/>
-      <c r="F13" s="182">
+      <c r="E13" s="143"/>
+      <c r="F13" s="152">
         <f>F12*G12</f>
         <v>9659999.9999999981</v>
       </c>
-      <c r="G13" s="183"/>
-      <c r="H13" s="181">
+      <c r="G13" s="159"/>
+      <c r="H13" s="143">
         <f>H12*I12</f>
         <v>11108999.999999996</v>
       </c>
-      <c r="I13" s="181"/>
-      <c r="J13" s="182">
+      <c r="I13" s="143"/>
+      <c r="J13" s="152">
         <f>J12*K12</f>
         <v>12775349.999999996</v>
       </c>
-      <c r="K13" s="183"/>
-      <c r="L13" s="181">
+      <c r="K13" s="159"/>
+      <c r="L13" s="143">
         <f>L12*M12</f>
         <v>14691652.499999993</v>
       </c>
-      <c r="M13" s="181"/>
-      <c r="N13" s="182">
+      <c r="M13" s="143"/>
+      <c r="N13" s="152">
         <f>N12*O12</f>
         <v>16895400.374999993</v>
       </c>
-      <c r="O13" s="183"/>
-      <c r="P13" s="100"/>
-    </row>
-    <row r="14" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="100"/>
-      <c r="C14" s="190" t="s">
+      <c r="O13" s="159"/>
+      <c r="P13" s="87"/>
+    </row>
+    <row r="14" spans="2:16" ht="13" thickBot="1">
+      <c r="B14" s="87"/>
+      <c r="C14" s="147" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="110"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110">
+      <c r="D14" s="92"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="92">
         <f>0.3*F10</f>
         <v>34.499999999999993</v>
       </c>
-      <c r="G14" s="110">
+      <c r="G14" s="92">
         <v>50000</v>
       </c>
-      <c r="H14" s="110">
+      <c r="H14" s="92">
         <f>0.3*H10</f>
         <v>39.67499999999999</v>
       </c>
-      <c r="I14" s="110">
+      <c r="I14" s="92">
         <v>50000</v>
       </c>
-      <c r="J14" s="110">
+      <c r="J14" s="92">
         <f>0.3*J10</f>
         <v>45.626249999999985</v>
       </c>
-      <c r="K14" s="110">
+      <c r="K14" s="92">
         <v>50000</v>
       </c>
-      <c r="L14" s="110">
+      <c r="L14" s="92">
         <f>0.3*L10</f>
         <v>52.47018749999998</v>
       </c>
-      <c r="M14" s="110">
+      <c r="M14" s="92">
         <v>50000</v>
       </c>
-      <c r="N14" s="110">
+      <c r="N14" s="92">
         <f>0.3*N10</f>
         <v>60.340715624999973</v>
       </c>
-      <c r="O14" s="110">
+      <c r="O14" s="92">
         <v>50000</v>
       </c>
-      <c r="P14" s="100"/>
-    </row>
-    <row r="15" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="100"/>
-      <c r="C15" s="190"/>
-      <c r="D15" s="179">
+      <c r="P14" s="87"/>
+    </row>
+    <row r="15" spans="2:16" ht="13" thickBot="1">
+      <c r="B15" s="87"/>
+      <c r="C15" s="147"/>
+      <c r="D15" s="149">
         <f>D14*E14</f>
         <v>0</v>
       </c>
-      <c r="E15" s="184"/>
-      <c r="F15" s="179">
+      <c r="E15" s="150"/>
+      <c r="F15" s="149">
         <f>F14*G14</f>
         <v>1724999.9999999995</v>
       </c>
-      <c r="G15" s="180"/>
-      <c r="H15" s="184">
+      <c r="G15" s="151"/>
+      <c r="H15" s="150">
         <f>H14*I14</f>
         <v>1983749.9999999995</v>
       </c>
-      <c r="I15" s="184"/>
-      <c r="J15" s="179">
+      <c r="I15" s="150"/>
+      <c r="J15" s="149">
         <f>J14*K14</f>
         <v>2281312.4999999991</v>
       </c>
-      <c r="K15" s="180"/>
-      <c r="L15" s="184">
+      <c r="K15" s="151"/>
+      <c r="L15" s="150">
         <f>L14*M14</f>
         <v>2623509.3749999991</v>
       </c>
-      <c r="M15" s="184"/>
-      <c r="N15" s="179">
+      <c r="M15" s="150"/>
+      <c r="N15" s="149">
         <f>N14*O14</f>
         <v>3017035.7812499986</v>
       </c>
-      <c r="O15" s="180"/>
-      <c r="P15" s="100"/>
-    </row>
-    <row r="16" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="100"/>
-      <c r="C16" s="189" t="s">
+      <c r="O15" s="151"/>
+      <c r="P15" s="87"/>
+    </row>
+    <row r="16" spans="2:16" ht="13" thickBot="1">
+      <c r="B16" s="87"/>
+      <c r="C16" s="146" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="110"/>
-      <c r="E16" s="110"/>
-      <c r="F16" s="110">
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92">
         <f>0.5*F10</f>
         <v>57.499999999999993</v>
       </c>
-      <c r="G16" s="110">
+      <c r="G16" s="92">
         <v>100000</v>
       </c>
-      <c r="H16" s="110">
+      <c r="H16" s="92">
         <f>0.5*H10</f>
         <v>66.124999999999986</v>
       </c>
-      <c r="I16" s="110">
+      <c r="I16" s="92">
         <v>100000</v>
       </c>
-      <c r="J16" s="110">
+      <c r="J16" s="92">
         <f>0.5*J10</f>
         <v>76.043749999999974</v>
       </c>
-      <c r="K16" s="110">
+      <c r="K16" s="92">
         <v>100000</v>
       </c>
-      <c r="L16" s="110">
+      <c r="L16" s="92">
         <f>0.5*L10</f>
         <v>87.450312499999967</v>
       </c>
-      <c r="M16" s="110">
+      <c r="M16" s="92">
         <v>100000</v>
       </c>
-      <c r="N16" s="110">
+      <c r="N16" s="92">
         <f>0.5*N10</f>
         <v>100.56785937499995</v>
       </c>
-      <c r="O16" s="110">
+      <c r="O16" s="92">
         <v>100000</v>
       </c>
-      <c r="P16" s="100"/>
-    </row>
-    <row r="17" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="100"/>
-      <c r="C17" s="191"/>
-      <c r="D17" s="175">
+      <c r="P16" s="87"/>
+    </row>
+    <row r="17" spans="2:16" ht="13" thickBot="1">
+      <c r="B17" s="87"/>
+      <c r="C17" s="148"/>
+      <c r="D17" s="144">
         <f>D16*E16</f>
         <v>0</v>
       </c>
-      <c r="E17" s="178"/>
-      <c r="F17" s="175">
+      <c r="E17" s="145"/>
+      <c r="F17" s="144">
         <f>F16*G16</f>
         <v>5749999.9999999991</v>
       </c>
-      <c r="G17" s="176"/>
-      <c r="H17" s="178">
+      <c r="G17" s="160"/>
+      <c r="H17" s="145">
         <f>H16*I16</f>
         <v>6612499.9999999981</v>
       </c>
-      <c r="I17" s="178"/>
-      <c r="J17" s="175">
+      <c r="I17" s="145"/>
+      <c r="J17" s="144">
         <f>J16*K16</f>
         <v>7604374.9999999972</v>
       </c>
-      <c r="K17" s="176"/>
-      <c r="L17" s="178">
+      <c r="K17" s="160"/>
+      <c r="L17" s="145">
         <f>L16*M16</f>
         <v>8745031.2499999963</v>
       </c>
-      <c r="M17" s="178"/>
-      <c r="N17" s="175">
+      <c r="M17" s="145"/>
+      <c r="N17" s="144">
         <f>N16*O16</f>
         <v>10056785.937499996</v>
       </c>
-      <c r="O17" s="176"/>
-      <c r="P17" s="100"/>
-    </row>
-    <row r="18" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="100"/>
-      <c r="C18" s="104" t="s">
+      <c r="O17" s="160"/>
+      <c r="P17" s="87"/>
+    </row>
+    <row r="18" spans="2:16" ht="13" thickBot="1">
+      <c r="B18" s="87"/>
+      <c r="C18" s="91" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="173">
+      <c r="D18" s="153">
         <f>D7+D9+D11+D13+D15+D17</f>
         <v>109500000</v>
       </c>
-      <c r="E18" s="177"/>
-      <c r="F18" s="173">
+      <c r="E18" s="154"/>
+      <c r="F18" s="153">
         <f>F7+F9+F11+F13+F15+F17</f>
         <v>135999999.99999997</v>
       </c>
-      <c r="G18" s="174"/>
-      <c r="H18" s="177">
+      <c r="G18" s="155"/>
+      <c r="H18" s="154">
         <f>H7+H9+H11+H13+H15+H17</f>
         <v>153591999.99999997</v>
       </c>
-      <c r="I18" s="177"/>
-      <c r="J18" s="173">
+      <c r="I18" s="154"/>
+      <c r="J18" s="153">
         <f>J7+J9+J11+J13+J15+J17</f>
         <v>173567527.27272725</v>
       </c>
-      <c r="K18" s="174"/>
-      <c r="L18" s="177">
+      <c r="K18" s="155"/>
+      <c r="L18" s="154">
         <f>L7+L9+L11+L13+L15+L17</f>
         <v>196260904.29752061</v>
       </c>
-      <c r="M18" s="177"/>
-      <c r="N18" s="173">
+      <c r="M18" s="154"/>
+      <c r="N18" s="153">
         <f>N7+N9+N11+N13+N15+N17</f>
         <v>222054492.23365882</v>
       </c>
-      <c r="O18" s="174"/>
-      <c r="P18" s="100"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B19" s="100"/>
-      <c r="C19" s="100"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="100"/>
-      <c r="F19" s="100"/>
-      <c r="G19" s="100"/>
-      <c r="H19" s="100"/>
-      <c r="I19" s="100"/>
-      <c r="J19" s="100"/>
-      <c r="K19" s="100"/>
-      <c r="L19" s="100"/>
-      <c r="M19" s="100"/>
-      <c r="N19" s="100"/>
-      <c r="O19" s="100"/>
-      <c r="P19" s="100"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C20" s="100"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="100"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="100"/>
-      <c r="H20" s="100"/>
-      <c r="I20" s="100"/>
-      <c r="J20" s="100"/>
-      <c r="K20" s="100"/>
-      <c r="L20" s="100"/>
-      <c r="M20" s="100"/>
-      <c r="N20" s="100"/>
-      <c r="O20" s="100"/>
-      <c r="P20" s="100"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C21" s="188" t="s">
+      <c r="O18" s="155"/>
+      <c r="P18" s="87"/>
+    </row>
+    <row r="19" spans="2:16">
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
+      <c r="H19" s="87"/>
+      <c r="I19" s="87"/>
+      <c r="J19" s="87"/>
+      <c r="K19" s="87"/>
+      <c r="L19" s="87"/>
+      <c r="M19" s="87"/>
+      <c r="N19" s="87"/>
+      <c r="O19" s="87"/>
+      <c r="P19" s="87"/>
+    </row>
+    <row r="20" spans="2:16">
+      <c r="C20" s="87"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="87"/>
+      <c r="K20" s="87"/>
+      <c r="L20" s="87"/>
+      <c r="M20" s="87"/>
+      <c r="N20" s="87"/>
+      <c r="O20" s="87"/>
+      <c r="P20" s="87"/>
+    </row>
+    <row r="21" spans="2:16">
+      <c r="C21" s="142" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C22" s="188"/>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C23" s="147">
+    <row r="22" spans="2:16">
+      <c r="C22" s="142"/>
+    </row>
+    <row r="23" spans="2:16">
+      <c r="C23" s="116">
         <v>50000</v>
       </c>
     </row>
-    <row r="25" spans="2:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="C25" s="143" t="s">
+    <row r="25" spans="2:16" ht="24">
+      <c r="C25" s="112" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C26" s="144">
+    <row r="26" spans="2:16">
+      <c r="C26" s="113">
         <v>0.15</v>
       </c>
     </row>
-    <row r="28" spans="2:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="C28" s="145" t="s">
+    <row r="28" spans="2:16" ht="24">
+      <c r="C28" s="114" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C29" s="150">
+    <row r="29" spans="2:16">
+      <c r="C29" s="119">
         <f>(F6-D6)/F6</f>
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C30" s="149"/>
+    <row r="30" spans="2:16">
+      <c r="C30" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="L13:M13"/>
     <mergeCell ref="D17:E17"/>
@@ -3579,45 +3637,6 @@
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="J15:K15"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:K18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -3636,56 +3655,56 @@
   <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="100"/>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="G1" s="100"/>
-    </row>
-    <row r="2" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="G2" s="100"/>
-    </row>
-    <row r="3" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="100"/>
-      <c r="B3" s="127" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="87"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="G1" s="87"/>
+    </row>
+    <row r="2" spans="1:13" ht="13" thickBot="1">
+      <c r="A2" s="87"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="G2" s="87"/>
+    </row>
+    <row r="3" spans="1:13" ht="13" thickBot="1">
+      <c r="A3" s="87"/>
+      <c r="B3" s="109" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="126"/>
+      <c r="C3" s="108"/>
       <c r="D3" s="20" t="s">
         <v>39</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="129"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="100"/>
-      <c r="B4" s="195" t="s">
+      <c r="G3" s="111"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="87"/>
+      <c r="B4" s="170" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="196"/>
+      <c r="C4" s="171"/>
       <c r="D4" s="6">
         <v>600000</v>
       </c>
@@ -3693,14 +3712,14 @@
         <f>D4*12</f>
         <v>7200000</v>
       </c>
-      <c r="G4" s="100"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="100"/>
-      <c r="B5" s="193" t="s">
+      <c r="G4" s="87"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="87"/>
+      <c r="B5" s="165" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="194"/>
+      <c r="C5" s="166"/>
       <c r="D5" s="4">
         <f>IF('HW y SW'!C5=0,100000,0)</f>
         <v>0</v>
@@ -3709,32 +3728,32 @@
         <f>'HW y SW'!G4</f>
         <v>500000</v>
       </c>
-      <c r="G5" s="100"/>
-      <c r="H5" s="156">
+      <c r="G5" s="87"/>
+      <c r="H5" s="124">
         <v>1</v>
       </c>
-      <c r="I5" s="156">
+      <c r="I5" s="124">
         <v>2</v>
       </c>
-      <c r="J5" s="156">
+      <c r="J5" s="124">
         <v>3</v>
       </c>
-      <c r="K5" s="156">
+      <c r="K5" s="124">
         <v>4</v>
       </c>
-      <c r="L5" s="156">
+      <c r="L5" s="124">
         <v>5</v>
       </c>
-      <c r="M5" s="156">
+      <c r="M5" s="124">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="100"/>
-      <c r="B6" s="193" t="s">
+    <row r="6" spans="1:13">
+      <c r="A6" s="87"/>
+      <c r="B6" s="165" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="194"/>
+      <c r="C6" s="166"/>
       <c r="D6" s="4">
         <f>PERSONAL!E12</f>
         <v>8000000</v>
@@ -3743,40 +3762,40 @@
         <f t="shared" ref="E6:E11" si="0">D6*12</f>
         <v>96000000</v>
       </c>
-      <c r="G6" s="157" t="s">
+      <c r="G6" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="158">
+      <c r="H6" s="126">
         <f>E6</f>
         <v>96000000</v>
       </c>
-      <c r="I6" s="159">
+      <c r="I6" s="127">
         <f>H6*(1+$I$10)</f>
         <v>105600000.00000001</v>
       </c>
-      <c r="J6" s="159">
+      <c r="J6" s="127">
         <f t="shared" ref="J6:M6" si="1">I6*(1+$I$10)</f>
         <v>116160000.00000003</v>
       </c>
-      <c r="K6" s="159">
+      <c r="K6" s="127">
         <f t="shared" si="1"/>
         <v>127776000.00000004</v>
       </c>
-      <c r="L6" s="159">
+      <c r="L6" s="127">
         <f t="shared" si="1"/>
         <v>140553600.00000006</v>
       </c>
-      <c r="M6" s="159">
+      <c r="M6" s="127">
         <f t="shared" si="1"/>
         <v>154608960.00000009</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="100"/>
-      <c r="B7" s="193" t="s">
+    <row r="7" spans="1:13">
+      <c r="A7" s="87"/>
+      <c r="B7" s="165" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="194"/>
+      <c r="C7" s="166"/>
       <c r="D7" s="4">
         <v>100000</v>
       </c>
@@ -3784,78 +3803,78 @@
         <f t="shared" si="0"/>
         <v>1200000</v>
       </c>
-      <c r="G7" s="157" t="s">
+      <c r="G7" s="125" t="s">
         <v>130</v>
       </c>
-      <c r="H7" s="158">
+      <c r="H7" s="126">
         <f>SUM(E4:E13)-H6</f>
         <v>17378600</v>
       </c>
-      <c r="I7" s="159">
+      <c r="I7" s="127">
         <f>H7*(1+$I$11)</f>
         <v>18247530</v>
       </c>
-      <c r="J7" s="159">
+      <c r="J7" s="127">
         <f t="shared" ref="J7:M7" si="2">I7*(1+$I$11)</f>
         <v>19159906.5</v>
       </c>
-      <c r="K7" s="159">
+      <c r="K7" s="127">
         <f t="shared" si="2"/>
         <v>20117901.824999999</v>
       </c>
-      <c r="L7" s="159">
+      <c r="L7" s="127">
         <f t="shared" si="2"/>
         <v>21123796.916250002</v>
       </c>
-      <c r="M7" s="159">
+      <c r="M7" s="127">
         <f t="shared" si="2"/>
         <v>22179986.762062501</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="100"/>
-      <c r="B8" s="193" t="s">
+    <row r="8" spans="1:13">
+      <c r="A8" s="87"/>
+      <c r="B8" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="194"/>
+      <c r="C8" s="166"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4">
         <v>13000</v>
       </c>
-      <c r="G8" s="160" t="s">
+      <c r="G8" s="128" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="161">
+      <c r="H8" s="129">
         <f>H6+H7</f>
         <v>113378600</v>
       </c>
-      <c r="I8" s="162">
+      <c r="I8" s="130">
         <f t="shared" ref="I8:M8" si="3">SUM(I6:I7)</f>
         <v>123847530.00000001</v>
       </c>
-      <c r="J8" s="162">
+      <c r="J8" s="130">
         <f t="shared" si="3"/>
         <v>135319906.50000003</v>
       </c>
-      <c r="K8" s="162">
+      <c r="K8" s="130">
         <f t="shared" si="3"/>
         <v>147893901.82500005</v>
       </c>
-      <c r="L8" s="162">
+      <c r="L8" s="130">
         <f t="shared" si="3"/>
         <v>161677396.91625005</v>
       </c>
-      <c r="M8" s="162">
+      <c r="M8" s="130">
         <f t="shared" si="3"/>
         <v>176788946.76206258</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="100"/>
-      <c r="B9" s="193" t="s">
+    <row r="9" spans="1:13">
+      <c r="A9" s="87"/>
+      <c r="B9" s="165" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="194"/>
+      <c r="C9" s="166"/>
       <c r="D9" s="4">
         <v>50000</v>
       </c>
@@ -3863,14 +3882,14 @@
         <f t="shared" si="0"/>
         <v>600000</v>
       </c>
-      <c r="G9" s="100"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="100"/>
-      <c r="B10" s="193" t="s">
+      <c r="G9" s="87"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="87"/>
+      <c r="B10" s="165" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="194"/>
+      <c r="C10" s="166"/>
       <c r="D10" s="4">
         <v>45000</v>
       </c>
@@ -3878,20 +3897,20 @@
         <f t="shared" si="0"/>
         <v>540000</v>
       </c>
-      <c r="G10" s="192" t="s">
+      <c r="G10" s="169" t="s">
         <v>132</v>
       </c>
-      <c r="H10" s="192"/>
-      <c r="I10" s="163">
+      <c r="H10" s="169"/>
+      <c r="I10" s="131">
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="100"/>
-      <c r="B11" s="193" t="s">
+    <row r="11" spans="1:13">
+      <c r="A11" s="87"/>
+      <c r="B11" s="165" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="194"/>
+      <c r="C11" s="166"/>
       <c r="D11" s="4">
         <v>45000</v>
       </c>
@@ -3899,20 +3918,20 @@
         <f t="shared" si="0"/>
         <v>540000</v>
       </c>
-      <c r="G11" s="192" t="s">
+      <c r="G11" s="169" t="s">
         <v>133</v>
       </c>
-      <c r="H11" s="192"/>
-      <c r="I11" s="163">
+      <c r="H11" s="169"/>
+      <c r="I11" s="131">
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="100"/>
-      <c r="B12" s="193" t="s">
+    <row r="12" spans="1:13">
+      <c r="A12" s="87"/>
+      <c r="B12" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="194"/>
+      <c r="C12" s="166"/>
       <c r="D12" s="4">
         <f>'CREACIÓN CURSOS'!C9</f>
         <v>1100000</v>
@@ -3921,14 +3940,14 @@
         <f>'CREACIÓN CURSOS'!C14</f>
         <v>4400000</v>
       </c>
-      <c r="G12" s="100"/>
-    </row>
-    <row r="13" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="100"/>
-      <c r="B13" s="197" t="s">
+      <c r="G12" s="87"/>
+    </row>
+    <row r="13" spans="1:13" ht="13" thickBot="1">
+      <c r="A13" s="87"/>
+      <c r="B13" s="161" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="199"/>
+      <c r="C13" s="163"/>
       <c r="D13" s="5">
         <f>SUM(D4:D12)*0.02</f>
         <v>198800</v>
@@ -3937,92 +3956,92 @@
         <f>D13*12</f>
         <v>2385600</v>
       </c>
-      <c r="G13" s="100"/>
-    </row>
-    <row r="14" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="100"/>
-      <c r="B14" s="100"/>
-      <c r="C14" s="166" t="s">
+      <c r="G13" s="87"/>
+    </row>
+    <row r="14" spans="1:13" ht="13" thickBot="1">
+      <c r="A14" s="87"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="135" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="200"/>
+      <c r="D14" s="164"/>
       <c r="E14" s="11">
         <f>SUM(E4:E13)</f>
         <v>113378600</v>
       </c>
-      <c r="G14" s="100"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="100"/>
-      <c r="B15" s="100"/>
-      <c r="C15" s="100"/>
-      <c r="D15" s="128"/>
-      <c r="E15" s="128"/>
-      <c r="G15" s="100"/>
-    </row>
-    <row r="16" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="100"/>
-      <c r="B16" s="100"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="128"/>
-      <c r="E16" s="128"/>
-      <c r="G16" s="100"/>
-    </row>
-    <row r="17" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="100"/>
-      <c r="B17" s="201" t="s">
+      <c r="G14" s="87"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="87"/>
+      <c r="B15" s="87"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="110"/>
+      <c r="E15" s="110"/>
+      <c r="G15" s="87"/>
+    </row>
+    <row r="16" spans="1:13" ht="13" thickBot="1">
+      <c r="A16" s="87"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="110"/>
+      <c r="E16" s="110"/>
+      <c r="G16" s="87"/>
+    </row>
+    <row r="17" spans="1:7" ht="13" thickBot="1">
+      <c r="A17" s="87"/>
+      <c r="B17" s="167" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="202"/>
+      <c r="C17" s="168"/>
       <c r="D17" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="100"/>
-      <c r="G17" s="100"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="100"/>
+      <c r="E17" s="87"/>
+      <c r="G17" s="87"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="87"/>
       <c r="B18" s="24" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="25"/>
-      <c r="D18" s="98">
+      <c r="D18" s="85">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E18" s="100"/>
-      <c r="G18" s="100"/>
-    </row>
-    <row r="19" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="100"/>
-      <c r="B19" s="197" t="s">
+      <c r="E18" s="87"/>
+      <c r="G18" s="87"/>
+    </row>
+    <row r="19" spans="1:7" ht="13" thickBot="1">
+      <c r="A19" s="87"/>
+      <c r="B19" s="161" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="198"/>
-      <c r="D19" s="99">
+      <c r="C19" s="162"/>
+      <c r="D19" s="86">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E19" s="100"/>
-      <c r="G19" s="100"/>
-    </row>
-    <row r="20" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="100"/>
-      <c r="B20" s="100"/>
-      <c r="C20" s="100"/>
-      <c r="D20" s="125" t="s">
+      <c r="E19" s="87"/>
+      <c r="G19" s="87"/>
+    </row>
+    <row r="20" spans="1:7" ht="13" thickBot="1">
+      <c r="A20" s="87"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="100"/>
-      <c r="G20" s="100"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="100"/>
-      <c r="B21" s="100"/>
-      <c r="C21" s="100"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
-      <c r="G21" s="100"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E20" s="87"/>
+      <c r="G20" s="87"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="87"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="G21" s="87"/>
+    </row>
+    <row r="23" spans="1:7">
       <c r="D23">
         <f>E14*D19</f>
         <v>566893</v>
@@ -4030,12 +4049,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="B9:C9"/>
@@ -4045,10 +4058,15 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter alignWithMargins="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -4062,19 +4080,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:G9"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" ht="13" thickBot="1"/>
+    <row r="7" spans="2:7" ht="13" thickBot="1">
       <c r="B7" s="47"/>
       <c r="C7" s="74" t="s">
         <v>29</v>
@@ -4092,8 +4110,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="206" t="s">
+    <row r="8" spans="2:7" ht="13" thickBot="1">
+      <c r="B8" s="133" t="s">
         <v>66</v>
       </c>
       <c r="C8" s="48">
@@ -4112,7 +4130,7 @@
         <v>526666.66666666663</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" ht="13" thickBot="1">
       <c r="F9" s="75" t="s">
         <v>20</v>
       </c>
@@ -4137,20 +4155,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F19"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6">
       <c r="B4" s="1" t="s">
         <v>77</v>
       </c>
@@ -4158,7 +4176,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6">
       <c r="B5" s="56" t="s">
         <v>76</v>
       </c>
@@ -4167,13 +4185,13 @@
         <v>12366000</v>
       </c>
       <c r="D5" s="51"/>
-      <c r="E5" s="148">
+      <c r="E5" s="117">
         <f>PMT(C6,B17,C5)</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="F5" s="148"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F5" s="117"/>
+    </row>
+    <row r="6" spans="2:6">
       <c r="B6" s="62" t="s">
         <v>78</v>
       </c>
@@ -4184,7 +4202,7 @@
       <c r="E6" s="51"/>
       <c r="F6" s="51"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6">
       <c r="B7" s="62" t="s">
         <v>79</v>
       </c>
@@ -4195,21 +4213,21 @@
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:6">
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
       <c r="D8" s="57"/>
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:6">
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
       <c r="D9" s="57"/>
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
     </row>
-    <row r="10" spans="2:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="17.25" customHeight="1" thickBot="1">
       <c r="B10" s="58" t="s">
         <v>68</v>
       </c>
@@ -4226,24 +4244,24 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="89" t="s">
+    <row r="11" spans="2:6" ht="13" thickBot="1">
+      <c r="B11" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="90" t="s">
+      <c r="C11" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="91" t="s">
+      <c r="D11" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="92" t="s">
+      <c r="E11" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="93" t="s">
+      <c r="F11" s="80" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6">
       <c r="B12" s="60">
         <v>1</v>
       </c>
@@ -4264,7 +4282,7 @@
         <v>3297600</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:6">
       <c r="B13" s="53">
         <v>2</v>
       </c>
@@ -4285,7 +4303,7 @@
         <v>3091500</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:6">
       <c r="B14" s="53">
         <v>3</v>
       </c>
@@ -4306,7 +4324,7 @@
         <v>2885400</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:6">
       <c r="B15" s="53">
         <v>4</v>
       </c>
@@ -4327,7 +4345,7 @@
         <v>2679300</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6">
       <c r="B16" s="53">
         <v>5</v>
       </c>
@@ -4348,7 +4366,7 @@
         <v>2473200</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="13" thickBot="1">
       <c r="B17" s="54">
         <v>6</v>
       </c>
@@ -4369,11 +4387,11 @@
         <v>2267100</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6">
       <c r="C18" s="52"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="205"/>
+    <row r="19" spans="2:6">
+      <c r="C19" s="132"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4392,36 +4410,36 @@
   <sheetPr codeName="Hoja3" enableFormatConditionsCalculation="0"/>
   <dimension ref="B3:G16"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="13" thickBot="1">
       <c r="G3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" ht="13" thickBot="1">
       <c r="B4" s="22" t="s">
         <v>3</v>
       </c>
       <c r="F4" t="s">
         <v>116</v>
       </c>
-      <c r="G4" s="151">
+      <c r="G4" s="120">
         <v>500000</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="13" thickBot="1">
       <c r="B5" s="38" t="s">
         <v>13</v>
       </c>
@@ -4429,7 +4447,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" ht="13" thickBot="1">
       <c r="B6" s="36" t="s">
         <v>20</v>
       </c>
@@ -4438,28 +4456,28 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7">
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7">
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7">
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7">
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" ht="13" thickBot="1">
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" ht="13" thickBot="1">
       <c r="B12" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7">
       <c r="B13" s="30" t="s">
         <v>14</v>
       </c>
@@ -4467,7 +4485,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7">
       <c r="B14" s="32" t="s">
         <v>15</v>
       </c>
@@ -4475,7 +4493,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" ht="13" thickBot="1">
       <c r="B15" s="32" t="s">
         <v>102</v>
       </c>
@@ -4483,7 +4501,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" ht="13" thickBot="1">
       <c r="B16" s="34" t="s">
         <v>20</v>
       </c>
@@ -4509,17 +4527,17 @@
   <sheetPr codeName="Hoja4" enableFormatConditionsCalculation="0"/>
   <dimension ref="B1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="13" thickBot="1">
       <c r="F1">
         <v>2</v>
       </c>
@@ -4536,13 +4554,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="201" t="s">
+    <row r="2" spans="2:10" ht="13" thickBot="1">
+      <c r="D2" s="167" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="203"/>
-    </row>
-    <row r="3" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="172"/>
+    </row>
+    <row r="3" spans="2:10" ht="13" thickBot="1">
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
@@ -4556,22 +4574,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="95">
+    <row r="4" spans="2:10">
+      <c r="B4" s="82">
         <v>1</v>
       </c>
-      <c r="C4" s="96" t="s">
+      <c r="C4" s="83" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="44">
         <v>1500000</v>
       </c>
-      <c r="E4" s="97">
+      <c r="E4" s="84">
         <f t="shared" ref="E4:E11" si="0">B4*D4</f>
         <v>1500000</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10">
       <c r="B5" s="12">
         <v>1</v>
       </c>
@@ -4586,7 +4604,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10">
       <c r="B6" s="12">
         <v>2</v>
       </c>
@@ -4601,7 +4619,7 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10">
       <c r="B7" s="12">
         <v>3</v>
       </c>
@@ -4616,7 +4634,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10">
       <c r="B8" s="12">
         <v>1</v>
       </c>
@@ -4631,7 +4649,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10">
       <c r="B9" s="12">
         <v>1</v>
       </c>
@@ -4646,7 +4664,7 @@
         <v>850000</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10">
       <c r="B10" s="12">
         <v>1</v>
       </c>
@@ -4661,7 +4679,7 @@
         <v>850000</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="13" thickBot="1">
       <c r="B11" s="16">
         <v>1</v>
       </c>
@@ -4676,8 +4694,8 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="94">
+    <row r="12" spans="2:10" ht="13" thickBot="1">
+      <c r="E12" s="81">
         <f>SUM(E4:E11)</f>
         <v>8000000</v>
       </c>
@@ -4722,24 +4740,24 @@
   <sheetPr codeName="Hoja5" enableFormatConditionsCalculation="0"/>
   <dimension ref="B3:I14"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="F21" sqref="F21:F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="9" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="204" t="s">
+    <row r="3" spans="2:9" ht="13" thickBot="1"/>
+    <row r="4" spans="2:9" ht="13" thickBot="1">
+      <c r="B4" s="173" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="200"/>
-    </row>
-    <row r="5" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="164"/>
+    </row>
+    <row r="5" spans="2:9" ht="13" thickBot="1">
       <c r="B5" s="26" t="s">
         <v>32</v>
       </c>
@@ -4747,7 +4765,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9">
       <c r="B6" s="21" t="s">
         <v>31</v>
       </c>
@@ -4755,7 +4773,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9">
       <c r="B7" s="7" t="s">
         <v>123</v>
       </c>
@@ -4766,15 +4784,15 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="111" t="s">
+    <row r="8" spans="2:9" ht="13" thickBot="1">
+      <c r="B8" s="93" t="s">
         <v>103</v>
       </c>
       <c r="C8" s="5">
         <v>500000</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="13" thickBot="1">
       <c r="B9" s="27" t="s">
         <v>20</v>
       </c>
@@ -4783,32 +4801,32 @@
         <v>1100000</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="114" t="s">
+    <row r="11" spans="2:9" ht="13" thickBot="1"/>
+    <row r="12" spans="2:9" ht="13" thickBot="1">
+      <c r="C12" s="96" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="120" t="s">
+      <c r="D12" s="102" t="s">
         <v>93</v>
       </c>
-      <c r="E12" s="118" t="s">
+      <c r="E12" s="100" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="120" t="s">
+      <c r="F12" s="102" t="s">
         <v>97</v>
       </c>
-      <c r="G12" s="118" t="s">
+      <c r="G12" s="100" t="s">
         <v>98</v>
       </c>
-      <c r="H12" s="120" t="s">
+      <c r="H12" s="102" t="s">
         <v>99</v>
       </c>
-      <c r="I12" s="119" t="s">
+      <c r="I12" s="101" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="114" t="s">
+    <row r="13" spans="2:9">
+      <c r="B13" s="96" t="s">
         <v>105</v>
       </c>
       <c r="C13" s="30">
@@ -4817,51 +4835,51 @@
       <c r="D13" s="21">
         <v>4</v>
       </c>
-      <c r="E13" s="115">
+      <c r="E13" s="97">
         <v>4</v>
       </c>
       <c r="F13" s="21">
         <v>4</v>
       </c>
-      <c r="G13" s="115">
+      <c r="G13" s="97">
         <v>4</v>
       </c>
       <c r="H13" s="21">
         <v>4</v>
       </c>
-      <c r="I13" s="116">
+      <c r="I13" s="98">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="117" t="s">
+    <row r="14" spans="2:9" ht="13" thickBot="1">
+      <c r="B14" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="121">
+      <c r="C14" s="103">
         <f>$C$9*C13</f>
         <v>4400000</v>
       </c>
-      <c r="D14" s="122">
+      <c r="D14" s="104">
         <f t="shared" ref="D14:I14" si="0">$C$9*D13</f>
         <v>4400000</v>
       </c>
-      <c r="E14" s="123">
+      <c r="E14" s="105">
         <f t="shared" si="0"/>
         <v>4400000</v>
       </c>
-      <c r="F14" s="122">
+      <c r="F14" s="104">
         <f t="shared" si="0"/>
         <v>4400000</v>
       </c>
-      <c r="G14" s="123">
+      <c r="G14" s="105">
         <f t="shared" si="0"/>
         <v>4400000</v>
       </c>
-      <c r="H14" s="122">
+      <c r="H14" s="104">
         <f t="shared" si="0"/>
         <v>4400000</v>
       </c>
-      <c r="I14" s="124">
+      <c r="I14" s="106">
         <f t="shared" si="0"/>
         <v>4400000</v>
       </c>

</xml_diff>

<commit_message>
+ Cambios de Formato
</commit_message>
<xml_diff>
--- a/FLUJO PESIMISTA.xlsx
+++ b/FLUJO PESIMISTA.xlsx
@@ -446,7 +446,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -1019,10 +1019,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1275,126 +1283,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1404,31 +1292,25 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="12" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="12" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="12" fillId="10" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="12" fillId="10" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="12" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="12" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="12" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="12" fillId="9" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1439,27 +1321,153 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="12" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="12" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="35">
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
@@ -1472,6 +1480,10 @@
     <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
@@ -1484,6 +1496,10 @@
     <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentual" xfId="1" builtinId="5"/>
@@ -1866,7 +1882,7 @@
   <dimension ref="B1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B22" sqref="B22:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1878,582 +1894,582 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="17">
-      <c r="B1" s="134" t="s">
+      <c r="B1" s="159" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="159"/>
+      <c r="G1" s="159"/>
+      <c r="H1" s="159"/>
+      <c r="I1" s="159"/>
+      <c r="J1" s="159"/>
     </row>
     <row r="4" spans="2:10" ht="14" thickBot="1">
-      <c r="B4" s="187"/>
-      <c r="C4" s="188" t="s">
+      <c r="B4" s="145"/>
+      <c r="C4" s="146" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="189"/>
-      <c r="E4" s="187"/>
-      <c r="F4" s="187"/>
-      <c r="G4" s="187"/>
-      <c r="H4" s="187"/>
-      <c r="I4" s="187"/>
-      <c r="J4" s="187"/>
+      <c r="D4" s="147"/>
+      <c r="E4" s="145"/>
+      <c r="F4" s="145"/>
+      <c r="G4" s="145"/>
+      <c r="H4" s="145"/>
+      <c r="I4" s="145"/>
+      <c r="J4" s="145"/>
     </row>
     <row r="5" spans="2:10" ht="16" thickBot="1">
-      <c r="B5" s="174" t="s">
+      <c r="B5" s="134" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="174" t="s">
+      <c r="C5" s="134" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="175">
+      <c r="D5" s="135">
         <v>0</v>
       </c>
-      <c r="E5" s="175">
+      <c r="E5" s="135">
         <v>1</v>
       </c>
-      <c r="F5" s="175">
+      <c r="F5" s="135">
         <v>2</v>
       </c>
-      <c r="G5" s="175">
+      <c r="G5" s="135">
         <v>3</v>
       </c>
-      <c r="H5" s="175">
+      <c r="H5" s="135">
         <v>4</v>
       </c>
-      <c r="I5" s="175">
+      <c r="I5" s="135">
         <v>5</v>
       </c>
-      <c r="J5" s="175">
+      <c r="J5" s="135">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="13" thickBot="1">
-      <c r="B6" s="176" t="s">
+      <c r="B6" s="136" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="176" t="s">
+      <c r="C6" s="136" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="190"/>
-      <c r="E6" s="177">
+      <c r="D6" s="148"/>
+      <c r="E6" s="137">
         <f>INGRESOS!D18</f>
         <v>109500000</v>
       </c>
-      <c r="F6" s="177">
+      <c r="F6" s="137">
         <f>INGRESOS!F18</f>
         <v>135999999.99999997</v>
       </c>
-      <c r="G6" s="177">
+      <c r="G6" s="137">
         <f>INGRESOS!H18</f>
         <v>153591999.99999997</v>
       </c>
-      <c r="H6" s="177">
+      <c r="H6" s="137">
         <f>INGRESOS!J18</f>
         <v>173567527.27272725</v>
       </c>
-      <c r="I6" s="177">
+      <c r="I6" s="137">
         <f>INGRESOS!L18</f>
         <v>196260904.29752061</v>
       </c>
-      <c r="J6" s="177">
+      <c r="J6" s="137">
         <f>INGRESOS!N18</f>
         <v>222054492.23365882</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="13" thickBot="1">
-      <c r="B7" s="176" t="s">
+      <c r="B7" s="136" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="176" t="s">
+      <c r="C7" s="136" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="191"/>
-      <c r="E7" s="177">
+      <c r="D7" s="149"/>
+      <c r="E7" s="137">
         <v>5000000</v>
       </c>
-      <c r="F7" s="177">
+      <c r="F7" s="137">
         <f>E7*1.3</f>
         <v>6500000</v>
       </c>
-      <c r="G7" s="177">
+      <c r="G7" s="137">
         <f>F7*1.3</f>
         <v>8450000</v>
       </c>
-      <c r="H7" s="177">
+      <c r="H7" s="137">
         <f>G7*1.3</f>
         <v>10985000</v>
       </c>
-      <c r="I7" s="177">
+      <c r="I7" s="137">
         <f>H7*1.3</f>
         <v>14280500</v>
       </c>
-      <c r="J7" s="177">
+      <c r="J7" s="137">
         <f>I7*1.3</f>
         <v>18564650</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="13" thickBot="1">
-      <c r="B8" s="176" t="s">
+      <c r="B8" s="136" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="176" t="s">
+      <c r="C8" s="136" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="191"/>
-      <c r="E8" s="177">
+      <c r="D8" s="149"/>
+      <c r="E8" s="137">
         <f>-'CREACIÓN CURSOS'!D14</f>
         <v>-4400000</v>
       </c>
-      <c r="F8" s="177">
+      <c r="F8" s="137">
         <f>-'CREACIÓN CURSOS'!E14</f>
         <v>-4400000</v>
       </c>
-      <c r="G8" s="177">
+      <c r="G8" s="137">
         <f>-'CREACIÓN CURSOS'!F14</f>
         <v>-4400000</v>
       </c>
-      <c r="H8" s="177">
+      <c r="H8" s="137">
         <f>-'CREACIÓN CURSOS'!G14</f>
         <v>-4400000</v>
       </c>
-      <c r="I8" s="177">
+      <c r="I8" s="137">
         <f>-'CREACIÓN CURSOS'!H14</f>
         <v>-4400000</v>
       </c>
-      <c r="J8" s="177">
+      <c r="J8" s="137">
         <f>-'CREACIÓN CURSOS'!I14</f>
         <v>-4400000</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="13" thickBot="1">
-      <c r="B9" s="176" t="s">
+      <c r="B9" s="136" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="176" t="s">
+      <c r="C9" s="136" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="191"/>
-      <c r="E9" s="177">
+      <c r="D9" s="149"/>
+      <c r="E9" s="137">
         <f>-INGRESOS!D18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-8212500.0000000009</v>
       </c>
-      <c r="F9" s="177">
+      <c r="F9" s="137">
         <f>-INGRESOS!F18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-10200000</v>
       </c>
-      <c r="G9" s="177">
+      <c r="G9" s="137">
         <f>-INGRESOS!H18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-11519400</v>
       </c>
-      <c r="H9" s="177">
+      <c r="H9" s="137">
         <f>-INGRESOS!J18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-13017564.545454545</v>
       </c>
-      <c r="I9" s="177">
+      <c r="I9" s="137">
         <f>-INGRESOS!L18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-14719567.822314048</v>
       </c>
-      <c r="J9" s="177">
+      <c r="J9" s="137">
         <f>-INGRESOS!N18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-16654086.917524414</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="13" thickBot="1">
-      <c r="B10" s="176" t="s">
+      <c r="B10" s="136" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="176" t="s">
+      <c r="C10" s="136" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="191"/>
-      <c r="E10" s="177">
+      <c r="D10" s="149"/>
+      <c r="E10" s="137">
         <f>-'ESTRUCTURA DE COSTOS'!H8</f>
         <v>-113378600</v>
       </c>
-      <c r="F10" s="177">
+      <c r="F10" s="137">
         <f>-'ESTRUCTURA DE COSTOS'!I8</f>
         <v>-123847530.00000001</v>
       </c>
-      <c r="G10" s="177">
+      <c r="G10" s="137">
         <f>-'ESTRUCTURA DE COSTOS'!J8</f>
         <v>-135319906.50000003</v>
       </c>
-      <c r="H10" s="177">
+      <c r="H10" s="137">
         <f>-'ESTRUCTURA DE COSTOS'!K8</f>
         <v>-147893901.82500005</v>
       </c>
-      <c r="I10" s="177">
+      <c r="I10" s="137">
         <f>-'ESTRUCTURA DE COSTOS'!L8</f>
         <v>-161677396.91625005</v>
       </c>
-      <c r="J10" s="177">
+      <c r="J10" s="137">
         <f>-'ESTRUCTURA DE COSTOS'!M8</f>
         <v>-176788946.76206258</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="13" thickBot="1">
-      <c r="B11" s="176" t="s">
+      <c r="B11" s="136" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="176" t="s">
+      <c r="C11" s="136" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="191"/>
-      <c r="E11" s="177">
+      <c r="D11" s="149"/>
+      <c r="E11" s="137">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="F11" s="177">
+      <c r="F11" s="137">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="G11" s="177">
+      <c r="G11" s="137">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="H11" s="177">
+      <c r="H11" s="137">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="I11" s="177">
+      <c r="I11" s="137">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="J11" s="177">
+      <c r="J11" s="137">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="13" thickBot="1">
-      <c r="B12" s="178" t="s">
+      <c r="B12" s="138" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="178" t="s">
+      <c r="C12" s="138" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="192"/>
-      <c r="E12" s="179">
+      <c r="D12" s="150"/>
+      <c r="E12" s="139">
         <f t="shared" ref="E12:J12" si="0">SUM(E6:E11)</f>
         <v>-12017766.666666666</v>
       </c>
-      <c r="F12" s="179">
+      <c r="F12" s="139">
         <f t="shared" si="0"/>
         <v>3525803.3333332888</v>
       </c>
-      <c r="G12" s="179">
+      <c r="G12" s="139">
         <f t="shared" si="0"/>
         <v>10276026.833333274</v>
       </c>
-      <c r="H12" s="179">
+      <c r="H12" s="139">
         <f t="shared" si="0"/>
         <v>18714394.235606004</v>
       </c>
-      <c r="I12" s="179">
+      <c r="I12" s="139">
         <f t="shared" si="0"/>
         <v>29217772.892289836</v>
       </c>
-      <c r="J12" s="179">
+      <c r="J12" s="139">
         <f t="shared" si="0"/>
         <v>42249441.88740515</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="13" thickBot="1">
-      <c r="B13" s="176" t="s">
+      <c r="B13" s="136" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="176" t="s">
+      <c r="C13" s="136" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="191"/>
-      <c r="E13" s="177">
+      <c r="D13" s="149"/>
+      <c r="E13" s="137">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="F13" s="177">
+      <c r="F13" s="137">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="G13" s="177">
+      <c r="G13" s="137">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="H13" s="177">
+      <c r="H13" s="137">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="I13" s="177">
+      <c r="I13" s="137">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="J13" s="177">
+      <c r="J13" s="137">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="13" thickBot="1">
-      <c r="B14" s="178" t="s">
+      <c r="B14" s="138" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="178" t="s">
+      <c r="C14" s="138" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="192"/>
-      <c r="E14" s="179">
+      <c r="D14" s="150"/>
+      <c r="E14" s="139">
         <f t="shared" ref="E14:J14" si="1">SUM(E12:E13)</f>
         <v>-14857091.532231411</v>
       </c>
-      <c r="F14" s="179">
+      <c r="F14" s="139">
         <f t="shared" si="1"/>
         <v>686478.4677685434</v>
       </c>
-      <c r="G14" s="179">
+      <c r="G14" s="139">
         <f t="shared" si="1"/>
         <v>7436701.9677685294</v>
       </c>
-      <c r="H14" s="179">
+      <c r="H14" s="139">
         <f t="shared" si="1"/>
         <v>15875069.370041259</v>
       </c>
-      <c r="I14" s="179">
+      <c r="I14" s="139">
         <f t="shared" si="1"/>
         <v>26378448.026725091</v>
       </c>
-      <c r="J14" s="179">
+      <c r="J14" s="139">
         <f t="shared" si="1"/>
         <v>39410117.021840401</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="13" thickBot="1">
-      <c r="B15" s="176" t="s">
+      <c r="B15" s="136" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="176" t="s">
+      <c r="C15" s="136" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="191"/>
-      <c r="E15" s="177">
+      <c r="D15" s="149"/>
+      <c r="E15" s="137">
         <f t="shared" ref="E15:J15" si="2">+IF(E14&gt;0,-(E14*0.17),0)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="177">
+      <c r="F15" s="137">
         <f t="shared" si="2"/>
         <v>-116701.33952065239</v>
       </c>
-      <c r="G15" s="177">
+      <c r="G15" s="137">
         <f t="shared" si="2"/>
         <v>-1264239.3345206501</v>
       </c>
-      <c r="H15" s="177">
+      <c r="H15" s="137">
         <f t="shared" si="2"/>
         <v>-2698761.792907014</v>
       </c>
-      <c r="I15" s="177">
+      <c r="I15" s="137">
         <f t="shared" si="2"/>
         <v>-4484336.1645432655</v>
       </c>
-      <c r="J15" s="177">
+      <c r="J15" s="137">
         <f t="shared" si="2"/>
         <v>-6699719.8937128689</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="13" thickBot="1">
-      <c r="B16" s="176" t="s">
+      <c r="B16" s="136" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="176" t="s">
+      <c r="C16" s="136" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="191"/>
-      <c r="E16" s="177">
+      <c r="D16" s="149"/>
+      <c r="E16" s="137">
         <f t="shared" ref="E16:J16" si="3">-(E11)</f>
         <v>526666.66666666663</v>
       </c>
-      <c r="F16" s="177">
+      <c r="F16" s="137">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
-      <c r="G16" s="177">
+      <c r="G16" s="137">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
-      <c r="H16" s="177">
+      <c r="H16" s="137">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
-      <c r="I16" s="177">
+      <c r="I16" s="137">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
-      <c r="J16" s="177">
+      <c r="J16" s="137">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="13" thickBot="1">
-      <c r="B17" s="176" t="s">
+      <c r="B17" s="136" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="176" t="s">
+      <c r="C17" s="136" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="191"/>
-      <c r="E17" s="177">
+      <c r="D17" s="149"/>
+      <c r="E17" s="137">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="F17" s="177">
+      <c r="F17" s="137">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="G17" s="177">
+      <c r="G17" s="137">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="H17" s="177">
+      <c r="H17" s="137">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="I17" s="177">
+      <c r="I17" s="137">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="J17" s="177">
+      <c r="J17" s="137">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="13" thickBot="1">
-      <c r="B18" s="176" t="s">
+      <c r="B18" s="136" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="176" t="s">
+      <c r="C18" s="136" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="193">
+      <c r="D18" s="151">
         <f>-INVERSION!D20</f>
         <v>-20610000</v>
       </c>
-      <c r="E18" s="177"/>
-      <c r="F18" s="177"/>
-      <c r="G18" s="177"/>
-      <c r="H18" s="177"/>
-      <c r="I18" s="177"/>
-      <c r="J18" s="177"/>
+      <c r="E18" s="137"/>
+      <c r="F18" s="137"/>
+      <c r="G18" s="137"/>
+      <c r="H18" s="137"/>
+      <c r="I18" s="137"/>
+      <c r="J18" s="137"/>
     </row>
     <row r="19" spans="2:10" ht="13" thickBot="1">
-      <c r="B19" s="176"/>
-      <c r="C19" s="176" t="s">
+      <c r="B19" s="136"/>
+      <c r="C19" s="136" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="194">
+      <c r="D19" s="152">
         <f>'G. FINANCIERO'!C5</f>
         <v>12366000</v>
       </c>
-      <c r="E19" s="177"/>
-      <c r="F19" s="177"/>
-      <c r="G19" s="177"/>
-      <c r="H19" s="177"/>
-      <c r="I19" s="177"/>
-      <c r="J19" s="177"/>
+      <c r="E19" s="137"/>
+      <c r="F19" s="137"/>
+      <c r="G19" s="137"/>
+      <c r="H19" s="137"/>
+      <c r="I19" s="137"/>
+      <c r="J19" s="137"/>
     </row>
     <row r="20" spans="2:10" ht="13" thickBot="1">
-      <c r="B20" s="180" t="s">
+      <c r="B20" s="140" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="180" t="s">
+      <c r="C20" s="140" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="181">
+      <c r="D20" s="141">
         <f>SUM(D18:D19)</f>
         <v>-8244000</v>
       </c>
-      <c r="E20" s="182">
+      <c r="E20" s="142">
         <f t="shared" ref="E20:J20" si="4">SUM(E14:E19)</f>
         <v>-16391424.865564745</v>
       </c>
-      <c r="F20" s="182">
+      <c r="F20" s="142">
         <f t="shared" si="4"/>
         <v>-964556.2050854424</v>
       </c>
-      <c r="G20" s="182">
+      <c r="G20" s="142">
         <f t="shared" si="4"/>
         <v>4638129.2999145463</v>
       </c>
-      <c r="H20" s="182">
+      <c r="H20" s="142">
         <f t="shared" si="4"/>
         <v>11641974.24380091</v>
       </c>
-      <c r="I20" s="182">
+      <c r="I20" s="142">
         <f t="shared" si="4"/>
         <v>20359778.528848495</v>
       </c>
-      <c r="J20" s="182">
+      <c r="J20" s="142">
         <f t="shared" si="4"/>
         <v>31176063.794794198</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="13" thickBot="1">
-      <c r="B21" s="195"/>
-      <c r="C21" s="195"/>
-      <c r="D21" s="196"/>
-      <c r="E21" s="196"/>
-      <c r="F21" s="196"/>
-      <c r="G21" s="196"/>
-      <c r="H21" s="196"/>
-      <c r="I21" s="196"/>
-      <c r="J21" s="196"/>
+      <c r="B21" s="153"/>
+      <c r="C21" s="153"/>
+      <c r="D21" s="154"/>
+      <c r="E21" s="154"/>
+      <c r="F21" s="154"/>
+      <c r="G21" s="154"/>
+      <c r="H21" s="154"/>
+      <c r="I21" s="154"/>
+      <c r="J21" s="154"/>
     </row>
     <row r="22" spans="2:10" ht="16" thickBot="1">
-      <c r="B22" s="183" t="s">
+      <c r="B22" s="157" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="184"/>
-      <c r="D22" s="185">
+      <c r="C22" s="158"/>
+      <c r="D22" s="143">
         <f>NPV(D24,E20:J20)+D20</f>
         <v>10079906.799768489</v>
       </c>
-      <c r="E22" s="196"/>
-      <c r="F22" s="197"/>
-      <c r="G22" s="196"/>
-      <c r="H22" s="196"/>
-      <c r="I22" s="196"/>
-      <c r="J22" s="196"/>
+      <c r="E22" s="154"/>
+      <c r="F22" s="155"/>
+      <c r="G22" s="154"/>
+      <c r="H22" s="154"/>
+      <c r="I22" s="154"/>
+      <c r="J22" s="154"/>
     </row>
     <row r="23" spans="2:10" ht="16" thickBot="1">
-      <c r="B23" s="183" t="s">
+      <c r="B23" s="157" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="184"/>
-      <c r="D23" s="186">
+      <c r="C23" s="158"/>
+      <c r="D23" s="144">
         <f>IRR(D20:J20)</f>
         <v>0.25017156683584729</v>
       </c>
-      <c r="E23" s="195"/>
-      <c r="F23" s="198"/>
-      <c r="G23" s="195"/>
-      <c r="H23" s="195"/>
-      <c r="I23" s="195"/>
-      <c r="J23" s="195"/>
+      <c r="E23" s="153"/>
+      <c r="F23" s="156"/>
+      <c r="G23" s="153"/>
+      <c r="H23" s="153"/>
+      <c r="I23" s="153"/>
+      <c r="J23" s="153"/>
     </row>
     <row r="24" spans="2:10" ht="16" thickBot="1">
-      <c r="B24" s="183" t="s">
+      <c r="B24" s="157" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="183"/>
-      <c r="D24" s="186">
+      <c r="C24" s="157"/>
+      <c r="D24" s="144">
         <v>0.15</v>
       </c>
-      <c r="E24" s="195"/>
-      <c r="F24" s="195"/>
-      <c r="G24" s="195"/>
-      <c r="H24" s="195"/>
-      <c r="I24" s="195"/>
-      <c r="J24" s="195"/>
+      <c r="E24" s="153"/>
+      <c r="F24" s="153"/>
+      <c r="G24" s="153"/>
+      <c r="H24" s="153"/>
+      <c r="I24" s="153"/>
+      <c r="J24" s="153"/>
     </row>
     <row r="27" spans="2:10">
       <c r="C27" s="121"/>
@@ -2671,19 +2687,19 @@
   <sheetData>
     <row r="3" spans="2:4" ht="13" thickBot="1"/>
     <row r="4" spans="2:4" ht="13" thickBot="1">
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="140"/>
+      <c r="C4" s="165"/>
       <c r="D4" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="13" thickBot="1">
-      <c r="B5" s="137" t="s">
+      <c r="B5" s="162" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="138"/>
+      <c r="C5" s="163"/>
       <c r="D5" s="44"/>
     </row>
     <row r="6" spans="2:4">
@@ -2701,28 +2717,28 @@
       <c r="D7" s="18"/>
     </row>
     <row r="8" spans="2:4" ht="13" thickBot="1">
-      <c r="B8" s="137" t="s">
+      <c r="B8" s="162" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="141"/>
+      <c r="C8" s="166"/>
       <c r="D8" s="45">
         <v>5000000</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="13" thickBot="1">
-      <c r="B9" s="137" t="s">
+      <c r="B9" s="162" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="138"/>
+      <c r="C9" s="163"/>
       <c r="D9" s="45">
         <v>2500000</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="13" thickBot="1">
-      <c r="B10" s="137" t="s">
+      <c r="B10" s="162" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="138"/>
+      <c r="C10" s="163"/>
       <c r="D10" s="44"/>
     </row>
     <row r="11" spans="2:4">
@@ -2760,10 +2776,10 @@
       </c>
     </row>
     <row r="14" spans="2:4" ht="13" thickBot="1">
-      <c r="B14" s="137" t="s">
+      <c r="B14" s="162" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="138"/>
+      <c r="C14" s="163"/>
       <c r="D14" s="44"/>
     </row>
     <row r="15" spans="2:4">
@@ -2813,10 +2829,10 @@
       </c>
     </row>
     <row r="20" spans="2:4" ht="13" thickBot="1">
-      <c r="B20" s="135" t="s">
+      <c r="B20" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="136"/>
+      <c r="C20" s="161"/>
       <c r="D20" s="46">
         <f>SUM(D5:D19)</f>
         <v>20610000</v>
@@ -2907,30 +2923,30 @@
     <row r="4" spans="2:16" ht="13" thickBot="1">
       <c r="B4" s="87"/>
       <c r="C4" s="87"/>
-      <c r="D4" s="156" t="s">
+      <c r="D4" s="179" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="158"/>
-      <c r="F4" s="156" t="s">
+      <c r="E4" s="181"/>
+      <c r="F4" s="179" t="s">
         <v>96</v>
       </c>
-      <c r="G4" s="157"/>
-      <c r="H4" s="158" t="s">
+      <c r="G4" s="180"/>
+      <c r="H4" s="181" t="s">
         <v>97</v>
       </c>
-      <c r="I4" s="158"/>
-      <c r="J4" s="156" t="s">
+      <c r="I4" s="181"/>
+      <c r="J4" s="179" t="s">
         <v>98</v>
       </c>
-      <c r="K4" s="157"/>
-      <c r="L4" s="158" t="s">
+      <c r="K4" s="180"/>
+      <c r="L4" s="181" t="s">
         <v>99</v>
       </c>
-      <c r="M4" s="158"/>
-      <c r="N4" s="156" t="s">
+      <c r="M4" s="181"/>
+      <c r="N4" s="179" t="s">
         <v>100</v>
       </c>
-      <c r="O4" s="157"/>
+      <c r="O4" s="180"/>
       <c r="P4" s="87"/>
     </row>
     <row r="5" spans="2:16" ht="13" thickBot="1">
@@ -2976,7 +2992,7 @@
     </row>
     <row r="6" spans="2:16" ht="13" thickBot="1">
       <c r="B6" s="87"/>
-      <c r="C6" s="146" t="s">
+      <c r="C6" s="183" t="s">
         <v>89</v>
       </c>
       <c r="D6" s="115">
@@ -3025,42 +3041,42 @@
     </row>
     <row r="7" spans="2:16" ht="13" thickBot="1">
       <c r="B7" s="87"/>
-      <c r="C7" s="147"/>
-      <c r="D7" s="149">
+      <c r="C7" s="184"/>
+      <c r="D7" s="173">
         <f>D6*E6</f>
         <v>43200000</v>
       </c>
-      <c r="E7" s="150"/>
-      <c r="F7" s="149">
+      <c r="E7" s="178"/>
+      <c r="F7" s="173">
         <f>F6*G6</f>
         <v>47520000</v>
       </c>
-      <c r="G7" s="151"/>
-      <c r="H7" s="150">
+      <c r="G7" s="174"/>
+      <c r="H7" s="178">
         <f>H6*I6</f>
         <v>51840000</v>
       </c>
-      <c r="I7" s="150"/>
-      <c r="J7" s="149">
+      <c r="I7" s="178"/>
+      <c r="J7" s="173">
         <f>J6*K6</f>
         <v>56552727.272727266</v>
       </c>
-      <c r="K7" s="151"/>
-      <c r="L7" s="150">
+      <c r="K7" s="174"/>
+      <c r="L7" s="178">
         <f>L6*M6</f>
         <v>61693884.297520652</v>
       </c>
-      <c r="M7" s="150"/>
-      <c r="N7" s="149">
+      <c r="M7" s="178"/>
+      <c r="N7" s="173">
         <f>N6*O6</f>
         <v>67302419.23365888</v>
       </c>
-      <c r="O7" s="151"/>
+      <c r="O7" s="174"/>
       <c r="P7" s="87"/>
     </row>
     <row r="8" spans="2:16" ht="13" thickBot="1">
       <c r="B8" s="87"/>
-      <c r="C8" s="146" t="s">
+      <c r="C8" s="183" t="s">
         <v>114</v>
       </c>
       <c r="D8" s="92">
@@ -3109,42 +3125,42 @@
     </row>
     <row r="9" spans="2:16" ht="13" thickBot="1">
       <c r="B9" s="87"/>
-      <c r="C9" s="148"/>
-      <c r="D9" s="152">
+      <c r="C9" s="185"/>
+      <c r="D9" s="176">
         <f>D8*E8</f>
         <v>6300000</v>
       </c>
-      <c r="E9" s="143"/>
-      <c r="F9" s="152">
+      <c r="E9" s="175"/>
+      <c r="F9" s="176">
         <f>F8*G8</f>
         <v>2344999.9999999991</v>
       </c>
-      <c r="G9" s="159"/>
-      <c r="H9" s="143">
+      <c r="G9" s="177"/>
+      <c r="H9" s="175">
         <f>H8*I8</f>
         <v>2696749.9999999995</v>
       </c>
-      <c r="I9" s="143"/>
-      <c r="J9" s="152">
+      <c r="I9" s="175"/>
+      <c r="J9" s="176">
         <f>J8*K8</f>
         <v>3101262.4999999986</v>
       </c>
-      <c r="K9" s="159"/>
-      <c r="L9" s="143">
+      <c r="K9" s="177"/>
+      <c r="L9" s="175">
         <f>L8*M8</f>
         <v>3566451.8749999981</v>
       </c>
-      <c r="M9" s="143"/>
-      <c r="N9" s="152">
+      <c r="M9" s="175"/>
+      <c r="N9" s="176">
         <f>N8*O8</f>
         <v>4101419.6562499977</v>
       </c>
-      <c r="O9" s="159"/>
+      <c r="O9" s="177"/>
       <c r="P9" s="87"/>
     </row>
     <row r="10" spans="2:16" ht="13" thickBot="1">
       <c r="B10" s="87"/>
-      <c r="C10" s="147" t="s">
+      <c r="C10" s="184" t="s">
         <v>90</v>
       </c>
       <c r="D10" s="92">
@@ -3198,42 +3214,42 @@
     </row>
     <row r="11" spans="2:16" ht="13" thickBot="1">
       <c r="B11" s="87"/>
-      <c r="C11" s="147"/>
-      <c r="D11" s="149">
+      <c r="C11" s="184"/>
+      <c r="D11" s="173">
         <f>D10*E10</f>
         <v>60000000</v>
       </c>
-      <c r="E11" s="150"/>
-      <c r="F11" s="149">
+      <c r="E11" s="178"/>
+      <c r="F11" s="173">
         <f>F10*G10</f>
         <v>68999999.999999985</v>
       </c>
-      <c r="G11" s="151"/>
-      <c r="H11" s="150">
+      <c r="G11" s="174"/>
+      <c r="H11" s="178">
         <f>H10*I10</f>
         <v>79349999.999999985</v>
       </c>
-      <c r="I11" s="150"/>
-      <c r="J11" s="149">
+      <c r="I11" s="178"/>
+      <c r="J11" s="173">
         <f>J10*K10</f>
         <v>91252499.99999997</v>
       </c>
-      <c r="K11" s="151"/>
-      <c r="L11" s="150">
+      <c r="K11" s="174"/>
+      <c r="L11" s="178">
         <f>L10*M10</f>
         <v>104940374.99999996</v>
       </c>
-      <c r="M11" s="150"/>
-      <c r="N11" s="149">
+      <c r="M11" s="178"/>
+      <c r="N11" s="173">
         <f>N10*O10</f>
         <v>120681431.24999994</v>
       </c>
-      <c r="O11" s="151"/>
+      <c r="O11" s="174"/>
       <c r="P11" s="87"/>
     </row>
     <row r="12" spans="2:16" ht="13" thickBot="1">
       <c r="B12" s="87"/>
-      <c r="C12" s="146" t="s">
+      <c r="C12" s="183" t="s">
         <v>122</v>
       </c>
       <c r="D12" s="92"/>
@@ -3282,42 +3298,42 @@
     </row>
     <row r="13" spans="2:16" ht="13" thickBot="1">
       <c r="B13" s="87"/>
-      <c r="C13" s="148"/>
-      <c r="D13" s="152">
+      <c r="C13" s="185"/>
+      <c r="D13" s="176">
         <f>D12*E12</f>
         <v>0</v>
       </c>
-      <c r="E13" s="143"/>
-      <c r="F13" s="152">
+      <c r="E13" s="175"/>
+      <c r="F13" s="176">
         <f>F12*G12</f>
         <v>9659999.9999999981</v>
       </c>
-      <c r="G13" s="159"/>
-      <c r="H13" s="143">
+      <c r="G13" s="177"/>
+      <c r="H13" s="175">
         <f>H12*I12</f>
         <v>11108999.999999996</v>
       </c>
-      <c r="I13" s="143"/>
-      <c r="J13" s="152">
+      <c r="I13" s="175"/>
+      <c r="J13" s="176">
         <f>J12*K12</f>
         <v>12775349.999999996</v>
       </c>
-      <c r="K13" s="159"/>
-      <c r="L13" s="143">
+      <c r="K13" s="177"/>
+      <c r="L13" s="175">
         <f>L12*M12</f>
         <v>14691652.499999993</v>
       </c>
-      <c r="M13" s="143"/>
-      <c r="N13" s="152">
+      <c r="M13" s="175"/>
+      <c r="N13" s="176">
         <f>N12*O12</f>
         <v>16895400.374999993</v>
       </c>
-      <c r="O13" s="159"/>
+      <c r="O13" s="177"/>
       <c r="P13" s="87"/>
     </row>
     <row r="14" spans="2:16" ht="13" thickBot="1">
       <c r="B14" s="87"/>
-      <c r="C14" s="147" t="s">
+      <c r="C14" s="184" t="s">
         <v>94</v>
       </c>
       <c r="D14" s="92"/>
@@ -3361,42 +3377,42 @@
     </row>
     <row r="15" spans="2:16" ht="13" thickBot="1">
       <c r="B15" s="87"/>
-      <c r="C15" s="147"/>
-      <c r="D15" s="149">
+      <c r="C15" s="184"/>
+      <c r="D15" s="173">
         <f>D14*E14</f>
         <v>0</v>
       </c>
-      <c r="E15" s="150"/>
-      <c r="F15" s="149">
+      <c r="E15" s="178"/>
+      <c r="F15" s="173">
         <f>F14*G14</f>
         <v>1724999.9999999995</v>
       </c>
-      <c r="G15" s="151"/>
-      <c r="H15" s="150">
+      <c r="G15" s="174"/>
+      <c r="H15" s="178">
         <f>H14*I14</f>
         <v>1983749.9999999995</v>
       </c>
-      <c r="I15" s="150"/>
-      <c r="J15" s="149">
+      <c r="I15" s="178"/>
+      <c r="J15" s="173">
         <f>J14*K14</f>
         <v>2281312.4999999991</v>
       </c>
-      <c r="K15" s="151"/>
-      <c r="L15" s="150">
+      <c r="K15" s="174"/>
+      <c r="L15" s="178">
         <f>L14*M14</f>
         <v>2623509.3749999991</v>
       </c>
-      <c r="M15" s="150"/>
-      <c r="N15" s="149">
+      <c r="M15" s="178"/>
+      <c r="N15" s="173">
         <f>N14*O14</f>
         <v>3017035.7812499986</v>
       </c>
-      <c r="O15" s="151"/>
+      <c r="O15" s="174"/>
       <c r="P15" s="87"/>
     </row>
     <row r="16" spans="2:16" ht="13" thickBot="1">
       <c r="B16" s="87"/>
-      <c r="C16" s="146" t="s">
+      <c r="C16" s="183" t="s">
         <v>95</v>
       </c>
       <c r="D16" s="92"/>
@@ -3440,37 +3456,37 @@
     </row>
     <row r="17" spans="2:16" ht="13" thickBot="1">
       <c r="B17" s="87"/>
-      <c r="C17" s="148"/>
-      <c r="D17" s="144">
+      <c r="C17" s="185"/>
+      <c r="D17" s="169">
         <f>D16*E16</f>
         <v>0</v>
       </c>
-      <c r="E17" s="145"/>
-      <c r="F17" s="144">
+      <c r="E17" s="172"/>
+      <c r="F17" s="169">
         <f>F16*G16</f>
         <v>5749999.9999999991</v>
       </c>
-      <c r="G17" s="160"/>
-      <c r="H17" s="145">
+      <c r="G17" s="170"/>
+      <c r="H17" s="172">
         <f>H16*I16</f>
         <v>6612499.9999999981</v>
       </c>
-      <c r="I17" s="145"/>
-      <c r="J17" s="144">
+      <c r="I17" s="172"/>
+      <c r="J17" s="169">
         <f>J16*K16</f>
         <v>7604374.9999999972</v>
       </c>
-      <c r="K17" s="160"/>
-      <c r="L17" s="145">
+      <c r="K17" s="170"/>
+      <c r="L17" s="172">
         <f>L16*M16</f>
         <v>8745031.2499999963</v>
       </c>
-      <c r="M17" s="145"/>
-      <c r="N17" s="144">
+      <c r="M17" s="172"/>
+      <c r="N17" s="169">
         <f>N16*O16</f>
         <v>10056785.937499996</v>
       </c>
-      <c r="O17" s="160"/>
+      <c r="O17" s="170"/>
       <c r="P17" s="87"/>
     </row>
     <row r="18" spans="2:16" ht="13" thickBot="1">
@@ -3478,36 +3494,36 @@
       <c r="C18" s="91" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="153">
+      <c r="D18" s="167">
         <f>D7+D9+D11+D13+D15+D17</f>
         <v>109500000</v>
       </c>
-      <c r="E18" s="154"/>
-      <c r="F18" s="153">
+      <c r="E18" s="171"/>
+      <c r="F18" s="167">
         <f>F7+F9+F11+F13+F15+F17</f>
         <v>135999999.99999997</v>
       </c>
-      <c r="G18" s="155"/>
-      <c r="H18" s="154">
+      <c r="G18" s="168"/>
+      <c r="H18" s="171">
         <f>H7+H9+H11+H13+H15+H17</f>
         <v>153591999.99999997</v>
       </c>
-      <c r="I18" s="154"/>
-      <c r="J18" s="153">
+      <c r="I18" s="171"/>
+      <c r="J18" s="167">
         <f>J7+J9+J11+J13+J15+J17</f>
         <v>173567527.27272725</v>
       </c>
-      <c r="K18" s="155"/>
-      <c r="L18" s="154">
+      <c r="K18" s="168"/>
+      <c r="L18" s="171">
         <f>L7+L9+L11+L13+L15+L17</f>
         <v>196260904.29752061</v>
       </c>
-      <c r="M18" s="154"/>
-      <c r="N18" s="153">
+      <c r="M18" s="171"/>
+      <c r="N18" s="167">
         <f>N7+N9+N11+N13+N15+N17</f>
         <v>222054492.23365882</v>
       </c>
-      <c r="O18" s="155"/>
+      <c r="O18" s="168"/>
       <c r="P18" s="87"/>
     </row>
     <row r="19" spans="2:16">
@@ -3544,12 +3560,12 @@
       <c r="P20" s="87"/>
     </row>
     <row r="21" spans="2:16">
-      <c r="C21" s="142" t="s">
+      <c r="C21" s="182" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="22" spans="2:16">
-      <c r="C22" s="142"/>
+      <c r="C22" s="182"/>
     </row>
     <row r="23" spans="2:16">
       <c r="C23" s="116">
@@ -3582,45 +3598,6 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="L13:M13"/>
     <mergeCell ref="D17:E17"/>
@@ -3637,6 +3614,45 @@
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="J15:K15"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -3701,10 +3717,10 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="87"/>
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="189" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="171"/>
+      <c r="C4" s="190"/>
       <c r="D4" s="6">
         <v>600000</v>
       </c>
@@ -3716,10 +3732,10 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="87"/>
-      <c r="B5" s="165" t="s">
+      <c r="B5" s="187" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="166"/>
+      <c r="C5" s="188"/>
       <c r="D5" s="4">
         <f>IF('HW y SW'!C5=0,100000,0)</f>
         <v>0</v>
@@ -3750,10 +3766,10 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="87"/>
-      <c r="B6" s="165" t="s">
+      <c r="B6" s="187" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="166"/>
+      <c r="C6" s="188"/>
       <c r="D6" s="4">
         <f>PERSONAL!E12</f>
         <v>8000000</v>
@@ -3792,10 +3808,10 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="87"/>
-      <c r="B7" s="165" t="s">
+      <c r="B7" s="187" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="166"/>
+      <c r="C7" s="188"/>
       <c r="D7" s="4">
         <v>100000</v>
       </c>
@@ -3833,10 +3849,10 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="87"/>
-      <c r="B8" s="165" t="s">
+      <c r="B8" s="187" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="166"/>
+      <c r="C8" s="188"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4">
         <v>13000</v>
@@ -3871,10 +3887,10 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="87"/>
-      <c r="B9" s="165" t="s">
+      <c r="B9" s="187" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="166"/>
+      <c r="C9" s="188"/>
       <c r="D9" s="4">
         <v>50000</v>
       </c>
@@ -3886,10 +3902,10 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="87"/>
-      <c r="B10" s="165" t="s">
+      <c r="B10" s="187" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="166"/>
+      <c r="C10" s="188"/>
       <c r="D10" s="4">
         <v>45000</v>
       </c>
@@ -3897,20 +3913,20 @@
         <f t="shared" si="0"/>
         <v>540000</v>
       </c>
-      <c r="G10" s="169" t="s">
+      <c r="G10" s="186" t="s">
         <v>132</v>
       </c>
-      <c r="H10" s="169"/>
+      <c r="H10" s="186"/>
       <c r="I10" s="131">
         <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="87"/>
-      <c r="B11" s="165" t="s">
+      <c r="B11" s="187" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="166"/>
+      <c r="C11" s="188"/>
       <c r="D11" s="4">
         <v>45000</v>
       </c>
@@ -3918,20 +3934,20 @@
         <f t="shared" si="0"/>
         <v>540000</v>
       </c>
-      <c r="G11" s="169" t="s">
+      <c r="G11" s="186" t="s">
         <v>133</v>
       </c>
-      <c r="H11" s="169"/>
+      <c r="H11" s="186"/>
       <c r="I11" s="131">
         <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="87"/>
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="187" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="166"/>
+      <c r="C12" s="188"/>
       <c r="D12" s="4">
         <f>'CREACIÓN CURSOS'!C9</f>
         <v>1100000</v>
@@ -3944,10 +3960,10 @@
     </row>
     <row r="13" spans="1:13" ht="13" thickBot="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="161" t="s">
+      <c r="B13" s="191" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="163"/>
+      <c r="C13" s="193"/>
       <c r="D13" s="5">
         <f>SUM(D4:D12)*0.02</f>
         <v>198800</v>
@@ -3961,10 +3977,10 @@
     <row r="14" spans="1:13" ht="13" thickBot="1">
       <c r="A14" s="87"/>
       <c r="B14" s="87"/>
-      <c r="C14" s="135" t="s">
+      <c r="C14" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="164"/>
+      <c r="D14" s="194"/>
       <c r="E14" s="11">
         <f>SUM(E4:E13)</f>
         <v>113378600</v>
@@ -3989,10 +4005,10 @@
     </row>
     <row r="17" spans="1:7" ht="13" thickBot="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="167" t="s">
+      <c r="B17" s="195" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="168"/>
+      <c r="C17" s="196"/>
       <c r="D17" s="29" t="s">
         <v>61</v>
       </c>
@@ -4013,10 +4029,10 @@
     </row>
     <row r="19" spans="1:7" ht="13" thickBot="1">
       <c r="A19" s="87"/>
-      <c r="B19" s="161" t="s">
+      <c r="B19" s="191" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="162"/>
+      <c r="C19" s="192"/>
       <c r="D19" s="86">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -4049,6 +4065,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="B9:C9"/>
@@ -4058,12 +4080,6 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -4555,10 +4571,10 @@
       </c>
     </row>
     <row r="2" spans="2:10" ht="13" thickBot="1">
-      <c r="D2" s="167" t="s">
+      <c r="D2" s="195" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="172"/>
+      <c r="E2" s="197"/>
     </row>
     <row r="3" spans="2:10" ht="13" thickBot="1">
       <c r="B3" s="8" t="s">
@@ -4752,10 +4768,10 @@
   <sheetData>
     <row r="3" spans="2:9" ht="13" thickBot="1"/>
     <row r="4" spans="2:9" ht="13" thickBot="1">
-      <c r="B4" s="173" t="s">
+      <c r="B4" s="198" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="164"/>
+      <c r="C4" s="194"/>
     </row>
     <row r="5" spans="2:9" ht="13" thickBot="1">
       <c r="B5" s="26" t="s">

</xml_diff>

<commit_message>
Revert "+ Cambios de Formato"
This reverts commit 4d74d904110e8ee78a1cdcd877de0cc9d176c7a2.
</commit_message>
<xml_diff>
--- a/FLUJO PESIMISTA.xlsx
+++ b/FLUJO PESIMISTA.xlsx
@@ -446,7 +446,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -1019,18 +1019,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1283,6 +1275,126 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1292,25 +1404,31 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="12" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="10" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="12" fillId="10" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="12" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="12" fillId="9" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1321,153 +1439,27 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="12" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="27">
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
@@ -1480,10 +1472,6 @@
     <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
@@ -1496,10 +1484,6 @@
     <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentual" xfId="1" builtinId="5"/>
@@ -1882,7 +1866,7 @@
   <dimension ref="B1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:D24"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1894,582 +1878,582 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="17">
-      <c r="B1" s="159" t="s">
+      <c r="B1" s="134" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="159"/>
-      <c r="G1" s="159"/>
-      <c r="H1" s="159"/>
-      <c r="I1" s="159"/>
-      <c r="J1" s="159"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="134"/>
+      <c r="J1" s="134"/>
     </row>
     <row r="4" spans="2:10" ht="14" thickBot="1">
-      <c r="B4" s="145"/>
-      <c r="C4" s="146" t="s">
+      <c r="B4" s="187"/>
+      <c r="C4" s="188" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="147"/>
-      <c r="E4" s="145"/>
-      <c r="F4" s="145"/>
-      <c r="G4" s="145"/>
-      <c r="H4" s="145"/>
-      <c r="I4" s="145"/>
-      <c r="J4" s="145"/>
+      <c r="D4" s="189"/>
+      <c r="E4" s="187"/>
+      <c r="F4" s="187"/>
+      <c r="G4" s="187"/>
+      <c r="H4" s="187"/>
+      <c r="I4" s="187"/>
+      <c r="J4" s="187"/>
     </row>
     <row r="5" spans="2:10" ht="16" thickBot="1">
-      <c r="B5" s="134" t="s">
+      <c r="B5" s="174" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="134" t="s">
+      <c r="C5" s="174" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="135">
+      <c r="D5" s="175">
         <v>0</v>
       </c>
-      <c r="E5" s="135">
+      <c r="E5" s="175">
         <v>1</v>
       </c>
-      <c r="F5" s="135">
+      <c r="F5" s="175">
         <v>2</v>
       </c>
-      <c r="G5" s="135">
+      <c r="G5" s="175">
         <v>3</v>
       </c>
-      <c r="H5" s="135">
+      <c r="H5" s="175">
         <v>4</v>
       </c>
-      <c r="I5" s="135">
+      <c r="I5" s="175">
         <v>5</v>
       </c>
-      <c r="J5" s="135">
+      <c r="J5" s="175">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="13" thickBot="1">
-      <c r="B6" s="136" t="s">
+      <c r="B6" s="176" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="136" t="s">
+      <c r="C6" s="176" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="148"/>
-      <c r="E6" s="137">
+      <c r="D6" s="190"/>
+      <c r="E6" s="177">
         <f>INGRESOS!D18</f>
         <v>109500000</v>
       </c>
-      <c r="F6" s="137">
+      <c r="F6" s="177">
         <f>INGRESOS!F18</f>
         <v>135999999.99999997</v>
       </c>
-      <c r="G6" s="137">
+      <c r="G6" s="177">
         <f>INGRESOS!H18</f>
         <v>153591999.99999997</v>
       </c>
-      <c r="H6" s="137">
+      <c r="H6" s="177">
         <f>INGRESOS!J18</f>
         <v>173567527.27272725</v>
       </c>
-      <c r="I6" s="137">
+      <c r="I6" s="177">
         <f>INGRESOS!L18</f>
         <v>196260904.29752061</v>
       </c>
-      <c r="J6" s="137">
+      <c r="J6" s="177">
         <f>INGRESOS!N18</f>
         <v>222054492.23365882</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="13" thickBot="1">
-      <c r="B7" s="136" t="s">
+      <c r="B7" s="176" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="136" t="s">
+      <c r="C7" s="176" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="149"/>
-      <c r="E7" s="137">
+      <c r="D7" s="191"/>
+      <c r="E7" s="177">
         <v>5000000</v>
       </c>
-      <c r="F7" s="137">
+      <c r="F7" s="177">
         <f>E7*1.3</f>
         <v>6500000</v>
       </c>
-      <c r="G7" s="137">
+      <c r="G7" s="177">
         <f>F7*1.3</f>
         <v>8450000</v>
       </c>
-      <c r="H7" s="137">
+      <c r="H7" s="177">
         <f>G7*1.3</f>
         <v>10985000</v>
       </c>
-      <c r="I7" s="137">
+      <c r="I7" s="177">
         <f>H7*1.3</f>
         <v>14280500</v>
       </c>
-      <c r="J7" s="137">
+      <c r="J7" s="177">
         <f>I7*1.3</f>
         <v>18564650</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="13" thickBot="1">
-      <c r="B8" s="136" t="s">
+      <c r="B8" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="136" t="s">
+      <c r="C8" s="176" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="149"/>
-      <c r="E8" s="137">
+      <c r="D8" s="191"/>
+      <c r="E8" s="177">
         <f>-'CREACIÓN CURSOS'!D14</f>
         <v>-4400000</v>
       </c>
-      <c r="F8" s="137">
+      <c r="F8" s="177">
         <f>-'CREACIÓN CURSOS'!E14</f>
         <v>-4400000</v>
       </c>
-      <c r="G8" s="137">
+      <c r="G8" s="177">
         <f>-'CREACIÓN CURSOS'!F14</f>
         <v>-4400000</v>
       </c>
-      <c r="H8" s="137">
+      <c r="H8" s="177">
         <f>-'CREACIÓN CURSOS'!G14</f>
         <v>-4400000</v>
       </c>
-      <c r="I8" s="137">
+      <c r="I8" s="177">
         <f>-'CREACIÓN CURSOS'!H14</f>
         <v>-4400000</v>
       </c>
-      <c r="J8" s="137">
+      <c r="J8" s="177">
         <f>-'CREACIÓN CURSOS'!I14</f>
         <v>-4400000</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="13" thickBot="1">
-      <c r="B9" s="136" t="s">
+      <c r="B9" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="136" t="s">
+      <c r="C9" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="149"/>
-      <c r="E9" s="137">
+      <c r="D9" s="191"/>
+      <c r="E9" s="177">
         <f>-INGRESOS!D18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-8212500.0000000009</v>
       </c>
-      <c r="F9" s="137">
+      <c r="F9" s="177">
         <f>-INGRESOS!F18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-10200000</v>
       </c>
-      <c r="G9" s="137">
+      <c r="G9" s="177">
         <f>-INGRESOS!H18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-11519400</v>
       </c>
-      <c r="H9" s="137">
+      <c r="H9" s="177">
         <f>-INGRESOS!J18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-13017564.545454545</v>
       </c>
-      <c r="I9" s="137">
+      <c r="I9" s="177">
         <f>-INGRESOS!L18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-14719567.822314048</v>
       </c>
-      <c r="J9" s="137">
+      <c r="J9" s="177">
         <f>-INGRESOS!N18*('ESTRUCTURA DE COSTOS'!$D$18+'ESTRUCTURA DE COSTOS'!$D$19)</f>
         <v>-16654086.917524414</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="13" thickBot="1">
-      <c r="B10" s="136" t="s">
+      <c r="B10" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="136" t="s">
+      <c r="C10" s="176" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="149"/>
-      <c r="E10" s="137">
+      <c r="D10" s="191"/>
+      <c r="E10" s="177">
         <f>-'ESTRUCTURA DE COSTOS'!H8</f>
         <v>-113378600</v>
       </c>
-      <c r="F10" s="137">
+      <c r="F10" s="177">
         <f>-'ESTRUCTURA DE COSTOS'!I8</f>
         <v>-123847530.00000001</v>
       </c>
-      <c r="G10" s="137">
+      <c r="G10" s="177">
         <f>-'ESTRUCTURA DE COSTOS'!J8</f>
         <v>-135319906.50000003</v>
       </c>
-      <c r="H10" s="137">
+      <c r="H10" s="177">
         <f>-'ESTRUCTURA DE COSTOS'!K8</f>
         <v>-147893901.82500005</v>
       </c>
-      <c r="I10" s="137">
+      <c r="I10" s="177">
         <f>-'ESTRUCTURA DE COSTOS'!L8</f>
         <v>-161677396.91625005</v>
       </c>
-      <c r="J10" s="137">
+      <c r="J10" s="177">
         <f>-'ESTRUCTURA DE COSTOS'!M8</f>
         <v>-176788946.76206258</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="13" thickBot="1">
-      <c r="B11" s="136" t="s">
+      <c r="B11" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="136" t="s">
+      <c r="C11" s="176" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="149"/>
-      <c r="E11" s="137">
+      <c r="D11" s="191"/>
+      <c r="E11" s="177">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="F11" s="137">
+      <c r="F11" s="177">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="G11" s="137">
+      <c r="G11" s="177">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="H11" s="137">
+      <c r="H11" s="177">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="I11" s="137">
+      <c r="I11" s="177">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
-      <c r="J11" s="137">
+      <c r="J11" s="177">
         <f>-DEPRECIACION!$G$9</f>
         <v>-526666.66666666663</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="13" thickBot="1">
-      <c r="B12" s="138" t="s">
+      <c r="B12" s="178" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="138" t="s">
+      <c r="C12" s="178" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="150"/>
-      <c r="E12" s="139">
+      <c r="D12" s="192"/>
+      <c r="E12" s="179">
         <f t="shared" ref="E12:J12" si="0">SUM(E6:E11)</f>
         <v>-12017766.666666666</v>
       </c>
-      <c r="F12" s="139">
+      <c r="F12" s="179">
         <f t="shared" si="0"/>
         <v>3525803.3333332888</v>
       </c>
-      <c r="G12" s="139">
+      <c r="G12" s="179">
         <f t="shared" si="0"/>
         <v>10276026.833333274</v>
       </c>
-      <c r="H12" s="139">
+      <c r="H12" s="179">
         <f t="shared" si="0"/>
         <v>18714394.235606004</v>
       </c>
-      <c r="I12" s="139">
+      <c r="I12" s="179">
         <f t="shared" si="0"/>
         <v>29217772.892289836</v>
       </c>
-      <c r="J12" s="139">
+      <c r="J12" s="179">
         <f t="shared" si="0"/>
         <v>42249441.88740515</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="13" thickBot="1">
-      <c r="B13" s="136" t="s">
+      <c r="B13" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="136" t="s">
+      <c r="C13" s="176" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="149"/>
-      <c r="E13" s="137">
+      <c r="D13" s="191"/>
+      <c r="E13" s="177">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="F13" s="137">
+      <c r="F13" s="177">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="G13" s="137">
+      <c r="G13" s="177">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="H13" s="137">
+      <c r="H13" s="177">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="I13" s="137">
+      <c r="I13" s="177">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
-      <c r="J13" s="137">
+      <c r="J13" s="177">
         <f>'G. FINANCIERO'!$E$5</f>
         <v>-2839324.8655647454</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="13" thickBot="1">
-      <c r="B14" s="138" t="s">
+      <c r="B14" s="178" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="138" t="s">
+      <c r="C14" s="178" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="150"/>
-      <c r="E14" s="139">
+      <c r="D14" s="192"/>
+      <c r="E14" s="179">
         <f t="shared" ref="E14:J14" si="1">SUM(E12:E13)</f>
         <v>-14857091.532231411</v>
       </c>
-      <c r="F14" s="139">
+      <c r="F14" s="179">
         <f t="shared" si="1"/>
         <v>686478.4677685434</v>
       </c>
-      <c r="G14" s="139">
+      <c r="G14" s="179">
         <f t="shared" si="1"/>
         <v>7436701.9677685294</v>
       </c>
-      <c r="H14" s="139">
+      <c r="H14" s="179">
         <f t="shared" si="1"/>
         <v>15875069.370041259</v>
       </c>
-      <c r="I14" s="139">
+      <c r="I14" s="179">
         <f t="shared" si="1"/>
         <v>26378448.026725091</v>
       </c>
-      <c r="J14" s="139">
+      <c r="J14" s="179">
         <f t="shared" si="1"/>
         <v>39410117.021840401</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="13" thickBot="1">
-      <c r="B15" s="136" t="s">
+      <c r="B15" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="136" t="s">
+      <c r="C15" s="176" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="149"/>
-      <c r="E15" s="137">
+      <c r="D15" s="191"/>
+      <c r="E15" s="177">
         <f t="shared" ref="E15:J15" si="2">+IF(E14&gt;0,-(E14*0.17),0)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="137">
+      <c r="F15" s="177">
         <f t="shared" si="2"/>
         <v>-116701.33952065239</v>
       </c>
-      <c r="G15" s="137">
+      <c r="G15" s="177">
         <f t="shared" si="2"/>
         <v>-1264239.3345206501</v>
       </c>
-      <c r="H15" s="137">
+      <c r="H15" s="177">
         <f t="shared" si="2"/>
         <v>-2698761.792907014</v>
       </c>
-      <c r="I15" s="137">
+      <c r="I15" s="177">
         <f t="shared" si="2"/>
         <v>-4484336.1645432655</v>
       </c>
-      <c r="J15" s="137">
+      <c r="J15" s="177">
         <f t="shared" si="2"/>
         <v>-6699719.8937128689</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="13" thickBot="1">
-      <c r="B16" s="136" t="s">
+      <c r="B16" s="176" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="136" t="s">
+      <c r="C16" s="176" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="149"/>
-      <c r="E16" s="137">
+      <c r="D16" s="191"/>
+      <c r="E16" s="177">
         <f t="shared" ref="E16:J16" si="3">-(E11)</f>
         <v>526666.66666666663</v>
       </c>
-      <c r="F16" s="137">
+      <c r="F16" s="177">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
-      <c r="G16" s="137">
+      <c r="G16" s="177">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
-      <c r="H16" s="137">
+      <c r="H16" s="177">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
-      <c r="I16" s="137">
+      <c r="I16" s="177">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
-      <c r="J16" s="137">
+      <c r="J16" s="177">
         <f t="shared" si="3"/>
         <v>526666.66666666663</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="13" thickBot="1">
-      <c r="B17" s="136" t="s">
+      <c r="B17" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="136" t="s">
+      <c r="C17" s="176" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="149"/>
-      <c r="E17" s="137">
+      <c r="D17" s="191"/>
+      <c r="E17" s="177">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="F17" s="137">
+      <c r="F17" s="177">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="G17" s="137">
+      <c r="G17" s="177">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="H17" s="137">
+      <c r="H17" s="177">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="I17" s="137">
+      <c r="I17" s="177">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
-      <c r="J17" s="137">
+      <c r="J17" s="177">
         <f>-'G. FINANCIERO'!$C$7</f>
         <v>-2061000</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="13" thickBot="1">
-      <c r="B18" s="136" t="s">
+      <c r="B18" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="136" t="s">
+      <c r="C18" s="176" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="151">
+      <c r="D18" s="193">
         <f>-INVERSION!D20</f>
         <v>-20610000</v>
       </c>
-      <c r="E18" s="137"/>
-      <c r="F18" s="137"/>
-      <c r="G18" s="137"/>
-      <c r="H18" s="137"/>
-      <c r="I18" s="137"/>
-      <c r="J18" s="137"/>
+      <c r="E18" s="177"/>
+      <c r="F18" s="177"/>
+      <c r="G18" s="177"/>
+      <c r="H18" s="177"/>
+      <c r="I18" s="177"/>
+      <c r="J18" s="177"/>
     </row>
     <row r="19" spans="2:10" ht="13" thickBot="1">
-      <c r="B19" s="136"/>
-      <c r="C19" s="136" t="s">
+      <c r="B19" s="176"/>
+      <c r="C19" s="176" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="152">
+      <c r="D19" s="194">
         <f>'G. FINANCIERO'!C5</f>
         <v>12366000</v>
       </c>
-      <c r="E19" s="137"/>
-      <c r="F19" s="137"/>
-      <c r="G19" s="137"/>
-      <c r="H19" s="137"/>
-      <c r="I19" s="137"/>
-      <c r="J19" s="137"/>
+      <c r="E19" s="177"/>
+      <c r="F19" s="177"/>
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177"/>
+      <c r="J19" s="177"/>
     </row>
     <row r="20" spans="2:10" ht="13" thickBot="1">
-      <c r="B20" s="140" t="s">
+      <c r="B20" s="180" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="140" t="s">
+      <c r="C20" s="180" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="141">
+      <c r="D20" s="181">
         <f>SUM(D18:D19)</f>
         <v>-8244000</v>
       </c>
-      <c r="E20" s="142">
+      <c r="E20" s="182">
         <f t="shared" ref="E20:J20" si="4">SUM(E14:E19)</f>
         <v>-16391424.865564745</v>
       </c>
-      <c r="F20" s="142">
+      <c r="F20" s="182">
         <f t="shared" si="4"/>
         <v>-964556.2050854424</v>
       </c>
-      <c r="G20" s="142">
+      <c r="G20" s="182">
         <f t="shared" si="4"/>
         <v>4638129.2999145463</v>
       </c>
-      <c r="H20" s="142">
+      <c r="H20" s="182">
         <f t="shared" si="4"/>
         <v>11641974.24380091</v>
       </c>
-      <c r="I20" s="142">
+      <c r="I20" s="182">
         <f t="shared" si="4"/>
         <v>20359778.528848495</v>
       </c>
-      <c r="J20" s="142">
+      <c r="J20" s="182">
         <f t="shared" si="4"/>
         <v>31176063.794794198</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="13" thickBot="1">
-      <c r="B21" s="153"/>
-      <c r="C21" s="153"/>
-      <c r="D21" s="154"/>
-      <c r="E21" s="154"/>
-      <c r="F21" s="154"/>
-      <c r="G21" s="154"/>
-      <c r="H21" s="154"/>
-      <c r="I21" s="154"/>
-      <c r="J21" s="154"/>
+      <c r="B21" s="195"/>
+      <c r="C21" s="195"/>
+      <c r="D21" s="196"/>
+      <c r="E21" s="196"/>
+      <c r="F21" s="196"/>
+      <c r="G21" s="196"/>
+      <c r="H21" s="196"/>
+      <c r="I21" s="196"/>
+      <c r="J21" s="196"/>
     </row>
     <row r="22" spans="2:10" ht="16" thickBot="1">
-      <c r="B22" s="157" t="s">
+      <c r="B22" s="183" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="158"/>
-      <c r="D22" s="143">
+      <c r="C22" s="184"/>
+      <c r="D22" s="185">
         <f>NPV(D24,E20:J20)+D20</f>
         <v>10079906.799768489</v>
       </c>
-      <c r="E22" s="154"/>
-      <c r="F22" s="155"/>
-      <c r="G22" s="154"/>
-      <c r="H22" s="154"/>
-      <c r="I22" s="154"/>
-      <c r="J22" s="154"/>
+      <c r="E22" s="196"/>
+      <c r="F22" s="197"/>
+      <c r="G22" s="196"/>
+      <c r="H22" s="196"/>
+      <c r="I22" s="196"/>
+      <c r="J22" s="196"/>
     </row>
     <row r="23" spans="2:10" ht="16" thickBot="1">
-      <c r="B23" s="157" t="s">
+      <c r="B23" s="183" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="158"/>
-      <c r="D23" s="144">
+      <c r="C23" s="184"/>
+      <c r="D23" s="186">
         <f>IRR(D20:J20)</f>
         <v>0.25017156683584729</v>
       </c>
-      <c r="E23" s="153"/>
-      <c r="F23" s="156"/>
-      <c r="G23" s="153"/>
-      <c r="H23" s="153"/>
-      <c r="I23" s="153"/>
-      <c r="J23" s="153"/>
+      <c r="E23" s="195"/>
+      <c r="F23" s="198"/>
+      <c r="G23" s="195"/>
+      <c r="H23" s="195"/>
+      <c r="I23" s="195"/>
+      <c r="J23" s="195"/>
     </row>
     <row r="24" spans="2:10" ht="16" thickBot="1">
-      <c r="B24" s="157" t="s">
+      <c r="B24" s="183" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="157"/>
-      <c r="D24" s="144">
+      <c r="C24" s="183"/>
+      <c r="D24" s="186">
         <v>0.15</v>
       </c>
-      <c r="E24" s="153"/>
-      <c r="F24" s="153"/>
-      <c r="G24" s="153"/>
-      <c r="H24" s="153"/>
-      <c r="I24" s="153"/>
-      <c r="J24" s="153"/>
+      <c r="E24" s="195"/>
+      <c r="F24" s="195"/>
+      <c r="G24" s="195"/>
+      <c r="H24" s="195"/>
+      <c r="I24" s="195"/>
+      <c r="J24" s="195"/>
     </row>
     <row r="27" spans="2:10">
       <c r="C27" s="121"/>
@@ -2687,19 +2671,19 @@
   <sheetData>
     <row r="3" spans="2:4" ht="13" thickBot="1"/>
     <row r="4" spans="2:4" ht="13" thickBot="1">
-      <c r="B4" s="164" t="s">
+      <c r="B4" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="165"/>
+      <c r="C4" s="140"/>
       <c r="D4" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="13" thickBot="1">
-      <c r="B5" s="162" t="s">
+      <c r="B5" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="163"/>
+      <c r="C5" s="138"/>
       <c r="D5" s="44"/>
     </row>
     <row r="6" spans="2:4">
@@ -2717,28 +2701,28 @@
       <c r="D7" s="18"/>
     </row>
     <row r="8" spans="2:4" ht="13" thickBot="1">
-      <c r="B8" s="162" t="s">
+      <c r="B8" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="166"/>
+      <c r="C8" s="141"/>
       <c r="D8" s="45">
         <v>5000000</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="13" thickBot="1">
-      <c r="B9" s="162" t="s">
+      <c r="B9" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="163"/>
+      <c r="C9" s="138"/>
       <c r="D9" s="45">
         <v>2500000</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="13" thickBot="1">
-      <c r="B10" s="162" t="s">
+      <c r="B10" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="163"/>
+      <c r="C10" s="138"/>
       <c r="D10" s="44"/>
     </row>
     <row r="11" spans="2:4">
@@ -2776,10 +2760,10 @@
       </c>
     </row>
     <row r="14" spans="2:4" ht="13" thickBot="1">
-      <c r="B14" s="162" t="s">
+      <c r="B14" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="163"/>
+      <c r="C14" s="138"/>
       <c r="D14" s="44"/>
     </row>
     <row r="15" spans="2:4">
@@ -2829,10 +2813,10 @@
       </c>
     </row>
     <row r="20" spans="2:4" ht="13" thickBot="1">
-      <c r="B20" s="160" t="s">
+      <c r="B20" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="161"/>
+      <c r="C20" s="136"/>
       <c r="D20" s="46">
         <f>SUM(D5:D19)</f>
         <v>20610000</v>
@@ -2923,30 +2907,30 @@
     <row r="4" spans="2:16" ht="13" thickBot="1">
       <c r="B4" s="87"/>
       <c r="C4" s="87"/>
-      <c r="D4" s="179" t="s">
+      <c r="D4" s="156" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="181"/>
-      <c r="F4" s="179" t="s">
+      <c r="E4" s="158"/>
+      <c r="F4" s="156" t="s">
         <v>96</v>
       </c>
-      <c r="G4" s="180"/>
-      <c r="H4" s="181" t="s">
+      <c r="G4" s="157"/>
+      <c r="H4" s="158" t="s">
         <v>97</v>
       </c>
-      <c r="I4" s="181"/>
-      <c r="J4" s="179" t="s">
+      <c r="I4" s="158"/>
+      <c r="J4" s="156" t="s">
         <v>98</v>
       </c>
-      <c r="K4" s="180"/>
-      <c r="L4" s="181" t="s">
+      <c r="K4" s="157"/>
+      <c r="L4" s="158" t="s">
         <v>99</v>
       </c>
-      <c r="M4" s="181"/>
-      <c r="N4" s="179" t="s">
+      <c r="M4" s="158"/>
+      <c r="N4" s="156" t="s">
         <v>100</v>
       </c>
-      <c r="O4" s="180"/>
+      <c r="O4" s="157"/>
       <c r="P4" s="87"/>
     </row>
     <row r="5" spans="2:16" ht="13" thickBot="1">
@@ -2992,7 +2976,7 @@
     </row>
     <row r="6" spans="2:16" ht="13" thickBot="1">
       <c r="B6" s="87"/>
-      <c r="C6" s="183" t="s">
+      <c r="C6" s="146" t="s">
         <v>89</v>
       </c>
       <c r="D6" s="115">
@@ -3041,42 +3025,42 @@
     </row>
     <row r="7" spans="2:16" ht="13" thickBot="1">
       <c r="B7" s="87"/>
-      <c r="C7" s="184"/>
-      <c r="D7" s="173">
+      <c r="C7" s="147"/>
+      <c r="D7" s="149">
         <f>D6*E6</f>
         <v>43200000</v>
       </c>
-      <c r="E7" s="178"/>
-      <c r="F7" s="173">
+      <c r="E7" s="150"/>
+      <c r="F7" s="149">
         <f>F6*G6</f>
         <v>47520000</v>
       </c>
-      <c r="G7" s="174"/>
-      <c r="H7" s="178">
+      <c r="G7" s="151"/>
+      <c r="H7" s="150">
         <f>H6*I6</f>
         <v>51840000</v>
       </c>
-      <c r="I7" s="178"/>
-      <c r="J7" s="173">
+      <c r="I7" s="150"/>
+      <c r="J7" s="149">
         <f>J6*K6</f>
         <v>56552727.272727266</v>
       </c>
-      <c r="K7" s="174"/>
-      <c r="L7" s="178">
+      <c r="K7" s="151"/>
+      <c r="L7" s="150">
         <f>L6*M6</f>
         <v>61693884.297520652</v>
       </c>
-      <c r="M7" s="178"/>
-      <c r="N7" s="173">
+      <c r="M7" s="150"/>
+      <c r="N7" s="149">
         <f>N6*O6</f>
         <v>67302419.23365888</v>
       </c>
-      <c r="O7" s="174"/>
+      <c r="O7" s="151"/>
       <c r="P7" s="87"/>
     </row>
     <row r="8" spans="2:16" ht="13" thickBot="1">
       <c r="B8" s="87"/>
-      <c r="C8" s="183" t="s">
+      <c r="C8" s="146" t="s">
         <v>114</v>
       </c>
       <c r="D8" s="92">
@@ -3125,42 +3109,42 @@
     </row>
     <row r="9" spans="2:16" ht="13" thickBot="1">
       <c r="B9" s="87"/>
-      <c r="C9" s="185"/>
-      <c r="D9" s="176">
+      <c r="C9" s="148"/>
+      <c r="D9" s="152">
         <f>D8*E8</f>
         <v>6300000</v>
       </c>
-      <c r="E9" s="175"/>
-      <c r="F9" s="176">
+      <c r="E9" s="143"/>
+      <c r="F9" s="152">
         <f>F8*G8</f>
         <v>2344999.9999999991</v>
       </c>
-      <c r="G9" s="177"/>
-      <c r="H9" s="175">
+      <c r="G9" s="159"/>
+      <c r="H9" s="143">
         <f>H8*I8</f>
         <v>2696749.9999999995</v>
       </c>
-      <c r="I9" s="175"/>
-      <c r="J9" s="176">
+      <c r="I9" s="143"/>
+      <c r="J9" s="152">
         <f>J8*K8</f>
         <v>3101262.4999999986</v>
       </c>
-      <c r="K9" s="177"/>
-      <c r="L9" s="175">
+      <c r="K9" s="159"/>
+      <c r="L9" s="143">
         <f>L8*M8</f>
         <v>3566451.8749999981</v>
       </c>
-      <c r="M9" s="175"/>
-      <c r="N9" s="176">
+      <c r="M9" s="143"/>
+      <c r="N9" s="152">
         <f>N8*O8</f>
         <v>4101419.6562499977</v>
       </c>
-      <c r="O9" s="177"/>
+      <c r="O9" s="159"/>
       <c r="P9" s="87"/>
     </row>
     <row r="10" spans="2:16" ht="13" thickBot="1">
       <c r="B10" s="87"/>
-      <c r="C10" s="184" t="s">
+      <c r="C10" s="147" t="s">
         <v>90</v>
       </c>
       <c r="D10" s="92">
@@ -3214,42 +3198,42 @@
     </row>
     <row r="11" spans="2:16" ht="13" thickBot="1">
       <c r="B11" s="87"/>
-      <c r="C11" s="184"/>
-      <c r="D11" s="173">
+      <c r="C11" s="147"/>
+      <c r="D11" s="149">
         <f>D10*E10</f>
         <v>60000000</v>
       </c>
-      <c r="E11" s="178"/>
-      <c r="F11" s="173">
+      <c r="E11" s="150"/>
+      <c r="F11" s="149">
         <f>F10*G10</f>
         <v>68999999.999999985</v>
       </c>
-      <c r="G11" s="174"/>
-      <c r="H11" s="178">
+      <c r="G11" s="151"/>
+      <c r="H11" s="150">
         <f>H10*I10</f>
         <v>79349999.999999985</v>
       </c>
-      <c r="I11" s="178"/>
-      <c r="J11" s="173">
+      <c r="I11" s="150"/>
+      <c r="J11" s="149">
         <f>J10*K10</f>
         <v>91252499.99999997</v>
       </c>
-      <c r="K11" s="174"/>
-      <c r="L11" s="178">
+      <c r="K11" s="151"/>
+      <c r="L11" s="150">
         <f>L10*M10</f>
         <v>104940374.99999996</v>
       </c>
-      <c r="M11" s="178"/>
-      <c r="N11" s="173">
+      <c r="M11" s="150"/>
+      <c r="N11" s="149">
         <f>N10*O10</f>
         <v>120681431.24999994</v>
       </c>
-      <c r="O11" s="174"/>
+      <c r="O11" s="151"/>
       <c r="P11" s="87"/>
     </row>
     <row r="12" spans="2:16" ht="13" thickBot="1">
       <c r="B12" s="87"/>
-      <c r="C12" s="183" t="s">
+      <c r="C12" s="146" t="s">
         <v>122</v>
       </c>
       <c r="D12" s="92"/>
@@ -3298,42 +3282,42 @@
     </row>
     <row r="13" spans="2:16" ht="13" thickBot="1">
       <c r="B13" s="87"/>
-      <c r="C13" s="185"/>
-      <c r="D13" s="176">
+      <c r="C13" s="148"/>
+      <c r="D13" s="152">
         <f>D12*E12</f>
         <v>0</v>
       </c>
-      <c r="E13" s="175"/>
-      <c r="F13" s="176">
+      <c r="E13" s="143"/>
+      <c r="F13" s="152">
         <f>F12*G12</f>
         <v>9659999.9999999981</v>
       </c>
-      <c r="G13" s="177"/>
-      <c r="H13" s="175">
+      <c r="G13" s="159"/>
+      <c r="H13" s="143">
         <f>H12*I12</f>
         <v>11108999.999999996</v>
       </c>
-      <c r="I13" s="175"/>
-      <c r="J13" s="176">
+      <c r="I13" s="143"/>
+      <c r="J13" s="152">
         <f>J12*K12</f>
         <v>12775349.999999996</v>
       </c>
-      <c r="K13" s="177"/>
-      <c r="L13" s="175">
+      <c r="K13" s="159"/>
+      <c r="L13" s="143">
         <f>L12*M12</f>
         <v>14691652.499999993</v>
       </c>
-      <c r="M13" s="175"/>
-      <c r="N13" s="176">
+      <c r="M13" s="143"/>
+      <c r="N13" s="152">
         <f>N12*O12</f>
         <v>16895400.374999993</v>
       </c>
-      <c r="O13" s="177"/>
+      <c r="O13" s="159"/>
       <c r="P13" s="87"/>
     </row>
     <row r="14" spans="2:16" ht="13" thickBot="1">
       <c r="B14" s="87"/>
-      <c r="C14" s="184" t="s">
+      <c r="C14" s="147" t="s">
         <v>94</v>
       </c>
       <c r="D14" s="92"/>
@@ -3377,42 +3361,42 @@
     </row>
     <row r="15" spans="2:16" ht="13" thickBot="1">
       <c r="B15" s="87"/>
-      <c r="C15" s="184"/>
-      <c r="D15" s="173">
+      <c r="C15" s="147"/>
+      <c r="D15" s="149">
         <f>D14*E14</f>
         <v>0</v>
       </c>
-      <c r="E15" s="178"/>
-      <c r="F15" s="173">
+      <c r="E15" s="150"/>
+      <c r="F15" s="149">
         <f>F14*G14</f>
         <v>1724999.9999999995</v>
       </c>
-      <c r="G15" s="174"/>
-      <c r="H15" s="178">
+      <c r="G15" s="151"/>
+      <c r="H15" s="150">
         <f>H14*I14</f>
         <v>1983749.9999999995</v>
       </c>
-      <c r="I15" s="178"/>
-      <c r="J15" s="173">
+      <c r="I15" s="150"/>
+      <c r="J15" s="149">
         <f>J14*K14</f>
         <v>2281312.4999999991</v>
       </c>
-      <c r="K15" s="174"/>
-      <c r="L15" s="178">
+      <c r="K15" s="151"/>
+      <c r="L15" s="150">
         <f>L14*M14</f>
         <v>2623509.3749999991</v>
       </c>
-      <c r="M15" s="178"/>
-      <c r="N15" s="173">
+      <c r="M15" s="150"/>
+      <c r="N15" s="149">
         <f>N14*O14</f>
         <v>3017035.7812499986</v>
       </c>
-      <c r="O15" s="174"/>
+      <c r="O15" s="151"/>
       <c r="P15" s="87"/>
     </row>
     <row r="16" spans="2:16" ht="13" thickBot="1">
       <c r="B16" s="87"/>
-      <c r="C16" s="183" t="s">
+      <c r="C16" s="146" t="s">
         <v>95</v>
       </c>
       <c r="D16" s="92"/>
@@ -3456,37 +3440,37 @@
     </row>
     <row r="17" spans="2:16" ht="13" thickBot="1">
       <c r="B17" s="87"/>
-      <c r="C17" s="185"/>
-      <c r="D17" s="169">
+      <c r="C17" s="148"/>
+      <c r="D17" s="144">
         <f>D16*E16</f>
         <v>0</v>
       </c>
-      <c r="E17" s="172"/>
-      <c r="F17" s="169">
+      <c r="E17" s="145"/>
+      <c r="F17" s="144">
         <f>F16*G16</f>
         <v>5749999.9999999991</v>
       </c>
-      <c r="G17" s="170"/>
-      <c r="H17" s="172">
+      <c r="G17" s="160"/>
+      <c r="H17" s="145">
         <f>H16*I16</f>
         <v>6612499.9999999981</v>
       </c>
-      <c r="I17" s="172"/>
-      <c r="J17" s="169">
+      <c r="I17" s="145"/>
+      <c r="J17" s="144">
         <f>J16*K16</f>
         <v>7604374.9999999972</v>
       </c>
-      <c r="K17" s="170"/>
-      <c r="L17" s="172">
+      <c r="K17" s="160"/>
+      <c r="L17" s="145">
         <f>L16*M16</f>
         <v>8745031.2499999963</v>
       </c>
-      <c r="M17" s="172"/>
-      <c r="N17" s="169">
+      <c r="M17" s="145"/>
+      <c r="N17" s="144">
         <f>N16*O16</f>
         <v>10056785.937499996</v>
       </c>
-      <c r="O17" s="170"/>
+      <c r="O17" s="160"/>
       <c r="P17" s="87"/>
     </row>
     <row r="18" spans="2:16" ht="13" thickBot="1">
@@ -3494,36 +3478,36 @@
       <c r="C18" s="91" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="167">
+      <c r="D18" s="153">
         <f>D7+D9+D11+D13+D15+D17</f>
         <v>109500000</v>
       </c>
-      <c r="E18" s="171"/>
-      <c r="F18" s="167">
+      <c r="E18" s="154"/>
+      <c r="F18" s="153">
         <f>F7+F9+F11+F13+F15+F17</f>
         <v>135999999.99999997</v>
       </c>
-      <c r="G18" s="168"/>
-      <c r="H18" s="171">
+      <c r="G18" s="155"/>
+      <c r="H18" s="154">
         <f>H7+H9+H11+H13+H15+H17</f>
         <v>153591999.99999997</v>
       </c>
-      <c r="I18" s="171"/>
-      <c r="J18" s="167">
+      <c r="I18" s="154"/>
+      <c r="J18" s="153">
         <f>J7+J9+J11+J13+J15+J17</f>
         <v>173567527.27272725</v>
       </c>
-      <c r="K18" s="168"/>
-      <c r="L18" s="171">
+      <c r="K18" s="155"/>
+      <c r="L18" s="154">
         <f>L7+L9+L11+L13+L15+L17</f>
         <v>196260904.29752061</v>
       </c>
-      <c r="M18" s="171"/>
-      <c r="N18" s="167">
+      <c r="M18" s="154"/>
+      <c r="N18" s="153">
         <f>N7+N9+N11+N13+N15+N17</f>
         <v>222054492.23365882</v>
       </c>
-      <c r="O18" s="168"/>
+      <c r="O18" s="155"/>
       <c r="P18" s="87"/>
     </row>
     <row r="19" spans="2:16">
@@ -3560,12 +3544,12 @@
       <c r="P20" s="87"/>
     </row>
     <row r="21" spans="2:16">
-      <c r="C21" s="182" t="s">
+      <c r="C21" s="142" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="22" spans="2:16">
-      <c r="C22" s="182"/>
+      <c r="C22" s="142"/>
     </row>
     <row r="23" spans="2:16">
       <c r="C23" s="116">
@@ -3598,6 +3582,45 @@
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="L13:M13"/>
     <mergeCell ref="D17:E17"/>
@@ -3614,45 +3637,6 @@
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="J15:K15"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:K18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -3717,10 +3701,10 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="87"/>
-      <c r="B4" s="189" t="s">
+      <c r="B4" s="170" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="190"/>
+      <c r="C4" s="171"/>
       <c r="D4" s="6">
         <v>600000</v>
       </c>
@@ -3732,10 +3716,10 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="87"/>
-      <c r="B5" s="187" t="s">
+      <c r="B5" s="165" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="188"/>
+      <c r="C5" s="166"/>
       <c r="D5" s="4">
         <f>IF('HW y SW'!C5=0,100000,0)</f>
         <v>0</v>
@@ -3766,10 +3750,10 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="87"/>
-      <c r="B6" s="187" t="s">
+      <c r="B6" s="165" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="188"/>
+      <c r="C6" s="166"/>
       <c r="D6" s="4">
         <f>PERSONAL!E12</f>
         <v>8000000</v>
@@ -3808,10 +3792,10 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="87"/>
-      <c r="B7" s="187" t="s">
+      <c r="B7" s="165" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="188"/>
+      <c r="C7" s="166"/>
       <c r="D7" s="4">
         <v>100000</v>
       </c>
@@ -3849,10 +3833,10 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="87"/>
-      <c r="B8" s="187" t="s">
+      <c r="B8" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="188"/>
+      <c r="C8" s="166"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4">
         <v>13000</v>
@@ -3887,10 +3871,10 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="87"/>
-      <c r="B9" s="187" t="s">
+      <c r="B9" s="165" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="188"/>
+      <c r="C9" s="166"/>
       <c r="D9" s="4">
         <v>50000</v>
       </c>
@@ -3902,10 +3886,10 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="87"/>
-      <c r="B10" s="187" t="s">
+      <c r="B10" s="165" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="188"/>
+      <c r="C10" s="166"/>
       <c r="D10" s="4">
         <v>45000</v>
       </c>
@@ -3913,20 +3897,20 @@
         <f t="shared" si="0"/>
         <v>540000</v>
       </c>
-      <c r="G10" s="186" t="s">
+      <c r="G10" s="169" t="s">
         <v>132</v>
       </c>
-      <c r="H10" s="186"/>
+      <c r="H10" s="169"/>
       <c r="I10" s="131">
         <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="87"/>
-      <c r="B11" s="187" t="s">
+      <c r="B11" s="165" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="188"/>
+      <c r="C11" s="166"/>
       <c r="D11" s="4">
         <v>45000</v>
       </c>
@@ -3934,20 +3918,20 @@
         <f t="shared" si="0"/>
         <v>540000</v>
       </c>
-      <c r="G11" s="186" t="s">
+      <c r="G11" s="169" t="s">
         <v>133</v>
       </c>
-      <c r="H11" s="186"/>
+      <c r="H11" s="169"/>
       <c r="I11" s="131">
         <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="87"/>
-      <c r="B12" s="187" t="s">
+      <c r="B12" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="188"/>
+      <c r="C12" s="166"/>
       <c r="D12" s="4">
         <f>'CREACIÓN CURSOS'!C9</f>
         <v>1100000</v>
@@ -3960,10 +3944,10 @@
     </row>
     <row r="13" spans="1:13" ht="13" thickBot="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="191" t="s">
+      <c r="B13" s="161" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="193"/>
+      <c r="C13" s="163"/>
       <c r="D13" s="5">
         <f>SUM(D4:D12)*0.02</f>
         <v>198800</v>
@@ -3977,10 +3961,10 @@
     <row r="14" spans="1:13" ht="13" thickBot="1">
       <c r="A14" s="87"/>
       <c r="B14" s="87"/>
-      <c r="C14" s="160" t="s">
+      <c r="C14" s="135" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="194"/>
+      <c r="D14" s="164"/>
       <c r="E14" s="11">
         <f>SUM(E4:E13)</f>
         <v>113378600</v>
@@ -4005,10 +3989,10 @@
     </row>
     <row r="17" spans="1:7" ht="13" thickBot="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="195" t="s">
+      <c r="B17" s="167" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="196"/>
+      <c r="C17" s="168"/>
       <c r="D17" s="29" t="s">
         <v>61</v>
       </c>
@@ -4029,10 +4013,10 @@
     </row>
     <row r="19" spans="1:7" ht="13" thickBot="1">
       <c r="A19" s="87"/>
-      <c r="B19" s="191" t="s">
+      <c r="B19" s="161" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="192"/>
+      <c r="C19" s="162"/>
       <c r="D19" s="86">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -4065,12 +4049,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="B9:C9"/>
@@ -4080,6 +4058,12 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -4571,10 +4555,10 @@
       </c>
     </row>
     <row r="2" spans="2:10" ht="13" thickBot="1">
-      <c r="D2" s="195" t="s">
+      <c r="D2" s="167" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="197"/>
+      <c r="E2" s="172"/>
     </row>
     <row r="3" spans="2:10" ht="13" thickBot="1">
       <c r="B3" s="8" t="s">
@@ -4768,10 +4752,10 @@
   <sheetData>
     <row r="3" spans="2:9" ht="13" thickBot="1"/>
     <row r="4" spans="2:9" ht="13" thickBot="1">
-      <c r="B4" s="198" t="s">
+      <c r="B4" s="173" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="194"/>
+      <c r="C4" s="164"/>
     </row>
     <row r="5" spans="2:9" ht="13" thickBot="1">
       <c r="B5" s="26" t="s">

</xml_diff>